<commit_message>
Ops for November 2023 updated
Ops for November 2023 updated
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/Ops-2023-11.xlsx
+++ b/Offline/BusinessManagement/Ops/Ops-2023-11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Ops\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F406653A-50DB-446A-95B3-253226463086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884A634E-C0D1-4044-A536-23069174E414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
   </bookViews>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="195">
   <si>
     <t>Course</t>
   </si>
@@ -693,6 +693,18 @@
   <si>
     <t>Faculty: Subrata Ghosh     ||     Batch: B1: NEET &amp; IIT Crash Course Chemistry
 Timing: Thursday 4-6pm     ||     Start date: 07/Sep/2023</t>
+  </si>
+  <si>
+    <t>Chapters on Test</t>
+  </si>
+  <si>
+    <t>1) Matrix</t>
+  </si>
+  <si>
+    <t>2) Determinants</t>
+  </si>
+  <si>
+    <t>3) Complex Numbers</t>
   </si>
 </sst>
 </file>
@@ -1465,7 +1477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1667,55 +1679,9 @@
     <xf numFmtId="0" fontId="12" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1773,6 +1739,51 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2198,7 +2209,7 @@
     <col min="6" max="6" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.44140625" customWidth="1"/>
     <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.88671875" style="128" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.88671875" style="112" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="47.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="47.44140625" bestFit="1" customWidth="1"/>
@@ -2206,54 +2217,54 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="134" t="s">
         <v>186</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="113"/>
-      <c r="M2" s="130" t="s">
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="136"/>
+      <c r="M2" s="114" t="s">
         <v>182</v>
       </c>
-      <c r="N2" s="131" t="s">
+      <c r="N2" s="115" t="s">
         <v>180</v>
       </c>
-      <c r="O2" s="130" t="s">
+      <c r="O2" s="114" t="s">
         <v>183</v>
       </c>
-      <c r="P2" s="130" t="s">
+      <c r="P2" s="114" t="s">
         <v>184</v>
       </c>
-      <c r="Q2" s="130" t="s">
+      <c r="Q2" s="114" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="114"/>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="122" t="s">
+      <c r="B3" s="137"/>
+      <c r="C3" s="138"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="138"/>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="145" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="123"/>
-      <c r="J3" s="123"/>
-      <c r="K3" s="124"/>
+      <c r="I3" s="146"/>
+      <c r="J3" s="146"/>
+      <c r="K3" s="147"/>
       <c r="M3" s="78"/>
-      <c r="N3" s="129"/>
+      <c r="N3" s="113"/>
       <c r="O3" s="78"/>
       <c r="P3" s="78"/>
       <c r="Q3" s="78"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="118" t="s">
+      <c r="B4" s="141" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="120" t="s">
+      <c r="C4" s="143" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="44">
@@ -2273,7 +2284,7 @@
       <c r="M4" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="N4" s="129">
+      <c r="N4" s="113">
         <v>1</v>
       </c>
       <c r="O4" s="106" t="s">
@@ -2285,8 +2296,8 @@
       <c r="Q4" s="78"/>
     </row>
     <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="119"/>
-      <c r="C5" s="121"/>
+      <c r="B5" s="142"/>
+      <c r="C5" s="144"/>
       <c r="D5" s="81" t="s">
         <v>51</v>
       </c>
@@ -2296,13 +2307,13 @@
       <c r="F5" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="132"/>
+      <c r="G5" s="116"/>
       <c r="H5" s="70"/>
       <c r="I5" s="71"/>
       <c r="J5" s="71"/>
       <c r="K5" s="72"/>
       <c r="M5" s="78"/>
-      <c r="N5" s="129">
+      <c r="N5" s="113">
         <v>2</v>
       </c>
       <c r="O5" s="106" t="s">
@@ -2314,28 +2325,28 @@
       <c r="Q5" s="78"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B6" s="133">
+      <c r="B6" s="117">
         <v>1</v>
       </c>
-      <c r="C6" s="134" t="s">
+      <c r="C6" s="118" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="135" t="s">
+      <c r="D6" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="136" t="s">
+      <c r="E6" s="120" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="135" t="s">
+      <c r="F6" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="137"/>
+      <c r="G6" s="121"/>
       <c r="H6" s="64"/>
       <c r="I6" s="65"/>
       <c r="J6" s="65"/>
       <c r="K6" s="66"/>
       <c r="M6" s="78"/>
-      <c r="N6" s="129">
+      <c r="N6" s="113">
         <v>3</v>
       </c>
       <c r="O6" s="106" t="s">
@@ -2347,20 +2358,20 @@
       <c r="Q6" s="78"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B7" s="138">
+      <c r="B7" s="122">
         <v>2</v>
       </c>
-      <c r="C7" s="139"/>
-      <c r="D7" s="140"/>
-      <c r="E7" s="141"/>
-      <c r="F7" s="141"/>
-      <c r="G7" s="142"/>
+      <c r="C7" s="123"/>
+      <c r="D7" s="124"/>
+      <c r="E7" s="125"/>
+      <c r="F7" s="125"/>
+      <c r="G7" s="126"/>
       <c r="H7" s="62"/>
       <c r="I7" s="51"/>
       <c r="J7" s="51"/>
       <c r="K7" s="52"/>
       <c r="M7" s="78"/>
-      <c r="N7" s="129">
+      <c r="N7" s="113">
         <v>4</v>
       </c>
       <c r="O7" s="106" t="s">
@@ -2372,20 +2383,20 @@
       <c r="Q7" s="78"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B8" s="138">
+      <c r="B8" s="122">
         <v>3</v>
       </c>
-      <c r="C8" s="139"/>
-      <c r="D8" s="140"/>
-      <c r="E8" s="141"/>
-      <c r="F8" s="141"/>
-      <c r="G8" s="142"/>
+      <c r="C8" s="123"/>
+      <c r="D8" s="124"/>
+      <c r="E8" s="125"/>
+      <c r="F8" s="125"/>
+      <c r="G8" s="126"/>
       <c r="H8" s="62"/>
       <c r="I8" s="51"/>
       <c r="J8" s="51"/>
       <c r="K8" s="52"/>
       <c r="M8" s="78"/>
-      <c r="N8" s="129">
+      <c r="N8" s="113">
         <v>5</v>
       </c>
       <c r="O8" s="106" t="s">
@@ -2397,20 +2408,20 @@
       <c r="Q8" s="78"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B9" s="138">
+      <c r="B9" s="122">
         <v>4</v>
       </c>
-      <c r="C9" s="139"/>
-      <c r="D9" s="140"/>
-      <c r="E9" s="141"/>
-      <c r="F9" s="141"/>
-      <c r="G9" s="142"/>
+      <c r="C9" s="123"/>
+      <c r="D9" s="124"/>
+      <c r="E9" s="125"/>
+      <c r="F9" s="125"/>
+      <c r="G9" s="126"/>
       <c r="H9" s="62"/>
       <c r="I9" s="51"/>
       <c r="J9" s="51"/>
       <c r="K9" s="52"/>
       <c r="M9" s="78"/>
-      <c r="N9" s="129">
+      <c r="N9" s="113">
         <v>6</v>
       </c>
       <c r="O9" s="106" t="s">
@@ -2422,20 +2433,20 @@
       <c r="Q9" s="78"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B10" s="138">
+      <c r="B10" s="122">
         <v>5</v>
       </c>
-      <c r="C10" s="139"/>
-      <c r="D10" s="140"/>
-      <c r="E10" s="141"/>
-      <c r="F10" s="141"/>
-      <c r="G10" s="142"/>
+      <c r="C10" s="123"/>
+      <c r="D10" s="124"/>
+      <c r="E10" s="125"/>
+      <c r="F10" s="125"/>
+      <c r="G10" s="126"/>
       <c r="H10" s="62"/>
       <c r="I10" s="51"/>
       <c r="J10" s="51"/>
       <c r="K10" s="52"/>
       <c r="M10" s="78"/>
-      <c r="N10" s="129">
+      <c r="N10" s="113">
         <v>7</v>
       </c>
       <c r="O10" s="109" t="s">
@@ -2447,20 +2458,20 @@
       <c r="Q10" s="78"/>
     </row>
     <row r="11" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="143">
+      <c r="B11" s="127">
         <v>6</v>
       </c>
-      <c r="C11" s="144"/>
-      <c r="D11" s="145"/>
-      <c r="E11" s="146"/>
-      <c r="F11" s="146"/>
-      <c r="G11" s="147"/>
+      <c r="C11" s="128"/>
+      <c r="D11" s="129"/>
+      <c r="E11" s="130"/>
+      <c r="F11" s="130"/>
+      <c r="G11" s="131"/>
       <c r="H11" s="63"/>
       <c r="I11" s="54"/>
       <c r="J11" s="54"/>
       <c r="K11" s="55"/>
       <c r="M11" s="78"/>
-      <c r="N11" s="129">
+      <c r="N11" s="113">
         <v>8</v>
       </c>
       <c r="O11" s="106" t="s">
@@ -2472,11 +2483,11 @@
       <c r="Q11" s="78"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="125" t="s">
+      <c r="B12" s="148" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="125"/>
-      <c r="D12" s="126" t="s">
+      <c r="C12" s="148"/>
+      <c r="D12" s="111" t="s">
         <v>164</v>
       </c>
       <c r="E12" s="80" t="s">
@@ -2487,7 +2498,7 @@
       </c>
       <c r="G12" s="80"/>
       <c r="M12" s="78"/>
-      <c r="N12" s="129">
+      <c r="N12" s="113">
         <v>9</v>
       </c>
       <c r="O12" s="110" t="s">
@@ -2501,10 +2512,10 @@
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B13" s="80"/>
       <c r="C13" s="80"/>
-      <c r="D13" s="126" t="s">
+      <c r="D13" s="111" t="s">
         <v>165</v>
       </c>
-      <c r="E13" s="126" t="s">
+      <c r="E13" s="111" t="s">
         <v>169</v>
       </c>
       <c r="F13" s="80" t="s">
@@ -2512,7 +2523,7 @@
       </c>
       <c r="G13" s="80"/>
       <c r="M13" s="78"/>
-      <c r="N13" s="129">
+      <c r="N13" s="113">
         <v>10</v>
       </c>
       <c r="O13" s="106" t="s">
@@ -2531,7 +2542,7 @@
       <c r="D14" s="80" t="s">
         <v>166</v>
       </c>
-      <c r="E14" s="126" t="s">
+      <c r="E14" s="111" t="s">
         <v>170</v>
       </c>
       <c r="F14" s="80" t="s">
@@ -2539,7 +2550,7 @@
       </c>
       <c r="G14" s="80"/>
       <c r="M14" s="78"/>
-      <c r="N14" s="129">
+      <c r="N14" s="113">
         <v>11</v>
       </c>
       <c r="O14" s="106" t="s">
@@ -2564,7 +2575,7 @@
       </c>
       <c r="G15" s="80"/>
       <c r="M15" s="78"/>
-      <c r="N15" s="129">
+      <c r="N15" s="113">
         <v>12</v>
       </c>
       <c r="O15" s="106" t="s">
@@ -2589,7 +2600,7 @@
       <c r="M16" s="104" t="s">
         <v>126</v>
       </c>
-      <c r="N16" s="129">
+      <c r="N16" s="113">
         <v>13</v>
       </c>
       <c r="O16" s="107" t="s">
@@ -2604,13 +2615,13 @@
       <c r="B17" s="80"/>
       <c r="C17" s="80"/>
       <c r="D17" s="80"/>
-      <c r="E17" s="127" t="s">
+      <c r="E17" s="80" t="s">
         <v>176</v>
       </c>
       <c r="F17" s="80"/>
       <c r="G17" s="80"/>
       <c r="M17" s="78"/>
-      <c r="N17" s="129">
+      <c r="N17" s="113">
         <v>14</v>
       </c>
       <c r="O17" s="107" t="s">
@@ -2625,13 +2636,13 @@
       <c r="B18" s="80"/>
       <c r="C18" s="80"/>
       <c r="D18" s="80"/>
-      <c r="E18" s="127" t="s">
+      <c r="E18" s="80" t="s">
         <v>177</v>
       </c>
       <c r="F18" s="80"/>
       <c r="G18" s="80"/>
       <c r="M18" s="78"/>
-      <c r="N18" s="129">
+      <c r="N18" s="113">
         <v>15</v>
       </c>
       <c r="O18" s="107" t="s">
@@ -2644,7 +2655,7 @@
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M19" s="78"/>
-      <c r="N19" s="129">
+      <c r="N19" s="113">
         <v>16</v>
       </c>
       <c r="O19" s="107" t="s">
@@ -2657,7 +2668,7 @@
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M20" s="78"/>
-      <c r="N20" s="129">
+      <c r="N20" s="113">
         <v>17</v>
       </c>
       <c r="O20" s="107" t="s">
@@ -2670,7 +2681,7 @@
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M21" s="78"/>
-      <c r="N21" s="129">
+      <c r="N21" s="113">
         <v>18</v>
       </c>
       <c r="O21" s="107" t="s">
@@ -2683,7 +2694,7 @@
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M22" s="78"/>
-      <c r="N22" s="129">
+      <c r="N22" s="113">
         <v>19</v>
       </c>
       <c r="O22" s="107" t="s">
@@ -2696,7 +2707,7 @@
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M23" s="78"/>
-      <c r="N23" s="129">
+      <c r="N23" s="113">
         <v>20</v>
       </c>
       <c r="O23" s="107" t="s">
@@ -2709,7 +2720,7 @@
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M24" s="78"/>
-      <c r="N24" s="129">
+      <c r="N24" s="113">
         <v>21</v>
       </c>
       <c r="O24" s="107" t="s">
@@ -2722,7 +2733,7 @@
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M25" s="78"/>
-      <c r="N25" s="129">
+      <c r="N25" s="113">
         <v>22</v>
       </c>
       <c r="O25" s="107" t="s">
@@ -2735,7 +2746,7 @@
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M26" s="78"/>
-      <c r="N26" s="129">
+      <c r="N26" s="113">
         <v>23</v>
       </c>
       <c r="O26" s="107" t="s">
@@ -2748,7 +2759,7 @@
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M27" s="78"/>
-      <c r="N27" s="129">
+      <c r="N27" s="113">
         <v>24</v>
       </c>
       <c r="O27" s="107" t="s">
@@ -2763,7 +2774,7 @@
       <c r="M28" s="105" t="s">
         <v>127</v>
       </c>
-      <c r="N28" s="129">
+      <c r="N28" s="113">
         <v>25</v>
       </c>
       <c r="O28" s="108" t="s">
@@ -2778,7 +2789,7 @@
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M29" s="78"/>
-      <c r="N29" s="129">
+      <c r="N29" s="113">
         <v>26</v>
       </c>
       <c r="O29" s="108" t="s">
@@ -2791,7 +2802,7 @@
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M30" s="78"/>
-      <c r="N30" s="129">
+      <c r="N30" s="113">
         <v>27</v>
       </c>
       <c r="O30" s="108" t="s">
@@ -2804,7 +2815,7 @@
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M31" s="78"/>
-      <c r="N31" s="129">
+      <c r="N31" s="113">
         <v>28</v>
       </c>
       <c r="O31" s="108" t="s">
@@ -2817,7 +2828,7 @@
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.3">
       <c r="M32" s="78"/>
-      <c r="N32" s="129">
+      <c r="N32" s="113">
         <v>29</v>
       </c>
       <c r="O32" s="108" t="s">
@@ -2830,7 +2841,7 @@
     </row>
     <row r="33" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M33" s="78"/>
-      <c r="N33" s="129">
+      <c r="N33" s="113">
         <v>30</v>
       </c>
       <c r="O33" s="108" t="s">
@@ -2843,7 +2854,7 @@
     </row>
     <row r="34" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M34" s="78"/>
-      <c r="N34" s="129">
+      <c r="N34" s="113">
         <v>31</v>
       </c>
       <c r="O34" s="108" t="s">
@@ -2856,7 +2867,7 @@
     </row>
     <row r="35" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M35" s="78"/>
-      <c r="N35" s="129">
+      <c r="N35" s="113">
         <v>32</v>
       </c>
       <c r="O35" s="108" t="s">
@@ -2869,7 +2880,7 @@
     </row>
     <row r="36" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M36" s="78"/>
-      <c r="N36" s="129">
+      <c r="N36" s="113">
         <v>33</v>
       </c>
       <c r="O36" s="108" t="s">
@@ -2882,7 +2893,7 @@
     </row>
     <row r="37" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M37" s="78"/>
-      <c r="N37" s="129">
+      <c r="N37" s="113">
         <v>34</v>
       </c>
       <c r="O37" s="108" t="s">
@@ -2895,14 +2906,14 @@
     </row>
     <row r="38" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M38" s="78"/>
-      <c r="N38" s="129"/>
+      <c r="N38" s="113"/>
       <c r="O38" s="78"/>
       <c r="P38" s="78"/>
       <c r="Q38" s="78"/>
     </row>
     <row r="39" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M39" s="78"/>
-      <c r="N39" s="129"/>
+      <c r="N39" s="113"/>
       <c r="O39" s="105" t="s">
         <v>33</v>
       </c>
@@ -2914,7 +2925,7 @@
     </row>
     <row r="40" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M40" s="78"/>
-      <c r="N40" s="129"/>
+      <c r="N40" s="113"/>
       <c r="O40" s="105" t="s">
         <v>185</v>
       </c>
@@ -2925,7 +2936,7 @@
     </row>
     <row r="41" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M41" s="78"/>
-      <c r="N41" s="129"/>
+      <c r="N41" s="113"/>
       <c r="O41" s="105" t="s">
         <v>181</v>
       </c>
@@ -3895,34 +3906,34 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="134" t="s">
         <v>190</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="113"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="136"/>
     </row>
     <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="114"/>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="122" t="s">
+      <c r="B3" s="137"/>
+      <c r="C3" s="138"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="138"/>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="145" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="123"/>
-      <c r="J3" s="123"/>
-      <c r="K3" s="124"/>
+      <c r="I3" s="146"/>
+      <c r="J3" s="146"/>
+      <c r="K3" s="147"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="118" t="s">
+      <c r="B4" s="141" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="120" t="s">
+      <c r="C4" s="143" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="44">
@@ -3939,8 +3950,8 @@
       <c r="K4" s="69"/>
     </row>
     <row r="5" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="119"/>
-      <c r="C5" s="121"/>
+      <c r="B5" s="142"/>
+      <c r="C5" s="144"/>
       <c r="D5" s="81" t="s">
         <v>47</v>
       </c>
@@ -4045,10 +4056,10 @@
       <c r="K11" s="55"/>
     </row>
     <row r="12" spans="2:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="116" t="s">
+      <c r="B12" s="139" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="117"/>
+      <c r="C12" s="140"/>
       <c r="D12" s="43" t="s">
         <v>63</v>
       </c>
@@ -4101,14 +4112,14 @@
   <sheetData>
     <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="134" t="s">
         <v>189</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="113"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="136"/>
       <c r="M2">
         <v>1</v>
       </c>
@@ -4117,18 +4128,18 @@
       </c>
     </row>
     <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="114"/>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="122" t="s">
+      <c r="B3" s="137"/>
+      <c r="C3" s="138"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="138"/>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="145" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="123"/>
-      <c r="J3" s="123"/>
-      <c r="K3" s="124"/>
+      <c r="I3" s="146"/>
+      <c r="J3" s="146"/>
+      <c r="K3" s="147"/>
       <c r="M3">
         <v>2</v>
       </c>
@@ -4137,10 +4148,10 @@
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="118" t="s">
+      <c r="B4" s="141" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="120" t="s">
+      <c r="C4" s="143" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="44">
@@ -4163,8 +4174,8 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="119"/>
-      <c r="C5" s="121"/>
+      <c r="B5" s="142"/>
+      <c r="C5" s="144"/>
       <c r="D5" s="46" t="s">
         <v>49</v>
       </c>
@@ -4311,10 +4322,10 @@
       </c>
     </row>
     <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="116" t="s">
+      <c r="B12" s="139" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="117"/>
+      <c r="C12" s="140"/>
       <c r="D12" s="43" t="s">
         <v>63</v>
       </c>
@@ -4490,36 +4501,36 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="134" t="s">
         <v>188</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="113"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="136"/>
     </row>
     <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="114"/>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="115"/>
-      <c r="I3" s="122" t="s">
+      <c r="B3" s="137"/>
+      <c r="C3" s="138"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="138"/>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="138"/>
+      <c r="I3" s="145" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="123"/>
-      <c r="K3" s="123"/>
-      <c r="L3" s="124"/>
+      <c r="J3" s="146"/>
+      <c r="K3" s="146"/>
+      <c r="L3" s="147"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="118" t="s">
+      <c r="B4" s="141" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="120" t="s">
+      <c r="C4" s="143" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="44">
@@ -4539,8 +4550,8 @@
       <c r="L4" s="69"/>
     </row>
     <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="119"/>
-      <c r="C5" s="121"/>
+      <c r="B5" s="142"/>
+      <c r="C5" s="144"/>
       <c r="D5" s="73" t="s">
         <v>53</v>
       </c>
@@ -4656,10 +4667,10 @@
       <c r="L11" s="55"/>
     </row>
     <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="116" t="s">
+      <c r="B12" s="139" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="117"/>
+      <c r="C12" s="140"/>
       <c r="D12" s="43"/>
       <c r="E12" s="35" t="s">
         <v>155</v>
@@ -4690,10 +4701,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0268C353-496F-4BD6-A7EF-D042619A03C3}">
-  <dimension ref="B1:L14"/>
+  <dimension ref="B1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4711,36 +4722,36 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="134" t="s">
         <v>187</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="113"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="136"/>
     </row>
     <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="114"/>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="115"/>
-      <c r="I3" s="122" t="s">
+      <c r="B3" s="137"/>
+      <c r="C3" s="138"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="138"/>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="138"/>
+      <c r="I3" s="145" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="123"/>
-      <c r="K3" s="123"/>
-      <c r="L3" s="124"/>
+      <c r="J3" s="146"/>
+      <c r="K3" s="146"/>
+      <c r="L3" s="147"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="118" t="s">
+      <c r="B4" s="141" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="120" t="s">
+      <c r="C4" s="143" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="44">
@@ -4757,19 +4768,19 @@
       <c r="I4" s="44">
         <v>45241</v>
       </c>
-      <c r="J4" s="148" t="s">
+      <c r="J4" s="132" t="s">
         <v>161</v>
       </c>
-      <c r="K4" s="148" t="s">
+      <c r="K4" s="132" t="s">
         <v>162</v>
       </c>
-      <c r="L4" s="149" t="s">
+      <c r="L4" s="133" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="119"/>
-      <c r="C5" s="121"/>
+      <c r="B5" s="142"/>
+      <c r="C5" s="144"/>
       <c r="D5" s="73" t="s">
         <v>52</v>
       </c>
@@ -4894,10 +4905,10 @@
       <c r="L11" s="55"/>
     </row>
     <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="116" t="s">
+      <c r="B12" s="139" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="117"/>
+      <c r="C12" s="140"/>
       <c r="D12" s="43"/>
       <c r="E12" s="35" t="s">
         <v>157</v>
@@ -4907,15 +4918,29 @@
       </c>
       <c r="G12" s="75"/>
       <c r="H12" s="78"/>
+      <c r="J12" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
         <v>159</v>
       </c>
+      <c r="J13" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F14" t="s">
         <v>160</v>
+      </c>
+      <c r="J14" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J15" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pratim Raha record for fees has been updated
Pratim Raha record for fees has been updated
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/Ops-2023-11.xlsx
+++ b/Offline/BusinessManagement/Ops/Ops-2023-11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Ops\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884A634E-C0D1-4044-A536-23069174E414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA1ADF0-C95F-4F18-B4F5-739F1215B3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
@@ -45,6 +45,29 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={CAC0B8C7-F59A-434E-826E-AE2871929596}</author>
+  </authors>
+  <commentList>
+    <comment ref="M15" authorId="0" shapeId="0" xr:uid="{CAC0B8C7-F59A-434E-826E-AE2871929596}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Paid Rs 5000 in cash. 
+Total Course Fee is Rs 20,000.
+Duration 2 months (Nov-2023 &amp; Dec-2023)
+In Nov-2023 we will charge Rs 10,000.
+Rest 10,000 will be charged on December.
+ </t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
     <author>tc={9982AFAF-E6E7-45C0-A44A-0C0167B0574C}</author>
   </authors>
   <commentList>
@@ -60,7 +83,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={9982AFAF-E6E7-45BF-A44A-0C0167B0574C}</author>
@@ -78,7 +101,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={4EE09740-4AB8-4767-BD8A-38F7D58F39B2}</author>
@@ -96,7 +119,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={77BE6F65-1B38-40C6-BD39-81B5DFEC0749}</author>
@@ -115,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="200">
   <si>
     <t>Course</t>
   </si>
@@ -705,6 +728,21 @@
   </si>
   <si>
     <t>3) Complex Numbers</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>Java,Advance Java and MySQL</t>
+  </si>
+  <si>
+    <t>Debashish Nath</t>
+  </si>
+  <si>
+    <t>Pratim Raha</t>
+  </si>
+  <si>
+    <t>Partial</t>
   </si>
 </sst>
 </file>
@@ -743,12 +781,6 @@
       <b/>
       <sz val="9"/>
       <color rgb="FFFF0000"/>
-      <name val="Oxygen"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF00B050"/>
       <name val="Oxygen"/>
     </font>
     <font>
@@ -806,6 +838,12 @@
       <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="16">
@@ -900,7 +938,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -927,21 +965,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -1477,30 +1500,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1508,178 +1532,173 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="9" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="8" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="2" fillId="3" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="2" fillId="3" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1688,103 +1707,109 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2105,13 +2130,26 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="M15" dT="2023-11-14T08:33:25.79" personId="{A98E9D41-33A5-4BF6-BDEF-83BD84C6E107}" id="{CAC0B8C7-F59A-434E-826E-AE2871929596}">
+    <text xml:space="preserve">Paid Rs 5000 in cash. 
+Total Course Fee is Rs 20,000.
+Duration 2 months (Nov-2023 &amp; Dec-2023)
+In Nov-2023 we will charge Rs 10,000.
+Rest 10,000 will be charged on December.
+ </text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="D12" dT="2023-11-02T12:47:03.22" personId="{A98E9D41-33A5-4BF6-BDEF-83BD84C6E107}" id="{9982AFAF-E6E7-45C0-A44A-0C0167B0574C}">
     <text>1) Redox</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="D12" dT="2023-11-02T12:47:03.22" personId="{A98E9D41-33A5-4BF6-BDEF-83BD84C6E107}" id="{9982AFAF-E6E7-45BF-A44A-0C0167B0574C}">
     <text>1) Redox</text>
@@ -2119,7 +2157,7 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="D12" dT="2023-11-04T08:33:38.77" personId="{A98E9D41-33A5-4BF6-BDEF-83BD84C6E107}" id="{4EE09740-4AB8-4767-BD8A-38F7D58F39B2}">
     <text>1) Elasticity</text>
@@ -2127,7 +2165,7 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/threadedComments/threadedComment5.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="D12" dT="2023-11-04T08:34:55.19" personId="{A98E9D41-33A5-4BF6-BDEF-83BD84C6E107}" id="{77BE6F65-1B38-40C6-BD39-81B5DFEC0749}">
     <text>1) Determinants</text>
@@ -2149,7 +2187,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="96" t="s">
         <v>75</v>
       </c>
       <c r="C1">
@@ -2157,7 +2195,7 @@
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="96" t="s">
         <v>74</v>
       </c>
       <c r="C2">
@@ -2165,7 +2203,7 @@
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="96" t="s">
         <v>73</v>
       </c>
       <c r="C3">
@@ -2173,7 +2211,7 @@
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="100" t="s">
+      <c r="B4" s="96" t="s">
         <v>76</v>
       </c>
       <c r="C4">
@@ -2181,7 +2219,7 @@
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="100" t="s">
+      <c r="B5" s="96" t="s">
         <v>77</v>
       </c>
       <c r="C5">
@@ -2209,7 +2247,7 @@
     <col min="6" max="6" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.44140625" customWidth="1"/>
     <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.88671875" style="112" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.88671875" style="108" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="47.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="47.44140625" bestFit="1" customWidth="1"/>
@@ -2217,734 +2255,734 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="134" t="s">
+      <c r="B2" s="130" t="s">
         <v>186</v>
       </c>
-      <c r="C2" s="135"/>
-      <c r="D2" s="135"/>
-      <c r="E2" s="135"/>
-      <c r="F2" s="135"/>
-      <c r="G2" s="136"/>
-      <c r="M2" s="114" t="s">
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="132"/>
+      <c r="M2" s="110" t="s">
         <v>182</v>
       </c>
-      <c r="N2" s="115" t="s">
+      <c r="N2" s="111" t="s">
         <v>180</v>
       </c>
-      <c r="O2" s="114" t="s">
+      <c r="O2" s="110" t="s">
         <v>183</v>
       </c>
-      <c r="P2" s="114" t="s">
+      <c r="P2" s="110" t="s">
         <v>184</v>
       </c>
-      <c r="Q2" s="114" t="s">
+      <c r="Q2" s="110" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="137"/>
-      <c r="C3" s="138"/>
-      <c r="D3" s="138"/>
-      <c r="E3" s="138"/>
-      <c r="F3" s="138"/>
-      <c r="G3" s="138"/>
-      <c r="H3" s="145" t="s">
+      <c r="B3" s="133"/>
+      <c r="C3" s="134"/>
+      <c r="D3" s="134"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="134"/>
+      <c r="H3" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="146"/>
-      <c r="J3" s="146"/>
-      <c r="K3" s="147"/>
-      <c r="M3" s="78"/>
-      <c r="N3" s="113"/>
-      <c r="O3" s="78"/>
-      <c r="P3" s="78"/>
-      <c r="Q3" s="78"/>
+      <c r="I3" s="142"/>
+      <c r="J3" s="142"/>
+      <c r="K3" s="143"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="109"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="74"/>
+      <c r="Q3" s="74"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="141" t="s">
+      <c r="B4" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="143" t="s">
+      <c r="C4" s="139" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="44">
+      <c r="D4" s="40">
         <v>45234</v>
       </c>
-      <c r="E4" s="45">
+      <c r="E4" s="41">
         <v>45235</v>
       </c>
-      <c r="F4" s="45">
+      <c r="F4" s="41">
         <v>45241</v>
       </c>
-      <c r="G4" s="57"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="68"/>
-      <c r="K4" s="69"/>
-      <c r="M4" s="103" t="s">
+      <c r="G4" s="53"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="65"/>
+      <c r="M4" s="99" t="s">
         <v>125</v>
       </c>
-      <c r="N4" s="113">
+      <c r="N4" s="109">
         <v>1</v>
       </c>
-      <c r="O4" s="106" t="s">
+      <c r="O4" s="102" t="s">
         <v>128</v>
       </c>
-      <c r="P4" s="78">
+      <c r="P4" s="74">
         <v>1</v>
       </c>
-      <c r="Q4" s="78"/>
+      <c r="Q4" s="74"/>
     </row>
     <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="142"/>
-      <c r="C5" s="144"/>
-      <c r="D5" s="81" t="s">
+      <c r="B5" s="138"/>
+      <c r="C5" s="140"/>
+      <c r="D5" s="77" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="81" t="s">
+      <c r="E5" s="77" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="81" t="s">
+      <c r="F5" s="77" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="116"/>
-      <c r="H5" s="70"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="72"/>
-      <c r="M5" s="78"/>
-      <c r="N5" s="113">
+      <c r="G5" s="112"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="68"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="109">
         <v>2</v>
       </c>
-      <c r="O5" s="106" t="s">
+      <c r="O5" s="102" t="s">
         <v>131</v>
       </c>
-      <c r="P5" s="78">
+      <c r="P5" s="74">
         <v>1</v>
       </c>
-      <c r="Q5" s="78"/>
+      <c r="Q5" s="74"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B6" s="117">
+      <c r="B6" s="113">
         <v>1</v>
       </c>
-      <c r="C6" s="118" t="s">
+      <c r="C6" s="114" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="119" t="s">
+      <c r="D6" s="115" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="120" t="s">
+      <c r="E6" s="116" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="119" t="s">
+      <c r="F6" s="115" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="121"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="66"/>
-      <c r="M6" s="78"/>
-      <c r="N6" s="113">
+      <c r="G6" s="117"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="62"/>
+      <c r="M6" s="74"/>
+      <c r="N6" s="109">
         <v>3</v>
       </c>
-      <c r="O6" s="106" t="s">
+      <c r="O6" s="102" t="s">
         <v>134</v>
       </c>
-      <c r="P6" s="78">
+      <c r="P6" s="74">
         <v>1</v>
       </c>
-      <c r="Q6" s="78"/>
+      <c r="Q6" s="74"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B7" s="122">
+      <c r="B7" s="118">
         <v>2</v>
       </c>
-      <c r="C7" s="123"/>
-      <c r="D7" s="124"/>
-      <c r="E7" s="125"/>
-      <c r="F7" s="125"/>
-      <c r="G7" s="126"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="52"/>
-      <c r="M7" s="78"/>
-      <c r="N7" s="113">
+      <c r="C7" s="119"/>
+      <c r="D7" s="120"/>
+      <c r="E7" s="121"/>
+      <c r="F7" s="121"/>
+      <c r="G7" s="122"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="48"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="109">
         <v>4</v>
       </c>
-      <c r="O7" s="106" t="s">
+      <c r="O7" s="102" t="s">
         <v>136</v>
       </c>
-      <c r="P7" s="78">
+      <c r="P7" s="74">
         <v>1</v>
       </c>
-      <c r="Q7" s="78"/>
+      <c r="Q7" s="74"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B8" s="122">
+      <c r="B8" s="118">
         <v>3</v>
       </c>
-      <c r="C8" s="123"/>
-      <c r="D8" s="124"/>
-      <c r="E8" s="125"/>
-      <c r="F8" s="125"/>
-      <c r="G8" s="126"/>
-      <c r="H8" s="62"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="52"/>
-      <c r="M8" s="78"/>
-      <c r="N8" s="113">
+      <c r="C8" s="119"/>
+      <c r="D8" s="120"/>
+      <c r="E8" s="121"/>
+      <c r="F8" s="121"/>
+      <c r="G8" s="122"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="48"/>
+      <c r="M8" s="74"/>
+      <c r="N8" s="109">
         <v>5</v>
       </c>
-      <c r="O8" s="106" t="s">
+      <c r="O8" s="102" t="s">
         <v>139</v>
       </c>
-      <c r="P8" s="78">
+      <c r="P8" s="74">
         <v>0.2</v>
       </c>
-      <c r="Q8" s="78"/>
+      <c r="Q8" s="74"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B9" s="122">
+      <c r="B9" s="118">
         <v>4</v>
       </c>
-      <c r="C9" s="123"/>
-      <c r="D9" s="124"/>
-      <c r="E9" s="125"/>
-      <c r="F9" s="125"/>
-      <c r="G9" s="126"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="52"/>
-      <c r="M9" s="78"/>
-      <c r="N9" s="113">
+      <c r="C9" s="119"/>
+      <c r="D9" s="120"/>
+      <c r="E9" s="121"/>
+      <c r="F9" s="121"/>
+      <c r="G9" s="122"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="48"/>
+      <c r="M9" s="74"/>
+      <c r="N9" s="109">
         <v>6</v>
       </c>
-      <c r="O9" s="106" t="s">
+      <c r="O9" s="102" t="s">
         <v>141</v>
       </c>
-      <c r="P9" s="78">
+      <c r="P9" s="74">
         <v>0</v>
       </c>
-      <c r="Q9" s="78"/>
+      <c r="Q9" s="74"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B10" s="122">
+      <c r="B10" s="118">
         <v>5</v>
       </c>
-      <c r="C10" s="123"/>
-      <c r="D10" s="124"/>
-      <c r="E10" s="125"/>
-      <c r="F10" s="125"/>
-      <c r="G10" s="126"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="52"/>
-      <c r="M10" s="78"/>
-      <c r="N10" s="113">
+      <c r="C10" s="119"/>
+      <c r="D10" s="120"/>
+      <c r="E10" s="121"/>
+      <c r="F10" s="121"/>
+      <c r="G10" s="122"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="48"/>
+      <c r="M10" s="74"/>
+      <c r="N10" s="109">
         <v>7</v>
       </c>
-      <c r="O10" s="109" t="s">
+      <c r="O10" s="105" t="s">
         <v>144</v>
       </c>
-      <c r="P10" s="78">
+      <c r="P10" s="74">
         <v>0</v>
       </c>
-      <c r="Q10" s="78"/>
+      <c r="Q10" s="74"/>
     </row>
     <row r="11" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="127">
+      <c r="B11" s="123">
         <v>6</v>
       </c>
-      <c r="C11" s="128"/>
-      <c r="D11" s="129"/>
-      <c r="E11" s="130"/>
-      <c r="F11" s="130"/>
-      <c r="G11" s="131"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="55"/>
-      <c r="M11" s="78"/>
-      <c r="N11" s="113">
+      <c r="C11" s="124"/>
+      <c r="D11" s="125"/>
+      <c r="E11" s="126"/>
+      <c r="F11" s="126"/>
+      <c r="G11" s="127"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="51"/>
+      <c r="M11" s="74"/>
+      <c r="N11" s="109">
         <v>8</v>
       </c>
-      <c r="O11" s="106" t="s">
+      <c r="O11" s="102" t="s">
         <v>147</v>
       </c>
-      <c r="P11" s="78">
+      <c r="P11" s="74">
         <v>0</v>
       </c>
-      <c r="Q11" s="78"/>
+      <c r="Q11" s="74"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="148" t="s">
+      <c r="B12" s="144" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="148"/>
-      <c r="D12" s="111" t="s">
+      <c r="C12" s="144"/>
+      <c r="D12" s="107" t="s">
         <v>164</v>
       </c>
-      <c r="E12" s="80" t="s">
+      <c r="E12" s="76" t="s">
         <v>168</v>
       </c>
-      <c r="F12" s="80" t="s">
+      <c r="F12" s="76" t="s">
         <v>173</v>
       </c>
-      <c r="G12" s="80"/>
-      <c r="M12" s="78"/>
-      <c r="N12" s="113">
+      <c r="G12" s="76"/>
+      <c r="M12" s="74"/>
+      <c r="N12" s="109">
         <v>9</v>
       </c>
-      <c r="O12" s="110" t="s">
+      <c r="O12" s="106" t="s">
         <v>148</v>
       </c>
-      <c r="P12" s="78">
+      <c r="P12" s="74">
         <v>0</v>
       </c>
-      <c r="Q12" s="78"/>
+      <c r="Q12" s="74"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B13" s="80"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="111" t="s">
+      <c r="B13" s="76"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="107" t="s">
         <v>165</v>
       </c>
-      <c r="E13" s="111" t="s">
+      <c r="E13" s="107" t="s">
         <v>169</v>
       </c>
-      <c r="F13" s="80" t="s">
+      <c r="F13" s="76" t="s">
         <v>174</v>
       </c>
-      <c r="G13" s="80"/>
-      <c r="M13" s="78"/>
-      <c r="N13" s="113">
+      <c r="G13" s="76"/>
+      <c r="M13" s="74"/>
+      <c r="N13" s="109">
         <v>10</v>
       </c>
-      <c r="O13" s="106" t="s">
+      <c r="O13" s="102" t="s">
         <v>149</v>
       </c>
-      <c r="P13" s="78">
+      <c r="P13" s="74">
         <v>0.5</v>
       </c>
-      <c r="Q13" s="78" t="s">
+      <c r="Q13" s="74" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80" t="s">
+      <c r="B14" s="76"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76" t="s">
         <v>166</v>
       </c>
-      <c r="E14" s="111" t="s">
+      <c r="E14" s="107" t="s">
         <v>170</v>
       </c>
-      <c r="F14" s="80" t="s">
+      <c r="F14" s="76" t="s">
         <v>175</v>
       </c>
-      <c r="G14" s="80"/>
-      <c r="M14" s="78"/>
-      <c r="N14" s="113">
+      <c r="G14" s="76"/>
+      <c r="M14" s="74"/>
+      <c r="N14" s="109">
         <v>11</v>
       </c>
-      <c r="O14" s="106" t="s">
+      <c r="O14" s="102" t="s">
         <v>150</v>
       </c>
-      <c r="P14" s="78">
+      <c r="P14" s="74">
         <v>0</v>
       </c>
-      <c r="Q14" s="78"/>
+      <c r="Q14" s="74"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B15" s="80"/>
-      <c r="C15" s="80"/>
-      <c r="D15" s="80" t="s">
+      <c r="B15" s="76"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76" t="s">
         <v>167</v>
       </c>
-      <c r="E15" s="80" t="s">
+      <c r="E15" s="76" t="s">
         <v>171</v>
       </c>
-      <c r="F15" s="80" t="s">
+      <c r="F15" s="76" t="s">
         <v>178</v>
       </c>
-      <c r="G15" s="80"/>
-      <c r="M15" s="78"/>
-      <c r="N15" s="113">
+      <c r="G15" s="76"/>
+      <c r="M15" s="74"/>
+      <c r="N15" s="109">
         <v>12</v>
       </c>
-      <c r="O15" s="106" t="s">
+      <c r="O15" s="102" t="s">
         <v>151</v>
       </c>
-      <c r="P15" s="78">
+      <c r="P15" s="74">
         <v>0</v>
       </c>
-      <c r="Q15" s="78"/>
+      <c r="Q15" s="74"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B16" s="80"/>
-      <c r="C16" s="80"/>
-      <c r="D16" s="80"/>
-      <c r="E16" s="80" t="s">
+      <c r="B16" s="76"/>
+      <c r="C16" s="76"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76" t="s">
         <v>172</v>
       </c>
-      <c r="F16" s="80" t="s">
+      <c r="F16" s="76" t="s">
         <v>179</v>
       </c>
-      <c r="G16" s="80"/>
-      <c r="M16" s="104" t="s">
+      <c r="G16" s="76"/>
+      <c r="M16" s="100" t="s">
         <v>126</v>
       </c>
-      <c r="N16" s="113">
+      <c r="N16" s="109">
         <v>13</v>
       </c>
-      <c r="O16" s="107" t="s">
+      <c r="O16" s="103" t="s">
         <v>129</v>
       </c>
-      <c r="P16" s="78">
+      <c r="P16" s="74">
         <v>0.2</v>
       </c>
-      <c r="Q16" s="78"/>
+      <c r="Q16" s="74"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B17" s="80"/>
-      <c r="C17" s="80"/>
-      <c r="D17" s="80"/>
-      <c r="E17" s="80" t="s">
+      <c r="B17" s="76"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76" t="s">
         <v>176</v>
       </c>
-      <c r="F17" s="80"/>
-      <c r="G17" s="80"/>
-      <c r="M17" s="78"/>
-      <c r="N17" s="113">
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
+      <c r="M17" s="74"/>
+      <c r="N17" s="109">
         <v>14</v>
       </c>
-      <c r="O17" s="107" t="s">
+      <c r="O17" s="103" t="s">
         <v>132</v>
       </c>
-      <c r="P17" s="78">
+      <c r="P17" s="74">
         <v>0</v>
       </c>
-      <c r="Q17" s="78"/>
+      <c r="Q17" s="74"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B18" s="80"/>
-      <c r="C18" s="80"/>
-      <c r="D18" s="80"/>
-      <c r="E18" s="80" t="s">
+      <c r="B18" s="76"/>
+      <c r="C18" s="76"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76" t="s">
         <v>177</v>
       </c>
-      <c r="F18" s="80"/>
-      <c r="G18" s="80"/>
-      <c r="M18" s="78"/>
-      <c r="N18" s="113">
+      <c r="F18" s="76"/>
+      <c r="G18" s="76"/>
+      <c r="M18" s="74"/>
+      <c r="N18" s="109">
         <v>15</v>
       </c>
-      <c r="O18" s="107" t="s">
+      <c r="O18" s="103" t="s">
         <v>135</v>
       </c>
-      <c r="P18" s="78">
+      <c r="P18" s="74">
         <v>0</v>
       </c>
-      <c r="Q18" s="78"/>
+      <c r="Q18" s="74"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M19" s="78"/>
-      <c r="N19" s="113">
+      <c r="M19" s="74"/>
+      <c r="N19" s="109">
         <v>16</v>
       </c>
-      <c r="O19" s="107" t="s">
+      <c r="O19" s="103" t="s">
         <v>137</v>
       </c>
-      <c r="P19" s="78">
+      <c r="P19" s="74">
         <v>1</v>
       </c>
-      <c r="Q19" s="78"/>
+      <c r="Q19" s="74"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M20" s="78"/>
-      <c r="N20" s="113">
+      <c r="M20" s="74"/>
+      <c r="N20" s="109">
         <v>17</v>
       </c>
-      <c r="O20" s="107" t="s">
+      <c r="O20" s="103" t="s">
         <v>140</v>
       </c>
-      <c r="P20" s="78">
+      <c r="P20" s="74">
         <v>0</v>
       </c>
-      <c r="Q20" s="78"/>
+      <c r="Q20" s="74"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M21" s="78"/>
-      <c r="N21" s="113">
+      <c r="M21" s="74"/>
+      <c r="N21" s="109">
         <v>18</v>
       </c>
-      <c r="O21" s="107" t="s">
+      <c r="O21" s="103" t="s">
         <v>142</v>
       </c>
-      <c r="P21" s="78">
+      <c r="P21" s="74">
         <v>0</v>
       </c>
-      <c r="Q21" s="78"/>
+      <c r="Q21" s="74"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M22" s="78"/>
-      <c r="N22" s="113">
+      <c r="M22" s="74"/>
+      <c r="N22" s="109">
         <v>19</v>
       </c>
-      <c r="O22" s="107" t="s">
+      <c r="O22" s="103" t="s">
         <v>145</v>
       </c>
-      <c r="P22" s="78">
+      <c r="P22" s="74">
         <v>0</v>
       </c>
-      <c r="Q22" s="78"/>
+      <c r="Q22" s="74"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M23" s="78"/>
-      <c r="N23" s="113">
+      <c r="M23" s="74"/>
+      <c r="N23" s="109">
         <v>20</v>
       </c>
-      <c r="O23" s="107" t="s">
+      <c r="O23" s="103" t="s">
         <v>145</v>
       </c>
-      <c r="P23" s="78">
+      <c r="P23" s="74">
         <v>0</v>
       </c>
-      <c r="Q23" s="78"/>
+      <c r="Q23" s="74"/>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M24" s="78"/>
-      <c r="N24" s="113">
+      <c r="M24" s="74"/>
+      <c r="N24" s="109">
         <v>21</v>
       </c>
-      <c r="O24" s="107" t="s">
+      <c r="O24" s="103" t="s">
         <v>145</v>
       </c>
-      <c r="P24" s="78">
+      <c r="P24" s="74">
         <v>0</v>
       </c>
-      <c r="Q24" s="78"/>
+      <c r="Q24" s="74"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M25" s="78"/>
-      <c r="N25" s="113">
+      <c r="M25" s="74"/>
+      <c r="N25" s="109">
         <v>22</v>
       </c>
-      <c r="O25" s="107" t="s">
+      <c r="O25" s="103" t="s">
         <v>145</v>
       </c>
-      <c r="P25" s="78">
+      <c r="P25" s="74">
         <v>0</v>
       </c>
-      <c r="Q25" s="78"/>
+      <c r="Q25" s="74"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M26" s="78"/>
-      <c r="N26" s="113">
+      <c r="M26" s="74"/>
+      <c r="N26" s="109">
         <v>23</v>
       </c>
-      <c r="O26" s="107" t="s">
+      <c r="O26" s="103" t="s">
         <v>145</v>
       </c>
-      <c r="P26" s="78">
+      <c r="P26" s="74">
         <v>0</v>
       </c>
-      <c r="Q26" s="78"/>
+      <c r="Q26" s="74"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M27" s="78"/>
-      <c r="N27" s="113">
+      <c r="M27" s="74"/>
+      <c r="N27" s="109">
         <v>24</v>
       </c>
-      <c r="O27" s="107" t="s">
+      <c r="O27" s="103" t="s">
         <v>145</v>
       </c>
-      <c r="P27" s="78">
+      <c r="P27" s="74">
         <v>0</v>
       </c>
-      <c r="Q27" s="78"/>
+      <c r="Q27" s="74"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M28" s="105" t="s">
+      <c r="M28" s="101" t="s">
         <v>127</v>
       </c>
-      <c r="N28" s="113">
+      <c r="N28" s="109">
         <v>25</v>
       </c>
-      <c r="O28" s="108" t="s">
+      <c r="O28" s="104" t="s">
         <v>130</v>
       </c>
-      <c r="P28" s="78">
+      <c r="P28" s="74">
         <v>0.5</v>
       </c>
-      <c r="Q28" s="78" t="s">
+      <c r="Q28" s="74" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M29" s="78"/>
-      <c r="N29" s="113">
+      <c r="M29" s="74"/>
+      <c r="N29" s="109">
         <v>26</v>
       </c>
-      <c r="O29" s="108" t="s">
+      <c r="O29" s="104" t="s">
         <v>133</v>
       </c>
-      <c r="P29" s="78">
+      <c r="P29" s="74">
         <v>1</v>
       </c>
-      <c r="Q29" s="78"/>
+      <c r="Q29" s="74"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M30" s="78"/>
-      <c r="N30" s="113">
+      <c r="M30" s="74"/>
+      <c r="N30" s="109">
         <v>27</v>
       </c>
-      <c r="O30" s="108" t="s">
+      <c r="O30" s="104" t="s">
         <v>138</v>
       </c>
-      <c r="P30" s="78">
+      <c r="P30" s="74">
         <v>0</v>
       </c>
-      <c r="Q30" s="78"/>
+      <c r="Q30" s="74"/>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M31" s="78"/>
-      <c r="N31" s="113">
+      <c r="M31" s="74"/>
+      <c r="N31" s="109">
         <v>28</v>
       </c>
-      <c r="O31" s="108" t="s">
+      <c r="O31" s="104" t="s">
         <v>143</v>
       </c>
-      <c r="P31" s="78">
+      <c r="P31" s="74">
         <v>0</v>
       </c>
-      <c r="Q31" s="78"/>
+      <c r="Q31" s="74"/>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M32" s="78"/>
-      <c r="N32" s="113">
+      <c r="M32" s="74"/>
+      <c r="N32" s="109">
         <v>29</v>
       </c>
-      <c r="O32" s="108" t="s">
+      <c r="O32" s="104" t="s">
         <v>146</v>
       </c>
-      <c r="P32" s="78">
+      <c r="P32" s="74">
         <v>0</v>
       </c>
-      <c r="Q32" s="78"/>
+      <c r="Q32" s="74"/>
     </row>
     <row r="33" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M33" s="78"/>
-      <c r="N33" s="113">
+      <c r="M33" s="74"/>
+      <c r="N33" s="109">
         <v>30</v>
       </c>
-      <c r="O33" s="108" t="s">
+      <c r="O33" s="104" t="s">
         <v>145</v>
       </c>
-      <c r="P33" s="78">
+      <c r="P33" s="74">
         <v>0</v>
       </c>
-      <c r="Q33" s="78"/>
+      <c r="Q33" s="74"/>
     </row>
     <row r="34" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M34" s="78"/>
-      <c r="N34" s="113">
+      <c r="M34" s="74"/>
+      <c r="N34" s="109">
         <v>31</v>
       </c>
-      <c r="O34" s="108" t="s">
+      <c r="O34" s="104" t="s">
         <v>145</v>
       </c>
-      <c r="P34" s="78">
+      <c r="P34" s="74">
         <v>0</v>
       </c>
-      <c r="Q34" s="78"/>
+      <c r="Q34" s="74"/>
     </row>
     <row r="35" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M35" s="78"/>
-      <c r="N35" s="113">
+      <c r="M35" s="74"/>
+      <c r="N35" s="109">
         <v>32</v>
       </c>
-      <c r="O35" s="108" t="s">
+      <c r="O35" s="104" t="s">
         <v>145</v>
       </c>
-      <c r="P35" s="78">
+      <c r="P35" s="74">
         <v>0</v>
       </c>
-      <c r="Q35" s="78"/>
+      <c r="Q35" s="74"/>
     </row>
     <row r="36" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M36" s="78"/>
-      <c r="N36" s="113">
+      <c r="M36" s="74"/>
+      <c r="N36" s="109">
         <v>33</v>
       </c>
-      <c r="O36" s="108" t="s">
+      <c r="O36" s="104" t="s">
         <v>145</v>
       </c>
-      <c r="P36" s="78">
+      <c r="P36" s="74">
         <v>0</v>
       </c>
-      <c r="Q36" s="78"/>
+      <c r="Q36" s="74"/>
     </row>
     <row r="37" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M37" s="78"/>
-      <c r="N37" s="113">
+      <c r="M37" s="74"/>
+      <c r="N37" s="109">
         <v>34</v>
       </c>
-      <c r="O37" s="108" t="s">
+      <c r="O37" s="104" t="s">
         <v>145</v>
       </c>
-      <c r="P37" s="78">
+      <c r="P37" s="74">
         <v>0</v>
       </c>
-      <c r="Q37" s="78"/>
+      <c r="Q37" s="74"/>
     </row>
     <row r="38" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M38" s="78"/>
-      <c r="N38" s="113"/>
-      <c r="O38" s="78"/>
-      <c r="P38" s="78"/>
-      <c r="Q38" s="78"/>
+      <c r="M38" s="74"/>
+      <c r="N38" s="109"/>
+      <c r="O38" s="74"/>
+      <c r="P38" s="74"/>
+      <c r="Q38" s="74"/>
     </row>
     <row r="39" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M39" s="78"/>
-      <c r="N39" s="113"/>
-      <c r="O39" s="105" t="s">
+      <c r="M39" s="74"/>
+      <c r="N39" s="109"/>
+      <c r="O39" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="P39" s="80">
+      <c r="P39" s="76">
         <f>SUM(P4:P37)</f>
         <v>7.4</v>
       </c>
-      <c r="Q39" s="78"/>
+      <c r="Q39" s="74"/>
     </row>
     <row r="40" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M40" s="78"/>
-      <c r="N40" s="113"/>
-      <c r="O40" s="105" t="s">
+      <c r="M40" s="74"/>
+      <c r="N40" s="109"/>
+      <c r="O40" s="101" t="s">
         <v>185</v>
       </c>
-      <c r="P40" s="80">
+      <c r="P40" s="76">
         <v>34</v>
       </c>
-      <c r="Q40" s="78"/>
+      <c r="Q40" s="74"/>
     </row>
     <row r="41" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M41" s="78"/>
-      <c r="N41" s="113"/>
-      <c r="O41" s="105" t="s">
+      <c r="M41" s="74"/>
+      <c r="N41" s="109"/>
+      <c r="O41" s="101" t="s">
         <v>181</v>
       </c>
-      <c r="P41" s="80">
+      <c r="P41" s="76">
         <f>ROUND((P39/P40)*100,2)</f>
         <v>21.76</v>
       </c>
-      <c r="Q41" s="78"/>
+      <c r="Q41" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2959,11 +2997,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66DF67B1-7A31-46BB-8007-D9F915FBEBAF}">
-  <dimension ref="B1:M15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66DF67B1-7A31-46BB-8007-D9F915FBEBAF}">
+  <dimension ref="B1:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2976,6 +3014,8 @@
     <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -3043,9 +3083,9 @@
         <f>G3-H3</f>
         <v>0</v>
       </c>
-      <c r="J3" s="101"/>
-      <c r="K3" s="101"/>
-      <c r="L3" s="101"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
       <c r="M3" s="10" t="s">
         <v>27</v>
       </c>
@@ -3120,7 +3160,7 @@
       <c r="K6" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L6" s="98">
+      <c r="L6" s="94">
         <v>45239</v>
       </c>
       <c r="M6" s="19" t="s">
@@ -3195,7 +3235,7 @@
       <c r="K9" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="L9" s="99">
+      <c r="L9" s="95">
         <v>45239</v>
       </c>
       <c r="M9" s="10" t="s">
@@ -3270,7 +3310,7 @@
       <c r="K12" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L12" s="98">
+      <c r="L12" s="94">
         <v>45239</v>
       </c>
       <c r="M12" s="19" t="s">
@@ -3296,44 +3336,107 @@
       <c r="L13" s="1"/>
       <c r="M13" s="21"/>
     </row>
-    <row r="14" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="22"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B14" s="145"/>
+      <c r="C14" s="146"/>
+      <c r="D14" s="146"/>
+      <c r="E14" s="146">
         <v>3</v>
       </c>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23">
+      <c r="F14" s="146"/>
+      <c r="G14" s="146"/>
+      <c r="H14" s="146"/>
+      <c r="I14" s="146">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="24"/>
-    </row>
-    <row r="15" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F15" s="34" t="s">
+      <c r="J14" s="146"/>
+      <c r="K14" s="146"/>
+      <c r="L14" s="146"/>
+      <c r="M14" s="147"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G15" s="1">
+        <v>10000</v>
+      </c>
+      <c r="H15" s="1">
+        <v>5000</v>
+      </c>
+      <c r="I15" s="1">
+        <v>15000</v>
+      </c>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="150">
+        <v>45234</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F18" s="148" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="26">
-        <f>SUM(G3:G14)</f>
-        <v>12000</v>
-      </c>
-      <c r="H15" s="27">
-        <f>SUM(H3:H14)</f>
-        <v>12000</v>
-      </c>
-      <c r="I15" s="25">
-        <f>SUM(I3:I14)</f>
-        <v>0</v>
+      <c r="G18" s="149">
+        <f>SUM(G3:G17)</f>
+        <v>22000</v>
+      </c>
+      <c r="H18" s="149">
+        <f t="shared" ref="H18:I18" si="1">SUM(H3:H17)</f>
+        <v>17000</v>
+      </c>
+      <c r="I18" s="149">
+        <f t="shared" si="1"/>
+        <v>15000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3350,78 +3453,78 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" style="28" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.21875" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.77734375" style="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.44140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.88671875" style="28" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.77734375" style="28" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.77734375" style="28" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.77734375" style="28" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.21875" style="28" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="7.44140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.109375" style="28"/>
+    <col min="1" max="1" width="2.88671875" style="25" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.21875" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.77734375" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.88671875" style="25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.77734375" style="25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.77734375" style="25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.77734375" style="25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.21875" style="25" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="7.44140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.109375" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="12.6" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:17" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="30" t="s">
+      <c r="I2" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="J2" s="30" t="s">
+      <c r="J2" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="K2" s="30" t="s">
+      <c r="K2" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="L2" s="30" t="s">
+      <c r="L2" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="M2" s="30" t="s">
+      <c r="M2" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="N2" s="30" t="s">
+      <c r="N2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="30" t="s">
+      <c r="O2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="30" t="s">
+      <c r="P2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="Q2" s="31" t="s">
+      <c r="Q2" s="28" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="79" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -3449,11 +3552,11 @@
       <c r="O3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="32"/>
+      <c r="P3" s="29"/>
       <c r="Q3" s="10"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="84"/>
+      <c r="B4" s="80"/>
       <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
@@ -3481,38 +3584,38 @@
       <c r="Q4" s="12"/>
     </row>
     <row r="5" spans="2:17" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="88"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="90" t="s">
+      <c r="B5" s="84"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="86" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="90">
+      <c r="H5" s="86">
         <f>SUM(F3:G4)</f>
         <v>4500</v>
       </c>
-      <c r="I5" s="90">
+      <c r="I5" s="86">
         <f>H5</f>
         <v>4500</v>
       </c>
-      <c r="J5" s="91">
+      <c r="J5" s="87">
         <v>45239</v>
       </c>
-      <c r="K5" s="90"/>
-      <c r="L5" s="90"/>
-      <c r="M5" s="90"/>
-      <c r="N5" s="89"/>
-      <c r="O5" s="89"/>
-      <c r="P5" s="89"/>
-      <c r="Q5" s="92"/>
+      <c r="K5" s="86"/>
+      <c r="L5" s="86"/>
+      <c r="M5" s="86"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="88"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="95" t="s">
+      <c r="B6" s="91" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="97" t="s">
+      <c r="C6" s="93" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="18" t="s">
@@ -3545,8 +3648,8 @@
       <c r="Q6" s="19"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="85"/>
-      <c r="C7" s="94" t="s">
+      <c r="B7" s="81"/>
+      <c r="C7" s="90" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -3573,49 +3676,49 @@
       <c r="Q7" s="21"/>
     </row>
     <row r="8" spans="2:17" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="86"/>
+      <c r="B8" s="82"/>
       <c r="C8" s="23"/>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
       <c r="F8" s="23"/>
-      <c r="G8" s="33" t="s">
+      <c r="G8" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="33">
+      <c r="H8" s="30">
         <f>SUM(F6:G7)</f>
         <v>6000</v>
       </c>
-      <c r="I8" s="33">
+      <c r="I8" s="30">
         <f>H8</f>
         <v>6000</v>
       </c>
-      <c r="J8" s="87">
+      <c r="J8" s="83">
         <v>45239</v>
       </c>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
       <c r="N8" s="23"/>
       <c r="O8" s="23"/>
       <c r="P8" s="23"/>
       <c r="Q8" s="24"/>
     </row>
     <row r="9" spans="2:17" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G9" s="96" t="s">
+      <c r="G9" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="93">
+      <c r="H9" s="89">
         <f>SUM(H3:H8)</f>
         <v>10500</v>
       </c>
-      <c r="I9" s="93">
+      <c r="I9" s="89">
         <f>SUM(I3:I8)</f>
         <v>10500</v>
       </c>
-      <c r="J9" s="82"/>
-      <c r="K9" s="82"/>
-      <c r="L9" s="82"/>
-      <c r="M9" s="82"/>
+      <c r="J9" s="78"/>
+      <c r="K9" s="78"/>
+      <c r="L9" s="78"/>
+      <c r="M9" s="78"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3657,35 +3760,35 @@
     <col min="10" max="10" width="43.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="100" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="100" t="s">
+    <row r="1" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="100" t="s">
+      <c r="C1" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="100" t="s">
+      <c r="D1" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="100" t="s">
+      <c r="E1" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="100" t="s">
+      <c r="F1" s="96" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="100" t="s">
+      <c r="G1" s="96" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="100" t="s">
+      <c r="H1" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="100" t="s">
+      <c r="I1" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="100" t="s">
+      <c r="J1" s="96" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3702,7 +3805,7 @@
       <c r="D2" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="56">
+      <c r="E2" s="52">
         <v>45239</v>
       </c>
       <c r="F2" t="s">
@@ -3734,7 +3837,7 @@
       <c r="D3" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="56">
+      <c r="E3" s="52">
         <v>45239</v>
       </c>
       <c r="F3" t="s">
@@ -3766,7 +3869,7 @@
       <c r="D4" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="56">
+      <c r="E4" s="52">
         <v>45239</v>
       </c>
       <c r="F4" t="s">
@@ -3798,7 +3901,7 @@
       <c r="D5" t="s">
         <v>86</v>
       </c>
-      <c r="E5" s="56">
+      <c r="E5" s="52">
         <v>45239</v>
       </c>
       <c r="F5" t="s">
@@ -3830,7 +3933,7 @@
       <c r="D6" t="s">
         <v>93</v>
       </c>
-      <c r="E6" s="56">
+      <c r="E6" s="52">
         <v>45239</v>
       </c>
       <c r="F6" t="s">
@@ -3862,7 +3965,7 @@
       <c r="D7" t="s">
         <v>123</v>
       </c>
-      <c r="E7" s="56">
+      <c r="E7" s="52">
         <v>45240</v>
       </c>
       <c r="F7" t="s">
@@ -3906,168 +4009,168 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="134" t="s">
+      <c r="B2" s="130" t="s">
         <v>190</v>
       </c>
-      <c r="C2" s="135"/>
-      <c r="D2" s="135"/>
-      <c r="E2" s="135"/>
-      <c r="F2" s="135"/>
-      <c r="G2" s="136"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="132"/>
     </row>
     <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="137"/>
-      <c r="C3" s="138"/>
-      <c r="D3" s="138"/>
-      <c r="E3" s="138"/>
-      <c r="F3" s="138"/>
-      <c r="G3" s="138"/>
-      <c r="H3" s="145" t="s">
+      <c r="B3" s="133"/>
+      <c r="C3" s="134"/>
+      <c r="D3" s="134"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="134"/>
+      <c r="H3" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="146"/>
-      <c r="J3" s="146"/>
-      <c r="K3" s="147"/>
+      <c r="I3" s="142"/>
+      <c r="J3" s="142"/>
+      <c r="K3" s="143"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="141" t="s">
+      <c r="B4" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="143" t="s">
+      <c r="C4" s="139" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="44">
+      <c r="D4" s="40">
         <v>45232</v>
       </c>
-      <c r="E4" s="45">
+      <c r="E4" s="41">
         <v>45239</v>
       </c>
-      <c r="F4" s="45"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="68"/>
-      <c r="K4" s="69"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="65"/>
     </row>
     <row r="5" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="142"/>
-      <c r="C5" s="144"/>
-      <c r="D5" s="81" t="s">
+      <c r="B5" s="138"/>
+      <c r="C5" s="140"/>
+      <c r="D5" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="81" t="s">
+      <c r="E5" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="47"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="70"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="72"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="68"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="37">
+      <c r="B6" s="33">
         <v>1</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="49" t="s">
+      <c r="E6" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="49"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="66"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="62"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="39">
+      <c r="B7" s="35">
         <v>2</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="52"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="48"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="39">
+      <c r="B8" s="35">
         <v>3</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="62"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="52"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="48"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="39">
+      <c r="B9" s="35">
         <v>4</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="52"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="48"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="39">
+      <c r="B10" s="35">
         <v>5</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="52"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="48"/>
     </row>
     <row r="11" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="41">
+      <c r="B11" s="37">
         <v>6</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="55"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="51"/>
     </row>
     <row r="12" spans="2:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="139" t="s">
+      <c r="B12" s="135" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="140"/>
-      <c r="D12" s="43" t="s">
+      <c r="C12" s="136"/>
+      <c r="D12" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="F12" s="35"/>
-      <c r="G12" s="36"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="32"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="E13" t="s">
@@ -4112,14 +4215,14 @@
   <sheetData>
     <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="134" t="s">
+      <c r="B2" s="130" t="s">
         <v>189</v>
       </c>
-      <c r="C2" s="135"/>
-      <c r="D2" s="135"/>
-      <c r="E2" s="135"/>
-      <c r="F2" s="135"/>
-      <c r="G2" s="136"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="132"/>
       <c r="M2">
         <v>1</v>
       </c>
@@ -4128,18 +4231,18 @@
       </c>
     </row>
     <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="137"/>
-      <c r="C3" s="138"/>
-      <c r="D3" s="138"/>
-      <c r="E3" s="138"/>
-      <c r="F3" s="138"/>
-      <c r="G3" s="138"/>
-      <c r="H3" s="145" t="s">
+      <c r="B3" s="133"/>
+      <c r="C3" s="134"/>
+      <c r="D3" s="134"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="134"/>
+      <c r="H3" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="146"/>
-      <c r="J3" s="146"/>
-      <c r="K3" s="147"/>
+      <c r="I3" s="142"/>
+      <c r="J3" s="142"/>
+      <c r="K3" s="143"/>
       <c r="M3">
         <v>2</v>
       </c>
@@ -4148,24 +4251,24 @@
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="141" t="s">
+      <c r="B4" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="143" t="s">
+      <c r="C4" s="139" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="44">
+      <c r="D4" s="40">
         <v>45232</v>
       </c>
-      <c r="E4" s="45">
+      <c r="E4" s="41">
         <v>45234</v>
       </c>
-      <c r="F4" s="45"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="68"/>
-      <c r="K4" s="69"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="65"/>
       <c r="M4">
         <v>3</v>
       </c>
@@ -4174,20 +4277,20 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="142"/>
-      <c r="C5" s="144"/>
-      <c r="D5" s="46" t="s">
+      <c r="B5" s="138"/>
+      <c r="C5" s="140"/>
+      <c r="D5" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="47"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="70"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="72"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="68"/>
       <c r="M5">
         <v>4</v>
       </c>
@@ -4196,24 +4299,24 @@
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="37">
+      <c r="B6" s="33">
         <v>1</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="49" t="s">
+      <c r="E6" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="49"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="66"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="62"/>
       <c r="M6">
         <v>5</v>
       </c>
@@ -4222,18 +4325,18 @@
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="39">
+      <c r="B7" s="35">
         <v>2</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="52"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="48"/>
       <c r="M7">
         <v>6</v>
       </c>
@@ -4242,18 +4345,18 @@
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="39">
+      <c r="B8" s="35">
         <v>3</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="62"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="52"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="48"/>
       <c r="M8">
         <v>7</v>
       </c>
@@ -4262,18 +4365,18 @@
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="39">
+      <c r="B9" s="35">
         <v>4</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="52"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="48"/>
       <c r="M9">
         <v>8</v>
       </c>
@@ -4282,38 +4385,38 @@
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="39">
+      <c r="B10" s="35">
         <v>5</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="52"/>
-      <c r="M10" s="102">
+      <c r="C10" s="36"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="48"/>
+      <c r="M10" s="98">
         <v>9</v>
       </c>
-      <c r="N10" s="102" t="s">
+      <c r="N10" s="98" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="11" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="41">
+      <c r="B11" s="37">
         <v>6</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="55"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="51"/>
       <c r="M11">
         <v>10</v>
       </c>
@@ -4322,18 +4425,18 @@
       </c>
     </row>
     <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="139" t="s">
+      <c r="B12" s="135" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="140"/>
-      <c r="D12" s="43" t="s">
+      <c r="C12" s="136"/>
+      <c r="D12" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="F12" s="35"/>
-      <c r="G12" s="36"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="32"/>
       <c r="M12">
         <v>11</v>
       </c>
@@ -4356,10 +4459,10 @@
       <c r="E14" t="s">
         <v>90</v>
       </c>
-      <c r="M14" s="102">
+      <c r="M14" s="98">
         <v>13</v>
       </c>
-      <c r="N14" s="102" t="s">
+      <c r="N14" s="98" t="s">
         <v>107</v>
       </c>
     </row>
@@ -4501,185 +4604,185 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="134" t="s">
+      <c r="B2" s="130" t="s">
         <v>188</v>
       </c>
-      <c r="C2" s="135"/>
-      <c r="D2" s="135"/>
-      <c r="E2" s="135"/>
-      <c r="F2" s="135"/>
-      <c r="G2" s="135"/>
-      <c r="H2" s="136"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="132"/>
     </row>
     <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="137"/>
-      <c r="C3" s="138"/>
-      <c r="D3" s="138"/>
-      <c r="E3" s="138"/>
-      <c r="F3" s="138"/>
-      <c r="G3" s="138"/>
-      <c r="H3" s="138"/>
-      <c r="I3" s="145" t="s">
+      <c r="B3" s="133"/>
+      <c r="C3" s="134"/>
+      <c r="D3" s="134"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="134"/>
+      <c r="H3" s="134"/>
+      <c r="I3" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="146"/>
-      <c r="K3" s="146"/>
-      <c r="L3" s="147"/>
+      <c r="J3" s="142"/>
+      <c r="K3" s="142"/>
+      <c r="L3" s="143"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="141" t="s">
+      <c r="B4" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="143" t="s">
+      <c r="C4" s="139" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="44">
+      <c r="D4" s="40">
         <v>45234</v>
       </c>
-      <c r="E4" s="45">
+      <c r="E4" s="41">
         <v>45235</v>
       </c>
-      <c r="F4" s="44">
+      <c r="F4" s="40">
         <v>45241</v>
       </c>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="68"/>
-      <c r="K4" s="68"/>
-      <c r="L4" s="69"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="65"/>
     </row>
     <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="142"/>
-      <c r="C5" s="144"/>
-      <c r="D5" s="73" t="s">
+      <c r="B5" s="138"/>
+      <c r="C5" s="140"/>
+      <c r="D5" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="73" t="s">
+      <c r="E5" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="73" t="s">
+      <c r="F5" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="71"/>
-      <c r="L5" s="72"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="68"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="37">
+      <c r="B6" s="33">
         <v>1</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="49" t="s">
+      <c r="E6" s="45" t="s">
         <v>154</v>
       </c>
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="66"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="61"/>
+      <c r="L6" s="62"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="39">
+      <c r="B7" s="35">
         <v>2</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="52"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="48"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="39">
+      <c r="B8" s="35">
         <v>3</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="52"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="48"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="39">
+      <c r="B9" s="35">
         <v>4</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="52"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="48"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="39">
+      <c r="B10" s="35">
         <v>5</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="52"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="48"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="41">
+      <c r="B11" s="37">
         <v>6</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="79"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="54"/>
-      <c r="L11" s="55"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="75"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="51"/>
     </row>
     <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="139" t="s">
+      <c r="B12" s="135" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="140"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="35" t="s">
+      <c r="C12" s="136"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="F12" s="35" t="s">
+      <c r="F12" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="G12" s="75"/>
-      <c r="H12" s="80"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="76"/>
     </row>
     <row r="24" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K24" t="s">
@@ -4703,7 +4806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0268C353-496F-4BD6-A7EF-D042619A03C3}">
   <dimension ref="B1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
@@ -4722,202 +4825,202 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="134" t="s">
+      <c r="B2" s="130" t="s">
         <v>187</v>
       </c>
-      <c r="C2" s="135"/>
-      <c r="D2" s="135"/>
-      <c r="E2" s="135"/>
-      <c r="F2" s="135"/>
-      <c r="G2" s="135"/>
-      <c r="H2" s="136"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="132"/>
     </row>
     <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="137"/>
-      <c r="C3" s="138"/>
-      <c r="D3" s="138"/>
-      <c r="E3" s="138"/>
-      <c r="F3" s="138"/>
-      <c r="G3" s="138"/>
-      <c r="H3" s="138"/>
-      <c r="I3" s="145" t="s">
+      <c r="B3" s="133"/>
+      <c r="C3" s="134"/>
+      <c r="D3" s="134"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="134"/>
+      <c r="H3" s="134"/>
+      <c r="I3" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="146"/>
-      <c r="K3" s="146"/>
-      <c r="L3" s="147"/>
+      <c r="J3" s="142"/>
+      <c r="K3" s="142"/>
+      <c r="L3" s="143"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="141" t="s">
+      <c r="B4" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="143" t="s">
+      <c r="C4" s="139" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="44">
+      <c r="D4" s="40">
         <v>45234</v>
       </c>
-      <c r="E4" s="45">
+      <c r="E4" s="41">
         <v>45235</v>
       </c>
-      <c r="F4" s="44">
+      <c r="F4" s="40">
         <v>45241</v>
       </c>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="44">
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="40">
         <v>45241</v>
       </c>
-      <c r="J4" s="132" t="s">
+      <c r="J4" s="128" t="s">
         <v>161</v>
       </c>
-      <c r="K4" s="132" t="s">
+      <c r="K4" s="128" t="s">
         <v>162</v>
       </c>
-      <c r="L4" s="133" t="s">
+      <c r="L4" s="129" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="142"/>
-      <c r="C5" s="144"/>
-      <c r="D5" s="73" t="s">
+      <c r="B5" s="138"/>
+      <c r="C5" s="140"/>
+      <c r="D5" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="73" t="s">
+      <c r="E5" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="73" t="s">
+      <c r="F5" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="73"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="73" t="s">
+      <c r="G5" s="69"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="J5" s="71"/>
-      <c r="K5" s="71"/>
-      <c r="L5" s="72"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="68"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="37">
+      <c r="B6" s="33">
         <v>1</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="49" t="s">
+      <c r="E6" s="45" t="s">
         <v>154</v>
       </c>
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="59"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="76"/>
-      <c r="J6" s="65">
+      <c r="G6" s="55"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="61">
         <v>48</v>
       </c>
-      <c r="K6" s="65">
+      <c r="K6" s="61">
         <v>9</v>
       </c>
-      <c r="L6" s="66">
+      <c r="L6" s="62">
         <f>(K6/J6)*100</f>
         <v>18.75</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="39">
+      <c r="B7" s="35">
         <v>2</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="78"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="52"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="48"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="39">
+      <c r="B8" s="35">
         <v>3</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="52"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="48"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="39">
+      <c r="B9" s="35">
         <v>4</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="52"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="48"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="39">
+      <c r="B10" s="35">
         <v>5</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="78"/>
-      <c r="I10" s="50"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="52"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="48"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="41">
+      <c r="B11" s="37">
         <v>6</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="78"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="54"/>
-      <c r="L11" s="55"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="51"/>
     </row>
     <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="139" t="s">
+      <c r="B12" s="135" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="140"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="35" t="s">
+      <c r="C12" s="136"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="F12" s="35" t="s">
+      <c r="F12" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="G12" s="75"/>
-      <c r="H12" s="78"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="74"/>
       <c r="J12" t="s">
         <v>191</v>
       </c>
@@ -4951,7 +5054,7 @@
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B12:C12"/>
   </mergeCells>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
Updated Ops of Nov 2023
Updated Ops of Nov 2023
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/Ops-2023-11.xlsx
+++ b/Offline/BusinessManagement/Ops/Ops-2023-11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Ops\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C134008-685F-46A9-82D9-F537A780C28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBA188B-FA5B-49E6-B900-3E430AB18892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="243">
   <si>
     <t>Course</t>
   </si>
@@ -818,6 +818,60 @@
   </si>
   <si>
     <t>Partial Differentiation</t>
+  </si>
+  <si>
+    <t>1) Fluid Mechanics/Hydrostatics</t>
+  </si>
+  <si>
+    <t>Units,Dimension &amp; Measurements</t>
+  </si>
+  <si>
+    <t>Kinematics</t>
+  </si>
+  <si>
+    <t>Laws of Motion</t>
+  </si>
+  <si>
+    <t>Work,Power,Energy</t>
+  </si>
+  <si>
+    <t>Gravitation</t>
+  </si>
+  <si>
+    <t>Elasticity</t>
+  </si>
+  <si>
+    <t>Surface Tension</t>
+  </si>
+  <si>
+    <t>Fluid Mechanics/Hydrostatics</t>
+  </si>
+  <si>
+    <t>Thermal Expansion of Solid</t>
+  </si>
+  <si>
+    <t>Transmission Of Heat</t>
+  </si>
+  <si>
+    <t>Refraction of Light</t>
+  </si>
+  <si>
+    <t>Reflection Of Light</t>
+  </si>
+  <si>
+    <t>Lens</t>
+  </si>
+  <si>
+    <t>Photoelectricity</t>
+  </si>
+  <si>
+    <t>Integral Calculus</t>
+  </si>
+  <si>
+    <t>Ordinary Differntial Equation</t>
+  </si>
+  <si>
+    <t>Probability</t>
   </si>
 </sst>
 </file>
@@ -1580,7 +1634,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1723,14 +1777,8 @@
     <xf numFmtId="14" fontId="7" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1900,6 +1948,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2281,7 +2330,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="92" t="s">
         <v>75</v>
       </c>
       <c r="C1">
@@ -2289,7 +2338,7 @@
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="94" t="s">
+      <c r="B2" s="92" t="s">
         <v>74</v>
       </c>
       <c r="C2">
@@ -2297,7 +2346,7 @@
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="94" t="s">
+      <c r="B3" s="92" t="s">
         <v>73</v>
       </c>
       <c r="C3">
@@ -2305,7 +2354,7 @@
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="94" t="s">
+      <c r="B4" s="92" t="s">
         <v>76</v>
       </c>
       <c r="C4">
@@ -2313,7 +2362,7 @@
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="94" t="s">
+      <c r="B5" s="92" t="s">
         <v>77</v>
       </c>
       <c r="C5">
@@ -2341,7 +2390,7 @@
     <col min="6" max="6" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.44140625" customWidth="1"/>
     <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.88671875" style="105" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.88671875" style="103" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="47.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="47.44140625" bestFit="1" customWidth="1"/>
@@ -2349,54 +2398,54 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="136" t="s">
         <v>183</v>
       </c>
-      <c r="C2" s="139"/>
-      <c r="D2" s="139"/>
-      <c r="E2" s="139"/>
-      <c r="F2" s="139"/>
-      <c r="G2" s="140"/>
-      <c r="M2" s="107" t="s">
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
+      <c r="G2" s="138"/>
+      <c r="M2" s="105" t="s">
         <v>179</v>
       </c>
-      <c r="N2" s="108" t="s">
+      <c r="N2" s="106" t="s">
         <v>177</v>
       </c>
-      <c r="O2" s="107" t="s">
+      <c r="O2" s="105" t="s">
         <v>180</v>
       </c>
-      <c r="P2" s="107" t="s">
+      <c r="P2" s="105" t="s">
         <v>181</v>
       </c>
-      <c r="Q2" s="107" t="s">
+      <c r="Q2" s="105" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="141"/>
-      <c r="C3" s="142"/>
-      <c r="D3" s="142"/>
-      <c r="E3" s="142"/>
-      <c r="F3" s="142"/>
-      <c r="G3" s="142"/>
-      <c r="H3" s="148" t="s">
+      <c r="B3" s="139"/>
+      <c r="C3" s="140"/>
+      <c r="D3" s="140"/>
+      <c r="E3" s="140"/>
+      <c r="F3" s="140"/>
+      <c r="G3" s="140"/>
+      <c r="H3" s="146" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="149"/>
-      <c r="J3" s="149"/>
-      <c r="K3" s="150"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="106"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
-      <c r="Q3" s="72"/>
+      <c r="I3" s="147"/>
+      <c r="J3" s="147"/>
+      <c r="K3" s="148"/>
+      <c r="M3" s="70"/>
+      <c r="N3" s="104"/>
+      <c r="O3" s="70"/>
+      <c r="P3" s="70"/>
+      <c r="Q3" s="70"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="144" t="s">
+      <c r="B4" s="142" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="146" t="s">
+      <c r="C4" s="144" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="39">
@@ -2413,670 +2462,670 @@
       <c r="I4" s="62"/>
       <c r="J4" s="62"/>
       <c r="K4" s="63"/>
-      <c r="M4" s="96" t="s">
+      <c r="M4" s="94" t="s">
         <v>122</v>
       </c>
-      <c r="N4" s="106">
+      <c r="N4" s="104">
         <v>1</v>
       </c>
-      <c r="O4" s="99" t="s">
+      <c r="O4" s="97" t="s">
         <v>125</v>
       </c>
-      <c r="P4" s="72">
+      <c r="P4" s="70">
         <v>1</v>
       </c>
-      <c r="Q4" s="72"/>
+      <c r="Q4" s="70"/>
     </row>
     <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="145"/>
-      <c r="C5" s="147"/>
-      <c r="D5" s="75" t="s">
+      <c r="B5" s="143"/>
+      <c r="C5" s="145"/>
+      <c r="D5" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="75" t="s">
+      <c r="E5" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="75" t="s">
+      <c r="F5" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="109"/>
+      <c r="G5" s="107"/>
       <c r="H5" s="64"/>
       <c r="I5" s="65"/>
       <c r="J5" s="65"/>
       <c r="K5" s="66"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="106">
+      <c r="M5" s="70"/>
+      <c r="N5" s="104">
         <v>2</v>
       </c>
-      <c r="O5" s="99" t="s">
+      <c r="O5" s="97" t="s">
         <v>128</v>
       </c>
-      <c r="P5" s="72">
+      <c r="P5" s="70">
         <v>1</v>
       </c>
-      <c r="Q5" s="72"/>
+      <c r="Q5" s="70"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B6" s="110">
+      <c r="B6" s="108">
         <v>1</v>
       </c>
-      <c r="C6" s="111" t="s">
+      <c r="C6" s="109" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="112" t="s">
+      <c r="D6" s="110" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="113" t="s">
+      <c r="E6" s="111" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="112" t="s">
+      <c r="F6" s="110" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="114"/>
+      <c r="G6" s="112"/>
       <c r="H6" s="58"/>
       <c r="I6" s="59"/>
       <c r="J6" s="59"/>
       <c r="K6" s="60"/>
-      <c r="M6" s="72"/>
-      <c r="N6" s="106">
+      <c r="M6" s="70"/>
+      <c r="N6" s="104">
         <v>3</v>
       </c>
-      <c r="O6" s="99" t="s">
+      <c r="O6" s="97" t="s">
         <v>131</v>
       </c>
-      <c r="P6" s="72">
+      <c r="P6" s="70">
         <v>1</v>
       </c>
-      <c r="Q6" s="72"/>
+      <c r="Q6" s="70"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B7" s="115">
+      <c r="B7" s="113">
         <v>2</v>
       </c>
-      <c r="C7" s="116"/>
-      <c r="D7" s="117"/>
-      <c r="E7" s="118"/>
-      <c r="F7" s="118"/>
-      <c r="G7" s="119"/>
+      <c r="C7" s="114"/>
+      <c r="D7" s="115"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="116"/>
+      <c r="G7" s="117"/>
       <c r="H7" s="56"/>
       <c r="I7" s="45"/>
       <c r="J7" s="45"/>
       <c r="K7" s="46"/>
-      <c r="M7" s="72"/>
-      <c r="N7" s="106">
+      <c r="M7" s="70"/>
+      <c r="N7" s="104">
         <v>4</v>
       </c>
-      <c r="O7" s="99" t="s">
+      <c r="O7" s="97" t="s">
         <v>133</v>
       </c>
-      <c r="P7" s="72">
+      <c r="P7" s="70">
         <v>1</v>
       </c>
-      <c r="Q7" s="72"/>
+      <c r="Q7" s="70"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B8" s="115">
+      <c r="B8" s="113">
         <v>3</v>
       </c>
-      <c r="C8" s="116"/>
-      <c r="D8" s="117"/>
-      <c r="E8" s="118"/>
-      <c r="F8" s="118"/>
-      <c r="G8" s="119"/>
+      <c r="C8" s="114"/>
+      <c r="D8" s="115"/>
+      <c r="E8" s="116"/>
+      <c r="F8" s="116"/>
+      <c r="G8" s="117"/>
       <c r="H8" s="56"/>
       <c r="I8" s="45"/>
       <c r="J8" s="45"/>
       <c r="K8" s="46"/>
-      <c r="M8" s="72"/>
-      <c r="N8" s="106">
+      <c r="M8" s="70"/>
+      <c r="N8" s="104">
         <v>5</v>
       </c>
-      <c r="O8" s="99" t="s">
+      <c r="O8" s="97" t="s">
         <v>136</v>
       </c>
-      <c r="P8" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="72"/>
+      <c r="P8" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="70"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B9" s="115">
+      <c r="B9" s="113">
         <v>4</v>
       </c>
-      <c r="C9" s="116"/>
-      <c r="D9" s="117"/>
-      <c r="E9" s="118"/>
-      <c r="F9" s="118"/>
-      <c r="G9" s="119"/>
+      <c r="C9" s="114"/>
+      <c r="D9" s="115"/>
+      <c r="E9" s="116"/>
+      <c r="F9" s="116"/>
+      <c r="G9" s="117"/>
       <c r="H9" s="56"/>
       <c r="I9" s="45"/>
       <c r="J9" s="45"/>
       <c r="K9" s="46"/>
-      <c r="M9" s="72"/>
-      <c r="N9" s="106">
+      <c r="M9" s="70"/>
+      <c r="N9" s="104">
         <v>6</v>
       </c>
-      <c r="O9" s="99" t="s">
+      <c r="O9" s="97" t="s">
         <v>138</v>
       </c>
-      <c r="P9" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="72"/>
+      <c r="P9" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="70"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B10" s="115">
+      <c r="B10" s="113">
         <v>5</v>
       </c>
-      <c r="C10" s="116"/>
-      <c r="D10" s="117"/>
-      <c r="E10" s="118"/>
-      <c r="F10" s="118"/>
-      <c r="G10" s="119"/>
+      <c r="C10" s="114"/>
+      <c r="D10" s="115"/>
+      <c r="E10" s="116"/>
+      <c r="F10" s="116"/>
+      <c r="G10" s="117"/>
       <c r="H10" s="56"/>
       <c r="I10" s="45"/>
       <c r="J10" s="45"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="72"/>
-      <c r="N10" s="106">
+      <c r="M10" s="70"/>
+      <c r="N10" s="104">
         <v>7</v>
       </c>
-      <c r="O10" s="102" t="s">
+      <c r="O10" s="100" t="s">
         <v>141</v>
       </c>
-      <c r="P10" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="72"/>
+      <c r="P10" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="70"/>
     </row>
     <row r="11" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="120">
+      <c r="B11" s="118">
         <v>6</v>
       </c>
-      <c r="C11" s="121"/>
-      <c r="D11" s="122"/>
-      <c r="E11" s="123"/>
-      <c r="F11" s="123"/>
-      <c r="G11" s="124"/>
+      <c r="C11" s="119"/>
+      <c r="D11" s="120"/>
+      <c r="E11" s="121"/>
+      <c r="F11" s="121"/>
+      <c r="G11" s="122"/>
       <c r="H11" s="57"/>
       <c r="I11" s="48"/>
       <c r="J11" s="48"/>
       <c r="K11" s="49"/>
-      <c r="M11" s="72"/>
-      <c r="N11" s="106">
+      <c r="M11" s="70"/>
+      <c r="N11" s="104">
         <v>8</v>
       </c>
-      <c r="O11" s="99" t="s">
+      <c r="O11" s="97" t="s">
         <v>144</v>
       </c>
-      <c r="P11" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="72"/>
+      <c r="P11" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="70"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="143" t="s">
+      <c r="B12" s="141" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="143"/>
-      <c r="D12" s="104" t="s">
+      <c r="C12" s="141"/>
+      <c r="D12" s="102" t="s">
         <v>161</v>
       </c>
-      <c r="E12" s="74" t="s">
+      <c r="E12" s="72" t="s">
         <v>165</v>
       </c>
-      <c r="F12" s="74" t="s">
+      <c r="F12" s="72" t="s">
         <v>170</v>
       </c>
-      <c r="G12" s="74"/>
-      <c r="M12" s="72"/>
-      <c r="N12" s="106">
+      <c r="G12" s="72"/>
+      <c r="M12" s="70"/>
+      <c r="N12" s="104">
         <v>9</v>
       </c>
-      <c r="O12" s="103" t="s">
+      <c r="O12" s="101" t="s">
         <v>145</v>
       </c>
-      <c r="P12" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="72"/>
+      <c r="P12" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="70"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="104" t="s">
+      <c r="B13" s="72"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="102" t="s">
         <v>162</v>
       </c>
-      <c r="E13" s="104" t="s">
+      <c r="E13" s="102" t="s">
         <v>166</v>
       </c>
-      <c r="F13" s="74" t="s">
+      <c r="F13" s="72" t="s">
         <v>171</v>
       </c>
-      <c r="G13" s="74"/>
-      <c r="M13" s="72"/>
-      <c r="N13" s="106">
+      <c r="G13" s="72"/>
+      <c r="M13" s="70"/>
+      <c r="N13" s="104">
         <v>10</v>
       </c>
-      <c r="O13" s="99" t="s">
+      <c r="O13" s="97" t="s">
         <v>146</v>
       </c>
-      <c r="P13" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="72" t="s">
+      <c r="P13" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="70" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74" t="s">
+      <c r="B14" s="72"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72" t="s">
         <v>163</v>
       </c>
-      <c r="E14" s="104" t="s">
+      <c r="E14" s="102" t="s">
         <v>167</v>
       </c>
-      <c r="F14" s="74" t="s">
+      <c r="F14" s="72" t="s">
         <v>172</v>
       </c>
-      <c r="G14" s="74"/>
-      <c r="M14" s="72"/>
-      <c r="N14" s="106">
+      <c r="G14" s="72"/>
+      <c r="M14" s="70"/>
+      <c r="N14" s="104">
         <v>11</v>
       </c>
-      <c r="O14" s="99" t="s">
+      <c r="O14" s="97" t="s">
         <v>147</v>
       </c>
-      <c r="P14" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="72"/>
+      <c r="P14" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="70"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B15" s="74"/>
-      <c r="C15" s="74"/>
-      <c r="D15" s="74" t="s">
+      <c r="B15" s="72"/>
+      <c r="C15" s="72"/>
+      <c r="D15" s="72" t="s">
         <v>164</v>
       </c>
-      <c r="E15" s="74" t="s">
+      <c r="E15" s="72" t="s">
         <v>168</v>
       </c>
-      <c r="F15" s="74" t="s">
+      <c r="F15" s="72" t="s">
         <v>175</v>
       </c>
-      <c r="G15" s="74"/>
-      <c r="M15" s="72"/>
-      <c r="N15" s="106">
+      <c r="G15" s="72"/>
+      <c r="M15" s="70"/>
+      <c r="N15" s="104">
         <v>12</v>
       </c>
-      <c r="O15" s="99" t="s">
+      <c r="O15" s="97" t="s">
         <v>148</v>
       </c>
-      <c r="P15" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="72"/>
+      <c r="P15" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="70"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B16" s="74"/>
-      <c r="C16" s="74"/>
-      <c r="D16" s="74"/>
-      <c r="E16" s="74" t="s">
+      <c r="B16" s="72"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="F16" s="74" t="s">
+      <c r="F16" s="72" t="s">
         <v>176</v>
       </c>
-      <c r="G16" s="74"/>
-      <c r="M16" s="97" t="s">
+      <c r="G16" s="72"/>
+      <c r="M16" s="95" t="s">
         <v>123</v>
       </c>
-      <c r="N16" s="106">
+      <c r="N16" s="104">
         <v>13</v>
       </c>
-      <c r="O16" s="100" t="s">
+      <c r="O16" s="98" t="s">
         <v>126</v>
       </c>
-      <c r="P16" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="72"/>
+      <c r="P16" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="70"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B17" s="74"/>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74"/>
-      <c r="E17" s="74" t="s">
+      <c r="B17" s="72"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="72" t="s">
         <v>173</v>
       </c>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74"/>
-      <c r="M17" s="72"/>
-      <c r="N17" s="106">
+      <c r="F17" s="72"/>
+      <c r="G17" s="72"/>
+      <c r="M17" s="70"/>
+      <c r="N17" s="104">
         <v>14</v>
       </c>
-      <c r="O17" s="100" t="s">
+      <c r="O17" s="98" t="s">
         <v>129</v>
       </c>
-      <c r="P17" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="72"/>
+      <c r="P17" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="70"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B18" s="74"/>
-      <c r="C18" s="74"/>
-      <c r="D18" s="74"/>
-      <c r="E18" s="74" t="s">
+      <c r="B18" s="72"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="72" t="s">
         <v>174</v>
       </c>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74"/>
-      <c r="M18" s="72"/>
-      <c r="N18" s="106">
+      <c r="F18" s="72"/>
+      <c r="G18" s="72"/>
+      <c r="M18" s="70"/>
+      <c r="N18" s="104">
         <v>15</v>
       </c>
-      <c r="O18" s="100" t="s">
+      <c r="O18" s="98" t="s">
         <v>132</v>
       </c>
-      <c r="P18" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="72"/>
+      <c r="P18" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="70"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M19" s="72"/>
-      <c r="N19" s="106">
+      <c r="M19" s="70"/>
+      <c r="N19" s="104">
         <v>16</v>
       </c>
-      <c r="O19" s="100" t="s">
+      <c r="O19" s="98" t="s">
         <v>134</v>
       </c>
-      <c r="P19" s="72">
+      <c r="P19" s="70">
         <v>1</v>
       </c>
-      <c r="Q19" s="72"/>
+      <c r="Q19" s="70"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M20" s="72"/>
-      <c r="N20" s="106">
+      <c r="M20" s="70"/>
+      <c r="N20" s="104">
         <v>17</v>
       </c>
-      <c r="O20" s="100" t="s">
+      <c r="O20" s="98" t="s">
         <v>137</v>
       </c>
-      <c r="P20" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="72"/>
+      <c r="P20" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="70"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M21" s="72"/>
-      <c r="N21" s="106">
+      <c r="M21" s="70"/>
+      <c r="N21" s="104">
         <v>18</v>
       </c>
-      <c r="O21" s="100" t="s">
+      <c r="O21" s="98" t="s">
         <v>139</v>
       </c>
-      <c r="P21" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="72"/>
+      <c r="P21" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="70"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M22" s="72"/>
-      <c r="N22" s="106">
+      <c r="M22" s="70"/>
+      <c r="N22" s="104">
         <v>19</v>
       </c>
-      <c r="O22" s="100" t="s">
+      <c r="O22" s="98" t="s">
         <v>142</v>
       </c>
-      <c r="P22" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="72"/>
+      <c r="P22" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="70"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M23" s="72"/>
-      <c r="N23" s="106">
+      <c r="M23" s="70"/>
+      <c r="N23" s="104">
         <v>20</v>
       </c>
-      <c r="O23" s="100" t="s">
+      <c r="O23" s="98" t="s">
         <v>142</v>
       </c>
-      <c r="P23" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="72"/>
+      <c r="P23" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="70"/>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M24" s="72"/>
-      <c r="N24" s="106">
+      <c r="M24" s="70"/>
+      <c r="N24" s="104">
         <v>21</v>
       </c>
-      <c r="O24" s="100" t="s">
+      <c r="O24" s="98" t="s">
         <v>142</v>
       </c>
-      <c r="P24" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="72"/>
+      <c r="P24" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="70"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M25" s="72"/>
-      <c r="N25" s="106">
+      <c r="M25" s="70"/>
+      <c r="N25" s="104">
         <v>22</v>
       </c>
-      <c r="O25" s="100" t="s">
+      <c r="O25" s="98" t="s">
         <v>142</v>
       </c>
-      <c r="P25" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="72"/>
+      <c r="P25" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="70"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M26" s="72"/>
-      <c r="N26" s="106">
+      <c r="M26" s="70"/>
+      <c r="N26" s="104">
         <v>23</v>
       </c>
-      <c r="O26" s="100" t="s">
+      <c r="O26" s="98" t="s">
         <v>142</v>
       </c>
-      <c r="P26" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="72"/>
+      <c r="P26" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="70"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M27" s="72"/>
-      <c r="N27" s="106">
+      <c r="M27" s="70"/>
+      <c r="N27" s="104">
         <v>24</v>
       </c>
-      <c r="O27" s="100" t="s">
+      <c r="O27" s="98" t="s">
         <v>142</v>
       </c>
-      <c r="P27" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="72"/>
+      <c r="P27" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="70"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M28" s="98" t="s">
+      <c r="M28" s="96" t="s">
         <v>124</v>
       </c>
-      <c r="N28" s="106">
+      <c r="N28" s="104">
         <v>25</v>
       </c>
-      <c r="O28" s="101" t="s">
+      <c r="O28" s="99" t="s">
         <v>127</v>
       </c>
-      <c r="P28" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="72" t="s">
+      <c r="P28" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="70" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M29" s="72"/>
-      <c r="N29" s="106">
+      <c r="M29" s="70"/>
+      <c r="N29" s="104">
         <v>26</v>
       </c>
-      <c r="O29" s="101" t="s">
+      <c r="O29" s="99" t="s">
         <v>130</v>
       </c>
-      <c r="P29" s="72">
+      <c r="P29" s="70">
         <v>1</v>
       </c>
-      <c r="Q29" s="72"/>
+      <c r="Q29" s="70"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M30" s="72"/>
-      <c r="N30" s="106">
+      <c r="M30" s="70"/>
+      <c r="N30" s="104">
         <v>27</v>
       </c>
-      <c r="O30" s="101" t="s">
+      <c r="O30" s="99" t="s">
         <v>135</v>
       </c>
-      <c r="P30" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="72"/>
+      <c r="P30" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="70"/>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M31" s="72"/>
-      <c r="N31" s="106">
+      <c r="M31" s="70"/>
+      <c r="N31" s="104">
         <v>28</v>
       </c>
-      <c r="O31" s="101" t="s">
+      <c r="O31" s="99" t="s">
         <v>140</v>
       </c>
-      <c r="P31" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="72"/>
+      <c r="P31" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="70"/>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M32" s="72"/>
-      <c r="N32" s="106">
+      <c r="M32" s="70"/>
+      <c r="N32" s="104">
         <v>29</v>
       </c>
-      <c r="O32" s="101" t="s">
+      <c r="O32" s="99" t="s">
         <v>143</v>
       </c>
-      <c r="P32" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q32" s="72"/>
+      <c r="P32" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="70"/>
     </row>
     <row r="33" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M33" s="72"/>
-      <c r="N33" s="106">
+      <c r="M33" s="70"/>
+      <c r="N33" s="104">
         <v>30</v>
       </c>
-      <c r="O33" s="101" t="s">
+      <c r="O33" s="99" t="s">
         <v>142</v>
       </c>
-      <c r="P33" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q33" s="72"/>
+      <c r="P33" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="70"/>
     </row>
     <row r="34" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M34" s="72"/>
-      <c r="N34" s="106">
+      <c r="M34" s="70"/>
+      <c r="N34" s="104">
         <v>31</v>
       </c>
-      <c r="O34" s="101" t="s">
+      <c r="O34" s="99" t="s">
         <v>142</v>
       </c>
-      <c r="P34" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q34" s="72"/>
+      <c r="P34" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="70"/>
     </row>
     <row r="35" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M35" s="72"/>
-      <c r="N35" s="106">
+      <c r="M35" s="70"/>
+      <c r="N35" s="104">
         <v>32</v>
       </c>
-      <c r="O35" s="101" t="s">
+      <c r="O35" s="99" t="s">
         <v>142</v>
       </c>
-      <c r="P35" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q35" s="72"/>
+      <c r="P35" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="70"/>
     </row>
     <row r="36" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M36" s="72"/>
-      <c r="N36" s="106">
+      <c r="M36" s="70"/>
+      <c r="N36" s="104">
         <v>33</v>
       </c>
-      <c r="O36" s="101" t="s">
+      <c r="O36" s="99" t="s">
         <v>142</v>
       </c>
-      <c r="P36" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q36" s="72"/>
+      <c r="P36" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="70"/>
     </row>
     <row r="37" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M37" s="72"/>
-      <c r="N37" s="106">
+      <c r="M37" s="70"/>
+      <c r="N37" s="104">
         <v>34</v>
       </c>
-      <c r="O37" s="101" t="s">
+      <c r="O37" s="99" t="s">
         <v>142</v>
       </c>
-      <c r="P37" s="72">
-        <v>0</v>
-      </c>
-      <c r="Q37" s="72"/>
+      <c r="P37" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="70"/>
     </row>
     <row r="38" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M38" s="72"/>
-      <c r="N38" s="106"/>
-      <c r="O38" s="72"/>
-      <c r="P38" s="72"/>
-      <c r="Q38" s="72"/>
+      <c r="M38" s="70"/>
+      <c r="N38" s="104"/>
+      <c r="O38" s="70"/>
+      <c r="P38" s="70"/>
+      <c r="Q38" s="70"/>
     </row>
     <row r="39" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M39" s="72"/>
-      <c r="N39" s="106"/>
-      <c r="O39" s="98" t="s">
+      <c r="M39" s="70"/>
+      <c r="N39" s="104"/>
+      <c r="O39" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="P39" s="74">
+      <c r="P39" s="72">
         <f>SUM(P4:P37)</f>
         <v>6</v>
       </c>
-      <c r="Q39" s="72"/>
+      <c r="Q39" s="70"/>
     </row>
     <row r="40" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M40" s="72"/>
-      <c r="N40" s="106"/>
-      <c r="O40" s="98" t="s">
+      <c r="M40" s="70"/>
+      <c r="N40" s="104"/>
+      <c r="O40" s="96" t="s">
         <v>182</v>
       </c>
-      <c r="P40" s="74">
+      <c r="P40" s="72">
         <v>34</v>
       </c>
-      <c r="Q40" s="72"/>
+      <c r="Q40" s="70"/>
     </row>
     <row r="41" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M41" s="72"/>
-      <c r="N41" s="106"/>
-      <c r="O41" s="98" t="s">
+      <c r="M41" s="70"/>
+      <c r="N41" s="104"/>
+      <c r="O41" s="96" t="s">
         <v>178</v>
       </c>
-      <c r="P41" s="74">
+      <c r="P41" s="72">
         <f>ROUND((P39/P40)*100,2)</f>
         <v>17.649999999999999</v>
       </c>
-      <c r="Q41" s="72"/>
+      <c r="Q41" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3177,9 +3226,9 @@
         <f>G3-H3</f>
         <v>0</v>
       </c>
-      <c r="J3" s="95"/>
-      <c r="K3" s="95"/>
-      <c r="L3" s="95"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
       <c r="M3" s="10" t="s">
         <v>27</v>
       </c>
@@ -3254,7 +3303,7 @@
       <c r="K6" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L6" s="92">
+      <c r="L6" s="90">
         <v>45239</v>
       </c>
       <c r="M6" s="19" t="s">
@@ -3329,7 +3378,7 @@
       <c r="K9" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="L9" s="93">
+      <c r="L9" s="91">
         <v>45239</v>
       </c>
       <c r="M9" s="10" t="s">
@@ -3404,7 +3453,7 @@
       <c r="K12" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L12" s="92">
+      <c r="L12" s="90">
         <v>45239</v>
       </c>
       <c r="M12" s="19" t="s">
@@ -3431,23 +3480,23 @@
       <c r="M13" s="21"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="127"/>
-      <c r="C14" s="128"/>
-      <c r="D14" s="128"/>
-      <c r="E14" s="128">
+      <c r="B14" s="125"/>
+      <c r="C14" s="126"/>
+      <c r="D14" s="126"/>
+      <c r="E14" s="126">
         <v>3</v>
       </c>
-      <c r="F14" s="128"/>
-      <c r="G14" s="128"/>
-      <c r="H14" s="128"/>
-      <c r="I14" s="128">
+      <c r="F14" s="126"/>
+      <c r="G14" s="126"/>
+      <c r="H14" s="126"/>
+      <c r="I14" s="126">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J14" s="128"/>
-      <c r="K14" s="128"/>
-      <c r="L14" s="128"/>
-      <c r="M14" s="129"/>
+      <c r="J14" s="126"/>
+      <c r="K14" s="126"/>
+      <c r="L14" s="126"/>
+      <c r="M14" s="127"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
@@ -3476,7 +3525,7 @@
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="132">
+      <c r="L15" s="130">
         <v>45234</v>
       </c>
       <c r="M15" s="1" t="s">
@@ -3512,18 +3561,18 @@
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F18" s="130" t="s">
+      <c r="F18" s="128" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="131">
+      <c r="G18" s="129">
         <f>SUM(G3:G17)</f>
         <v>22000</v>
       </c>
-      <c r="H18" s="131">
+      <c r="H18" s="129">
         <f t="shared" ref="H18:I18" si="1">SUM(H3:H17)</f>
         <v>17000</v>
       </c>
-      <c r="I18" s="131">
+      <c r="I18" s="129">
         <f t="shared" si="1"/>
         <v>15000</v>
       </c>
@@ -3618,7 +3667,7 @@
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="75" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -3650,7 +3699,7 @@
       <c r="Q3" s="10"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="78"/>
+      <c r="B4" s="76"/>
       <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
@@ -3678,38 +3727,38 @@
       <c r="Q4" s="12"/>
     </row>
     <row r="5" spans="2:17" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="82"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="84" t="s">
+      <c r="B5" s="80"/>
+      <c r="C5" s="82"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="82" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="84">
+      <c r="H5" s="82">
         <f>SUM(F3:G4)</f>
         <v>4500</v>
       </c>
-      <c r="I5" s="84">
+      <c r="I5" s="82">
         <f>H5</f>
         <v>4500</v>
       </c>
-      <c r="J5" s="85">
+      <c r="J5" s="83">
         <v>45239</v>
       </c>
-      <c r="K5" s="84"/>
-      <c r="L5" s="84"/>
-      <c r="M5" s="84"/>
-      <c r="N5" s="83"/>
-      <c r="O5" s="83"/>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="86"/>
+      <c r="K5" s="82"/>
+      <c r="L5" s="82"/>
+      <c r="M5" s="82"/>
+      <c r="N5" s="81"/>
+      <c r="O5" s="81"/>
+      <c r="P5" s="81"/>
+      <c r="Q5" s="84"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="89" t="s">
+      <c r="B6" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="91" t="s">
+      <c r="C6" s="89" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="18" t="s">
@@ -3742,8 +3791,8 @@
       <c r="Q6" s="19"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="79"/>
-      <c r="C7" s="88" t="s">
+      <c r="B7" s="77"/>
+      <c r="C7" s="86" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -3770,7 +3819,7 @@
       <c r="Q7" s="21"/>
     </row>
     <row r="8" spans="2:17" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="80"/>
+      <c r="B8" s="78"/>
       <c r="C8" s="23"/>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
@@ -3786,7 +3835,7 @@
         <f>H8</f>
         <v>6000</v>
       </c>
-      <c r="J8" s="81">
+      <c r="J8" s="79">
         <v>45239</v>
       </c>
       <c r="K8" s="30"/>
@@ -3798,21 +3847,21 @@
       <c r="Q8" s="24"/>
     </row>
     <row r="9" spans="2:17" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G9" s="90" t="s">
+      <c r="G9" s="88" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="87">
+      <c r="H9" s="85">
         <f>SUM(H3:H8)</f>
         <v>10500</v>
       </c>
-      <c r="I9" s="87">
+      <c r="I9" s="85">
         <f>SUM(I3:I8)</f>
         <v>10500</v>
       </c>
-      <c r="J9" s="76"/>
-      <c r="K9" s="76"/>
-      <c r="L9" s="76"/>
-      <c r="M9" s="76"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="74"/>
+      <c r="L9" s="74"/>
+      <c r="M9" s="74"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3854,35 +3903,35 @@
     <col min="10" max="10" width="48.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="94" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="94" t="s">
+    <row r="1" spans="1:10" s="92" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="92" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="94" t="s">
+      <c r="C1" s="92" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="94" t="s">
+      <c r="D1" s="92" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="94" t="s">
+      <c r="E1" s="92" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="94" t="s">
+      <c r="F1" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="94" t="s">
+      <c r="G1" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="94" t="s">
+      <c r="H1" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="94" t="s">
+      <c r="I1" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="94" t="s">
+      <c r="J1" s="92" t="s">
         <v>71</v>
       </c>
     </row>
@@ -4100,57 +4149,57 @@
     <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.77734375" style="105" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.77734375" style="103" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="47.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5546875" style="105" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5546875" style="103" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="136" t="s">
         <v>187</v>
       </c>
-      <c r="C2" s="139"/>
-      <c r="D2" s="139"/>
-      <c r="E2" s="139"/>
-      <c r="F2" s="139"/>
-      <c r="G2" s="140"/>
-      <c r="M2" s="135" t="s">
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
+      <c r="G2" s="138"/>
+      <c r="M2" s="133" t="s">
         <v>177</v>
       </c>
-      <c r="N2" s="74" t="s">
+      <c r="N2" s="72" t="s">
         <v>180</v>
       </c>
-      <c r="O2" s="135" t="s">
+      <c r="O2" s="133" t="s">
         <v>197</v>
       </c>
-      <c r="P2" s="74" t="s">
+      <c r="P2" s="72" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="141"/>
-      <c r="C3" s="142"/>
-      <c r="D3" s="142"/>
-      <c r="E3" s="142"/>
-      <c r="F3" s="142"/>
-      <c r="G3" s="142"/>
-      <c r="H3" s="148" t="s">
+      <c r="B3" s="139"/>
+      <c r="C3" s="140"/>
+      <c r="D3" s="140"/>
+      <c r="E3" s="140"/>
+      <c r="F3" s="140"/>
+      <c r="G3" s="140"/>
+      <c r="H3" s="146" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="149"/>
-      <c r="J3" s="149"/>
-      <c r="K3" s="150"/>
-      <c r="M3" s="106"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="106"/>
-      <c r="P3" s="72"/>
+      <c r="I3" s="147"/>
+      <c r="J3" s="147"/>
+      <c r="K3" s="148"/>
+      <c r="M3" s="104"/>
+      <c r="N3" s="70"/>
+      <c r="O3" s="104"/>
+      <c r="P3" s="70"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="144" t="s">
+      <c r="B4" s="142" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="146" t="s">
+      <c r="C4" s="144" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="39">
@@ -4167,27 +4216,27 @@
       <c r="I4" s="62"/>
       <c r="J4" s="62"/>
       <c r="K4" s="63"/>
-      <c r="M4" s="106">
+      <c r="M4" s="104">
         <v>1</v>
       </c>
-      <c r="N4" s="72" t="s">
+      <c r="N4" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="O4" s="106">
-        <v>0</v>
-      </c>
-      <c r="P4" s="72"/>
+      <c r="O4" s="104">
+        <v>0</v>
+      </c>
+      <c r="P4" s="70"/>
     </row>
     <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="145"/>
-      <c r="C5" s="147"/>
-      <c r="D5" s="75" t="s">
+      <c r="B5" s="143"/>
+      <c r="C5" s="145"/>
+      <c r="D5" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="75" t="s">
+      <c r="E5" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="75" t="s">
+      <c r="F5" s="73" t="s">
         <v>47</v>
       </c>
       <c r="G5" s="52"/>
@@ -4195,16 +4244,16 @@
       <c r="I5" s="65"/>
       <c r="J5" s="65"/>
       <c r="K5" s="66"/>
-      <c r="M5" s="106">
+      <c r="M5" s="104">
         <v>2</v>
       </c>
-      <c r="N5" s="72" t="s">
+      <c r="N5" s="70" t="s">
         <v>93</v>
       </c>
-      <c r="O5" s="106">
-        <v>0</v>
-      </c>
-      <c r="P5" s="72"/>
+      <c r="O5" s="104">
+        <v>0</v>
+      </c>
+      <c r="P5" s="70"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="32">
@@ -4227,16 +4276,16 @@
       <c r="I6" s="59"/>
       <c r="J6" s="59"/>
       <c r="K6" s="60"/>
-      <c r="M6" s="106">
+      <c r="M6" s="104">
         <v>3</v>
       </c>
-      <c r="N6" s="72" t="s">
+      <c r="N6" s="70" t="s">
         <v>94</v>
       </c>
-      <c r="O6" s="106">
-        <v>0</v>
-      </c>
-      <c r="P6" s="72"/>
+      <c r="O6" s="104">
+        <v>0</v>
+      </c>
+      <c r="P6" s="70"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="34">
@@ -4251,16 +4300,16 @@
       <c r="I7" s="45"/>
       <c r="J7" s="45"/>
       <c r="K7" s="46"/>
-      <c r="M7" s="106">
+      <c r="M7" s="104">
         <v>4</v>
       </c>
-      <c r="N7" s="72" t="s">
+      <c r="N7" s="70" t="s">
         <v>95</v>
       </c>
-      <c r="O7" s="106">
-        <v>0</v>
-      </c>
-      <c r="P7" s="72"/>
+      <c r="O7" s="104">
+        <v>0</v>
+      </c>
+      <c r="P7" s="70"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="34">
@@ -4275,16 +4324,16 @@
       <c r="I8" s="45"/>
       <c r="J8" s="45"/>
       <c r="K8" s="46"/>
-      <c r="M8" s="106">
+      <c r="M8" s="104">
         <v>5</v>
       </c>
-      <c r="N8" s="72" t="s">
+      <c r="N8" s="70" t="s">
         <v>96</v>
       </c>
-      <c r="O8" s="106">
-        <v>0</v>
-      </c>
-      <c r="P8" s="72"/>
+      <c r="O8" s="104">
+        <v>0</v>
+      </c>
+      <c r="P8" s="70"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" s="34">
@@ -4299,16 +4348,16 @@
       <c r="I9" s="45"/>
       <c r="J9" s="45"/>
       <c r="K9" s="46"/>
-      <c r="M9" s="106">
+      <c r="M9" s="104">
         <v>6</v>
       </c>
-      <c r="N9" s="72" t="s">
+      <c r="N9" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="O9" s="106">
-        <v>0</v>
-      </c>
-      <c r="P9" s="72"/>
+      <c r="O9" s="104">
+        <v>0</v>
+      </c>
+      <c r="P9" s="70"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" s="34">
@@ -4323,329 +4372,329 @@
       <c r="I10" s="45"/>
       <c r="J10" s="45"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="106">
+      <c r="M10" s="104">
         <v>7</v>
       </c>
-      <c r="N10" s="72" t="s">
+      <c r="N10" s="70" t="s">
         <v>98</v>
       </c>
-      <c r="O10" s="106">
-        <v>0</v>
-      </c>
-      <c r="P10" s="72"/>
+      <c r="O10" s="104">
+        <v>0</v>
+      </c>
+      <c r="P10" s="70"/>
     </row>
     <row r="11" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="106">
+      <c r="B11" s="104">
         <v>6</v>
       </c>
-      <c r="C11" s="74"/>
-      <c r="D11" s="118"/>
-      <c r="E11" s="118"/>
-      <c r="F11" s="118"/>
-      <c r="G11" s="118"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="116"/>
+      <c r="E11" s="116"/>
+      <c r="F11" s="116"/>
+      <c r="G11" s="116"/>
       <c r="H11" s="47"/>
       <c r="I11" s="48"/>
       <c r="J11" s="48"/>
       <c r="K11" s="49"/>
-      <c r="M11" s="106">
+      <c r="M11" s="104">
         <v>8</v>
       </c>
-      <c r="N11" s="72" t="s">
+      <c r="N11" s="70" t="s">
         <v>99</v>
       </c>
-      <c r="O11" s="106">
-        <v>0</v>
-      </c>
-      <c r="P11" s="72"/>
+      <c r="O11" s="104">
+        <v>0</v>
+      </c>
+      <c r="P11" s="70"/>
     </row>
     <row r="12" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="143" t="s">
+      <c r="B12" s="141" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="143"/>
-      <c r="D12" s="72" t="s">
+      <c r="C12" s="141"/>
+      <c r="D12" s="70" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="72" t="s">
+      <c r="E12" s="70" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="72" t="s">
+      <c r="F12" s="70" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="72"/>
-      <c r="M12" s="133">
+      <c r="G12" s="70"/>
+      <c r="M12" s="131">
         <v>9</v>
       </c>
-      <c r="N12" s="134" t="s">
+      <c r="N12" s="132" t="s">
         <v>100</v>
       </c>
-      <c r="O12" s="133">
+      <c r="O12" s="131">
         <v>1</v>
       </c>
-      <c r="P12" s="72"/>
+      <c r="P12" s="70"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72" t="s">
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70" t="s">
         <v>209</v>
       </c>
-      <c r="F13" s="72" t="s">
+      <c r="F13" s="70" t="s">
         <v>211</v>
       </c>
-      <c r="G13" s="72"/>
-      <c r="M13" s="106">
+      <c r="G13" s="70"/>
+      <c r="M13" s="104">
         <v>10</v>
       </c>
-      <c r="N13" s="72" t="s">
+      <c r="N13" s="70" t="s">
         <v>101</v>
       </c>
-      <c r="O13" s="106">
-        <v>0</v>
-      </c>
-      <c r="P13" s="72"/>
+      <c r="O13" s="104">
+        <v>0</v>
+      </c>
+      <c r="P13" s="70"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72" t="s">
+      <c r="B14" s="70"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="70" t="s">
         <v>210</v>
       </c>
-      <c r="F14" s="72" t="s">
+      <c r="F14" s="70" t="s">
         <v>212</v>
       </c>
-      <c r="G14" s="72"/>
-      <c r="M14" s="106">
+      <c r="G14" s="70"/>
+      <c r="M14" s="104">
         <v>11</v>
       </c>
-      <c r="N14" s="72" t="s">
+      <c r="N14" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="O14" s="106">
-        <v>0</v>
-      </c>
-      <c r="P14" s="72"/>
+      <c r="O14" s="104">
+        <v>0</v>
+      </c>
+      <c r="P14" s="70"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="M15" s="106">
+      <c r="M15" s="104">
         <v>12</v>
       </c>
-      <c r="N15" s="72" t="s">
+      <c r="N15" s="70" t="s">
         <v>103</v>
       </c>
-      <c r="O15" s="106">
-        <v>0</v>
-      </c>
-      <c r="P15" s="72"/>
+      <c r="O15" s="104">
+        <v>0</v>
+      </c>
+      <c r="P15" s="70"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="M16" s="133">
+      <c r="M16" s="131">
         <v>13</v>
       </c>
-      <c r="N16" s="134" t="s">
+      <c r="N16" s="132" t="s">
         <v>104</v>
       </c>
-      <c r="O16" s="133">
+      <c r="O16" s="131">
         <v>1</v>
       </c>
-      <c r="P16" s="72"/>
+      <c r="P16" s="70"/>
     </row>
     <row r="17" spans="13:16" x14ac:dyDescent="0.3">
-      <c r="M17" s="106">
+      <c r="M17" s="104">
         <v>14</v>
       </c>
-      <c r="N17" s="72" t="s">
+      <c r="N17" s="70" t="s">
         <v>105</v>
       </c>
-      <c r="O17" s="106">
-        <v>0</v>
-      </c>
-      <c r="P17" s="72"/>
+      <c r="O17" s="104">
+        <v>0</v>
+      </c>
+      <c r="P17" s="70"/>
     </row>
     <row r="18" spans="13:16" x14ac:dyDescent="0.3">
-      <c r="M18" s="106">
+      <c r="M18" s="104">
         <v>15</v>
       </c>
-      <c r="N18" s="72" t="s">
+      <c r="N18" s="70" t="s">
         <v>106</v>
       </c>
-      <c r="O18" s="106">
-        <v>0</v>
-      </c>
-      <c r="P18" s="72"/>
+      <c r="O18" s="104">
+        <v>0</v>
+      </c>
+      <c r="P18" s="70"/>
     </row>
     <row r="19" spans="13:16" x14ac:dyDescent="0.3">
-      <c r="M19" s="106">
+      <c r="M19" s="104">
         <v>16</v>
       </c>
-      <c r="N19" s="72" t="s">
+      <c r="N19" s="70" t="s">
         <v>107</v>
       </c>
-      <c r="O19" s="106">
-        <v>0</v>
-      </c>
-      <c r="P19" s="72"/>
+      <c r="O19" s="104">
+        <v>0</v>
+      </c>
+      <c r="P19" s="70"/>
     </row>
     <row r="20" spans="13:16" x14ac:dyDescent="0.3">
-      <c r="M20" s="106">
+      <c r="M20" s="104">
         <v>17</v>
       </c>
-      <c r="N20" s="72" t="s">
+      <c r="N20" s="70" t="s">
         <v>108</v>
       </c>
-      <c r="O20" s="106">
-        <v>0</v>
-      </c>
-      <c r="P20" s="72"/>
+      <c r="O20" s="104">
+        <v>0</v>
+      </c>
+      <c r="P20" s="70"/>
     </row>
     <row r="21" spans="13:16" x14ac:dyDescent="0.3">
-      <c r="M21" s="106">
+      <c r="M21" s="104">
         <v>18</v>
       </c>
-      <c r="N21" s="72" t="s">
+      <c r="N21" s="70" t="s">
         <v>109</v>
       </c>
-      <c r="O21" s="106">
-        <v>0</v>
-      </c>
-      <c r="P21" s="72"/>
+      <c r="O21" s="104">
+        <v>0</v>
+      </c>
+      <c r="P21" s="70"/>
     </row>
     <row r="22" spans="13:16" x14ac:dyDescent="0.3">
-      <c r="M22" s="106">
+      <c r="M22" s="104">
         <v>19</v>
       </c>
-      <c r="N22" s="72" t="s">
+      <c r="N22" s="70" t="s">
         <v>110</v>
       </c>
-      <c r="O22" s="106">
-        <v>0</v>
-      </c>
-      <c r="P22" s="72"/>
+      <c r="O22" s="104">
+        <v>0</v>
+      </c>
+      <c r="P22" s="70"/>
     </row>
     <row r="23" spans="13:16" x14ac:dyDescent="0.3">
-      <c r="M23" s="106">
+      <c r="M23" s="104">
         <v>20</v>
       </c>
-      <c r="N23" s="72" t="s">
+      <c r="N23" s="70" t="s">
         <v>111</v>
       </c>
-      <c r="O23" s="106">
-        <v>0</v>
-      </c>
-      <c r="P23" s="72"/>
+      <c r="O23" s="104">
+        <v>0</v>
+      </c>
+      <c r="P23" s="70"/>
     </row>
     <row r="24" spans="13:16" x14ac:dyDescent="0.3">
-      <c r="M24" s="106">
+      <c r="M24" s="104">
         <v>21</v>
       </c>
-      <c r="N24" s="72" t="s">
+      <c r="N24" s="70" t="s">
         <v>112</v>
       </c>
-      <c r="O24" s="106">
-        <v>0</v>
-      </c>
-      <c r="P24" s="72"/>
+      <c r="O24" s="104">
+        <v>0</v>
+      </c>
+      <c r="P24" s="70"/>
     </row>
     <row r="25" spans="13:16" x14ac:dyDescent="0.3">
-      <c r="M25" s="106">
+      <c r="M25" s="104">
         <v>22</v>
       </c>
-      <c r="N25" s="72" t="s">
+      <c r="N25" s="70" t="s">
         <v>113</v>
       </c>
-      <c r="O25" s="106">
-        <v>0</v>
-      </c>
-      <c r="P25" s="72"/>
+      <c r="O25" s="104">
+        <v>0</v>
+      </c>
+      <c r="P25" s="70"/>
     </row>
     <row r="26" spans="13:16" x14ac:dyDescent="0.3">
-      <c r="M26" s="106">
+      <c r="M26" s="104">
         <v>23</v>
       </c>
-      <c r="N26" s="72" t="s">
+      <c r="N26" s="70" t="s">
         <v>114</v>
       </c>
-      <c r="O26" s="106">
-        <v>0</v>
-      </c>
-      <c r="P26" s="72"/>
+      <c r="O26" s="104">
+        <v>0</v>
+      </c>
+      <c r="P26" s="70"/>
     </row>
     <row r="27" spans="13:16" x14ac:dyDescent="0.3">
-      <c r="M27" s="106">
+      <c r="M27" s="104">
         <v>24</v>
       </c>
-      <c r="N27" s="72" t="s">
+      <c r="N27" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="O27" s="106">
-        <v>0</v>
-      </c>
-      <c r="P27" s="72"/>
+      <c r="O27" s="104">
+        <v>0</v>
+      </c>
+      <c r="P27" s="70"/>
     </row>
     <row r="28" spans="13:16" x14ac:dyDescent="0.3">
-      <c r="M28" s="106">
+      <c r="M28" s="104">
         <v>25</v>
       </c>
-      <c r="N28" s="72" t="s">
+      <c r="N28" s="70" t="s">
         <v>116</v>
       </c>
-      <c r="O28" s="106">
-        <v>0</v>
-      </c>
-      <c r="P28" s="72"/>
+      <c r="O28" s="104">
+        <v>0</v>
+      </c>
+      <c r="P28" s="70"/>
     </row>
     <row r="29" spans="13:16" x14ac:dyDescent="0.3">
-      <c r="M29" s="106">
+      <c r="M29" s="104">
         <v>26</v>
       </c>
-      <c r="N29" s="72" t="s">
+      <c r="N29" s="70" t="s">
         <v>117</v>
       </c>
-      <c r="O29" s="106">
-        <v>0</v>
-      </c>
-      <c r="P29" s="72"/>
+      <c r="O29" s="104">
+        <v>0</v>
+      </c>
+      <c r="P29" s="70"/>
     </row>
     <row r="30" spans="13:16" x14ac:dyDescent="0.3">
-      <c r="M30" s="106"/>
-      <c r="N30" s="72"/>
-      <c r="O30" s="106"/>
-      <c r="P30" s="72"/>
+      <c r="M30" s="104"/>
+      <c r="N30" s="70"/>
+      <c r="O30" s="104"/>
+      <c r="P30" s="70"/>
     </row>
     <row r="31" spans="13:16" x14ac:dyDescent="0.3">
-      <c r="M31" s="106"/>
-      <c r="N31" s="74" t="s">
+      <c r="M31" s="104"/>
+      <c r="N31" s="72" t="s">
         <v>198</v>
       </c>
-      <c r="O31" s="135">
+      <c r="O31" s="133">
         <f>SUM(O4:O29)</f>
         <v>2</v>
       </c>
-      <c r="P31" s="72"/>
+      <c r="P31" s="70"/>
     </row>
     <row r="32" spans="13:16" x14ac:dyDescent="0.3">
-      <c r="M32" s="106"/>
-      <c r="N32" s="74" t="s">
+      <c r="M32" s="104"/>
+      <c r="N32" s="72" t="s">
         <v>182</v>
       </c>
-      <c r="O32" s="135">
+      <c r="O32" s="133">
         <f>COUNT(O4:O29)</f>
         <v>26</v>
       </c>
-      <c r="P32" s="72"/>
+      <c r="P32" s="70"/>
     </row>
     <row r="33" spans="13:16" x14ac:dyDescent="0.3">
-      <c r="M33" s="106"/>
-      <c r="N33" s="74" t="s">
+      <c r="M33" s="104"/>
+      <c r="N33" s="72" t="s">
         <v>208</v>
       </c>
-      <c r="O33" s="135">
+      <c r="O33" s="133">
         <f>ROUND((O31/O32)*100,2)</f>
         <v>7.69</v>
       </c>
-      <c r="P33" s="72"/>
+      <c r="P33" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4682,50 +4731,50 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="136" t="s">
         <v>186</v>
       </c>
-      <c r="C2" s="139"/>
-      <c r="D2" s="139"/>
-      <c r="E2" s="139"/>
-      <c r="F2" s="139"/>
-      <c r="G2" s="140"/>
-      <c r="M2" s="135" t="s">
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
+      <c r="G2" s="138"/>
+      <c r="M2" s="133" t="s">
         <v>177</v>
       </c>
-      <c r="N2" s="74" t="s">
+      <c r="N2" s="72" t="s">
         <v>180</v>
       </c>
-      <c r="O2" s="135" t="s">
+      <c r="O2" s="133" t="s">
         <v>197</v>
       </c>
-      <c r="P2" s="74" t="s">
+      <c r="P2" s="72" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="141"/>
-      <c r="C3" s="142"/>
-      <c r="D3" s="142"/>
-      <c r="E3" s="142"/>
-      <c r="F3" s="142"/>
-      <c r="G3" s="142"/>
-      <c r="H3" s="148" t="s">
+      <c r="B3" s="139"/>
+      <c r="C3" s="140"/>
+      <c r="D3" s="140"/>
+      <c r="E3" s="140"/>
+      <c r="F3" s="140"/>
+      <c r="G3" s="140"/>
+      <c r="H3" s="146" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="149"/>
-      <c r="J3" s="149"/>
-      <c r="K3" s="150"/>
-      <c r="M3" s="106"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="106"/>
-      <c r="P3" s="72"/>
+      <c r="I3" s="147"/>
+      <c r="J3" s="147"/>
+      <c r="K3" s="148"/>
+      <c r="M3" s="104"/>
+      <c r="N3" s="70"/>
+      <c r="O3" s="104"/>
+      <c r="P3" s="70"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="144" t="s">
+      <c r="B4" s="142" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="146" t="s">
+      <c r="C4" s="144" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="39">
@@ -4742,27 +4791,27 @@
       <c r="I4" s="62"/>
       <c r="J4" s="62"/>
       <c r="K4" s="63"/>
-      <c r="M4" s="106">
+      <c r="M4" s="104">
         <v>1</v>
       </c>
-      <c r="N4" s="72" t="s">
+      <c r="N4" s="70" t="s">
         <v>199</v>
       </c>
-      <c r="O4" s="106">
-        <v>0</v>
-      </c>
-      <c r="P4" s="72"/>
+      <c r="O4" s="104">
+        <v>0</v>
+      </c>
+      <c r="P4" s="70"/>
     </row>
     <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="145"/>
-      <c r="C5" s="147"/>
+      <c r="B5" s="143"/>
+      <c r="C5" s="145"/>
       <c r="D5" s="41" t="s">
         <v>49</v>
       </c>
       <c r="E5" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="75" t="s">
+      <c r="F5" s="73" t="s">
         <v>47</v>
       </c>
       <c r="G5" s="52"/>
@@ -4770,16 +4819,16 @@
       <c r="I5" s="65"/>
       <c r="J5" s="65"/>
       <c r="K5" s="66"/>
-      <c r="M5" s="133">
+      <c r="M5" s="131">
         <v>2</v>
       </c>
-      <c r="N5" s="134" t="s">
+      <c r="N5" s="132" t="s">
         <v>200</v>
       </c>
-      <c r="O5" s="133">
+      <c r="O5" s="131">
         <v>1</v>
       </c>
-      <c r="P5" s="72"/>
+      <c r="P5" s="70"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="32">
@@ -4802,16 +4851,16 @@
       <c r="I6" s="59"/>
       <c r="J6" s="59"/>
       <c r="K6" s="60"/>
-      <c r="M6" s="106">
+      <c r="M6" s="104">
         <v>3</v>
       </c>
-      <c r="N6" s="72" t="s">
+      <c r="N6" s="70" t="s">
         <v>201</v>
       </c>
-      <c r="O6" s="106">
-        <v>0</v>
-      </c>
-      <c r="P6" s="72"/>
+      <c r="O6" s="104">
+        <v>0</v>
+      </c>
+      <c r="P6" s="70"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="34">
@@ -4826,16 +4875,16 @@
       <c r="I7" s="45"/>
       <c r="J7" s="45"/>
       <c r="K7" s="46"/>
-      <c r="M7" s="133">
+      <c r="M7" s="131">
         <v>4</v>
       </c>
-      <c r="N7" s="134" t="s">
+      <c r="N7" s="132" t="s">
         <v>202</v>
       </c>
-      <c r="O7" s="133">
+      <c r="O7" s="131">
         <v>1</v>
       </c>
-      <c r="P7" s="72"/>
+      <c r="P7" s="70"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="34">
@@ -4850,16 +4899,16 @@
       <c r="I8" s="45"/>
       <c r="J8" s="45"/>
       <c r="K8" s="46"/>
-      <c r="M8" s="106">
+      <c r="M8" s="104">
         <v>5</v>
       </c>
-      <c r="N8" s="72" t="s">
+      <c r="N8" s="70" t="s">
         <v>203</v>
       </c>
-      <c r="O8" s="106">
-        <v>0</v>
-      </c>
-      <c r="P8" s="72"/>
+      <c r="O8" s="104">
+        <v>0</v>
+      </c>
+      <c r="P8" s="70"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" s="34">
@@ -4874,16 +4923,16 @@
       <c r="I9" s="45"/>
       <c r="J9" s="45"/>
       <c r="K9" s="46"/>
-      <c r="M9" s="106">
+      <c r="M9" s="104">
         <v>6</v>
       </c>
-      <c r="N9" s="72" t="s">
+      <c r="N9" s="70" t="s">
         <v>204</v>
       </c>
-      <c r="O9" s="106">
-        <v>0</v>
-      </c>
-      <c r="P9" s="72"/>
+      <c r="O9" s="104">
+        <v>0</v>
+      </c>
+      <c r="P9" s="70"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" s="34">
@@ -4898,16 +4947,16 @@
       <c r="I10" s="45"/>
       <c r="J10" s="45"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="106">
+      <c r="M10" s="104">
         <v>7</v>
       </c>
-      <c r="N10" s="72" t="s">
+      <c r="N10" s="70" t="s">
         <v>205</v>
       </c>
-      <c r="O10" s="106">
-        <v>0</v>
-      </c>
-      <c r="P10" s="72"/>
+      <c r="O10" s="104">
+        <v>0</v>
+      </c>
+      <c r="P10" s="70"/>
     </row>
     <row r="11" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="36">
@@ -4922,93 +4971,93 @@
       <c r="I11" s="48"/>
       <c r="J11" s="48"/>
       <c r="K11" s="49"/>
-      <c r="M11" s="106">
+      <c r="M11" s="104">
         <v>8</v>
       </c>
-      <c r="N11" s="72" t="s">
+      <c r="N11" s="70" t="s">
         <v>206</v>
       </c>
-      <c r="O11" s="106">
-        <v>0</v>
-      </c>
-      <c r="P11" s="72"/>
+      <c r="O11" s="104">
+        <v>0</v>
+      </c>
+      <c r="P11" s="70"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B12" s="151" t="s">
+      <c r="B12" s="149" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="152"/>
-      <c r="D12" s="136" t="s">
+      <c r="C12" s="150"/>
+      <c r="D12" s="134" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="72" t="s">
+      <c r="E12" s="70" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="72" t="s">
+      <c r="F12" s="70" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="137"/>
-      <c r="M12" s="106"/>
-      <c r="N12" s="72"/>
-      <c r="O12" s="106"/>
-      <c r="P12" s="72"/>
+      <c r="G12" s="135"/>
+      <c r="M12" s="104"/>
+      <c r="N12" s="70"/>
+      <c r="O12" s="104"/>
+      <c r="P12" s="70"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72" t="s">
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70" t="s">
         <v>209</v>
       </c>
-      <c r="F13" s="72" t="s">
+      <c r="F13" s="70" t="s">
         <v>211</v>
       </c>
-      <c r="G13" s="72"/>
-      <c r="M13" s="106"/>
-      <c r="N13" s="74" t="s">
+      <c r="G13" s="70"/>
+      <c r="M13" s="104"/>
+      <c r="N13" s="72" t="s">
         <v>198</v>
       </c>
-      <c r="O13" s="135">
+      <c r="O13" s="133">
         <f>SUM(O4:O11)</f>
         <v>2</v>
       </c>
-      <c r="P13" s="72"/>
+      <c r="P13" s="70"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72" t="s">
+      <c r="B14" s="70"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="70" t="s">
         <v>210</v>
       </c>
-      <c r="F14" s="72" t="s">
+      <c r="F14" s="70" t="s">
         <v>212</v>
       </c>
-      <c r="G14" s="72"/>
-      <c r="M14" s="106"/>
-      <c r="N14" s="74" t="s">
+      <c r="G14" s="70"/>
+      <c r="M14" s="104"/>
+      <c r="N14" s="72" t="s">
         <v>182</v>
       </c>
-      <c r="O14" s="135">
+      <c r="O14" s="133">
         <f>COUNT(O4:O11)</f>
         <v>8</v>
       </c>
-      <c r="P14" s="72"/>
+      <c r="P14" s="70"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="M15" s="106"/>
-      <c r="N15" s="74" t="s">
+      <c r="M15" s="104"/>
+      <c r="N15" s="72" t="s">
         <v>207</v>
       </c>
-      <c r="O15" s="135">
+      <c r="O15" s="133">
         <f>ROUND((O13/O14)*100,2)</f>
         <v>25</v>
       </c>
-      <c r="P15" s="72"/>
+      <c r="P15" s="70"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="M16" s="105"/>
-      <c r="O16" s="105"/>
+      <c r="M16" s="103"/>
+      <c r="O16" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -5025,10 +5074,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DABE7A-7845-46EA-BB0E-44CB73A3B0F1}">
-  <dimension ref="B1:L24"/>
+  <dimension ref="B1:Q24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5039,41 +5088,60 @@
     <col min="5" max="5" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="138" t="s">
+    <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="136" t="s">
         <v>185</v>
       </c>
-      <c r="C2" s="139"/>
-      <c r="D2" s="139"/>
-      <c r="E2" s="139"/>
-      <c r="F2" s="139"/>
-      <c r="G2" s="139"/>
-      <c r="H2" s="140"/>
-    </row>
-    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="141"/>
-      <c r="C3" s="142"/>
-      <c r="D3" s="142"/>
-      <c r="E3" s="142"/>
-      <c r="F3" s="142"/>
-      <c r="G3" s="142"/>
-      <c r="H3" s="142"/>
-      <c r="I3" s="148" t="s">
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
+      <c r="G2" s="137"/>
+      <c r="H2" s="138"/>
+      <c r="N2" s="106" t="s">
+        <v>177</v>
+      </c>
+      <c r="O2" s="105" t="s">
+        <v>180</v>
+      </c>
+      <c r="P2" s="106" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q2" s="105" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="139"/>
+      <c r="C3" s="140"/>
+      <c r="D3" s="140"/>
+      <c r="E3" s="140"/>
+      <c r="F3" s="140"/>
+      <c r="G3" s="140"/>
+      <c r="H3" s="140"/>
+      <c r="I3" s="146" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="149"/>
-      <c r="K3" s="149"/>
-      <c r="L3" s="150"/>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="144" t="s">
+      <c r="J3" s="147"/>
+      <c r="K3" s="147"/>
+      <c r="L3" s="148"/>
+      <c r="N3" s="104"/>
+      <c r="O3" s="70"/>
+      <c r="P3" s="104"/>
+      <c r="Q3" s="70"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B4" s="142" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="146" t="s">
+      <c r="C4" s="144" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="39">
@@ -5088,15 +5156,27 @@
       <c r="G4" s="40">
         <v>45248</v>
       </c>
-      <c r="H4" s="40"/>
+      <c r="H4" s="40">
+        <v>45249</v>
+      </c>
       <c r="I4" s="61"/>
       <c r="J4" s="62"/>
       <c r="K4" s="62"/>
       <c r="L4" s="63"/>
-    </row>
-    <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="145"/>
-      <c r="C5" s="147"/>
+      <c r="N4" s="104">
+        <v>1</v>
+      </c>
+      <c r="O4" s="70" t="s">
+        <v>226</v>
+      </c>
+      <c r="P4" s="104">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="70"/>
+    </row>
+    <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="143"/>
+      <c r="C5" s="145"/>
       <c r="D5" s="67" t="s">
         <v>53</v>
       </c>
@@ -5109,13 +5189,25 @@
       <c r="G5" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="H5" s="68"/>
+      <c r="H5" s="67" t="s">
+        <v>53</v>
+      </c>
       <c r="I5" s="64"/>
       <c r="J5" s="65"/>
       <c r="K5" s="65"/>
       <c r="L5" s="66"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="N5" s="104">
+        <v>2</v>
+      </c>
+      <c r="O5" s="70" t="s">
+        <v>227</v>
+      </c>
+      <c r="P5" s="104">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="70"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="32">
         <v>1</v>
       </c>
@@ -5134,13 +5226,25 @@
       <c r="G6" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="53"/>
+      <c r="H6" s="42" t="s">
+        <v>48</v>
+      </c>
       <c r="I6" s="58"/>
       <c r="J6" s="59"/>
       <c r="K6" s="59"/>
       <c r="L6" s="60"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="N6" s="104">
+        <v>3</v>
+      </c>
+      <c r="O6" s="70" t="s">
+        <v>228</v>
+      </c>
+      <c r="P6" s="104">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="70"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="34">
         <v>2</v>
       </c>
@@ -5154,8 +5258,18 @@
       <c r="J7" s="45"/>
       <c r="K7" s="45"/>
       <c r="L7" s="46"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="N7" s="104">
+        <v>4</v>
+      </c>
+      <c r="O7" s="70" t="s">
+        <v>229</v>
+      </c>
+      <c r="P7" s="104">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="70"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="34">
         <v>3</v>
       </c>
@@ -5169,8 +5283,18 @@
       <c r="J8" s="45"/>
       <c r="K8" s="45"/>
       <c r="L8" s="46"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="N8" s="104">
+        <v>5</v>
+      </c>
+      <c r="O8" s="70" t="s">
+        <v>230</v>
+      </c>
+      <c r="P8" s="104">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="70"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" s="34">
         <v>4</v>
       </c>
@@ -5184,8 +5308,18 @@
       <c r="J9" s="45"/>
       <c r="K9" s="45"/>
       <c r="L9" s="46"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="N9" s="104">
+        <v>6</v>
+      </c>
+      <c r="O9" s="70" t="s">
+        <v>231</v>
+      </c>
+      <c r="P9" s="104">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="70"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="34">
         <v>5</v>
       </c>
@@ -5199,8 +5333,18 @@
       <c r="J10" s="45"/>
       <c r="K10" s="45"/>
       <c r="L10" s="46"/>
-    </row>
-    <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N10" s="104">
+        <v>7</v>
+      </c>
+      <c r="O10" s="70" t="s">
+        <v>232</v>
+      </c>
+      <c r="P10" s="104">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="70"/>
+    </row>
+    <row r="11" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="36">
         <v>6</v>
       </c>
@@ -5209,17 +5353,27 @@
       <c r="E11" s="48"/>
       <c r="F11" s="48"/>
       <c r="G11" s="55"/>
-      <c r="H11" s="73"/>
+      <c r="H11" s="71"/>
       <c r="I11" s="57"/>
       <c r="J11" s="48"/>
       <c r="K11" s="48"/>
       <c r="L11" s="49"/>
-    </row>
-    <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="153" t="s">
+      <c r="N11" s="104">
+        <v>8</v>
+      </c>
+      <c r="O11" s="70" t="s">
+        <v>233</v>
+      </c>
+      <c r="P11" s="104">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="70"/>
+    </row>
+    <row r="12" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="151" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="154"/>
+      <c r="C12" s="152"/>
       <c r="D12" s="38"/>
       <c r="E12" s="31" t="s">
         <v>152</v>
@@ -5227,17 +5381,132 @@
       <c r="F12" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="G12" s="69" t="s">
+      <c r="G12" s="68" t="s">
         <v>213</v>
       </c>
-      <c r="H12" s="74"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H12" s="153" t="s">
+        <v>225</v>
+      </c>
+      <c r="N12" s="104">
+        <v>9</v>
+      </c>
+      <c r="O12" s="70" t="s">
+        <v>234</v>
+      </c>
+      <c r="P12" s="104">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="70"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="G13" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="24" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="N13" s="154">
+        <v>10</v>
+      </c>
+      <c r="O13" s="155" t="s">
+        <v>235</v>
+      </c>
+      <c r="P13" s="154">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="70"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="N14" s="154">
+        <v>11</v>
+      </c>
+      <c r="O14" s="155" t="s">
+        <v>102</v>
+      </c>
+      <c r="P14" s="154">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="70"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="N15" s="154">
+        <v>12</v>
+      </c>
+      <c r="O15" s="155" t="s">
+        <v>237</v>
+      </c>
+      <c r="P15" s="154">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="70"/>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="N16" s="154">
+        <v>13</v>
+      </c>
+      <c r="O16" s="155" t="s">
+        <v>236</v>
+      </c>
+      <c r="P16" s="154">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="70"/>
+    </row>
+    <row r="17" spans="11:17" x14ac:dyDescent="0.3">
+      <c r="N17" s="154">
+        <v>14</v>
+      </c>
+      <c r="O17" s="155" t="s">
+        <v>238</v>
+      </c>
+      <c r="P17" s="154">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="70"/>
+    </row>
+    <row r="18" spans="11:17" x14ac:dyDescent="0.3">
+      <c r="N18" s="154">
+        <v>15</v>
+      </c>
+      <c r="O18" s="155" t="s">
+        <v>239</v>
+      </c>
+      <c r="P18" s="154">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="70"/>
+    </row>
+    <row r="21" spans="11:17" x14ac:dyDescent="0.3">
+      <c r="N21" s="104"/>
+      <c r="O21" s="72" t="s">
+        <v>198</v>
+      </c>
+      <c r="P21" s="133">
+        <f>SUM(P4:P15)</f>
+        <v>5</v>
+      </c>
+      <c r="Q21" s="70"/>
+    </row>
+    <row r="22" spans="11:17" x14ac:dyDescent="0.3">
+      <c r="N22" s="104"/>
+      <c r="O22" s="72" t="s">
+        <v>182</v>
+      </c>
+      <c r="P22" s="133">
+        <f>COUNT(P4:P18)</f>
+        <v>15</v>
+      </c>
+      <c r="Q22" s="70"/>
+    </row>
+    <row r="23" spans="11:17" x14ac:dyDescent="0.3">
+      <c r="N23" s="104"/>
+      <c r="O23" s="72" t="s">
+        <v>207</v>
+      </c>
+      <c r="P23" s="133">
+        <f>ROUND((P21/P22)*100,2)</f>
+        <v>33.33</v>
+      </c>
+      <c r="Q23" s="70"/>
+    </row>
+    <row r="24" spans="11:17" x14ac:dyDescent="0.3">
       <c r="K24" t="s">
         <v>46</v>
       </c>
@@ -5257,10 +5526,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0268C353-496F-4BD6-A7EF-D042619A03C3}">
-  <dimension ref="B1:Q23"/>
+  <dimension ref="B1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21:Q23"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5271,7 +5540,7 @@
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.88671875" customWidth="1"/>
     <col min="7" max="7" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
@@ -5282,52 +5551,52 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="136" t="s">
         <v>184</v>
       </c>
-      <c r="C2" s="139"/>
-      <c r="D2" s="139"/>
-      <c r="E2" s="139"/>
-      <c r="F2" s="139"/>
-      <c r="G2" s="139"/>
-      <c r="H2" s="140"/>
-      <c r="N2" s="135" t="s">
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
+      <c r="G2" s="137"/>
+      <c r="H2" s="138"/>
+      <c r="N2" s="106" t="s">
         <v>177</v>
       </c>
-      <c r="O2" s="74" t="s">
+      <c r="O2" s="105" t="s">
         <v>180</v>
       </c>
-      <c r="P2" s="135" t="s">
+      <c r="P2" s="106" t="s">
         <v>197</v>
       </c>
-      <c r="Q2" s="74" t="s">
+      <c r="Q2" s="105" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="141"/>
-      <c r="C3" s="142"/>
-      <c r="D3" s="142"/>
-      <c r="E3" s="142"/>
-      <c r="F3" s="142"/>
-      <c r="G3" s="142"/>
-      <c r="H3" s="142"/>
-      <c r="I3" s="148" t="s">
+      <c r="B3" s="139"/>
+      <c r="C3" s="140"/>
+      <c r="D3" s="140"/>
+      <c r="E3" s="140"/>
+      <c r="F3" s="140"/>
+      <c r="G3" s="140"/>
+      <c r="H3" s="140"/>
+      <c r="I3" s="146" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="149"/>
-      <c r="K3" s="149"/>
-      <c r="L3" s="150"/>
-      <c r="N3" s="106"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="106"/>
-      <c r="Q3" s="72"/>
+      <c r="J3" s="147"/>
+      <c r="K3" s="147"/>
+      <c r="L3" s="148"/>
+      <c r="N3" s="104"/>
+      <c r="O3" s="70"/>
+      <c r="P3" s="104"/>
+      <c r="Q3" s="70"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="144" t="s">
+      <c r="B4" s="142" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="146" t="s">
+      <c r="C4" s="144" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="39">
@@ -5342,33 +5611,35 @@
       <c r="G4" s="40">
         <v>45248</v>
       </c>
-      <c r="H4" s="40"/>
+      <c r="H4" s="40">
+        <v>45249</v>
+      </c>
       <c r="I4" s="39">
         <v>45241</v>
       </c>
-      <c r="J4" s="125" t="s">
+      <c r="J4" s="123" t="s">
         <v>158</v>
       </c>
-      <c r="K4" s="125" t="s">
+      <c r="K4" s="123" t="s">
         <v>159</v>
       </c>
-      <c r="L4" s="126" t="s">
+      <c r="L4" s="124" t="s">
         <v>160</v>
       </c>
-      <c r="N4" s="106">
+      <c r="N4" s="104">
         <v>1</v>
       </c>
-      <c r="O4" s="72" t="s">
+      <c r="O4" s="70" t="s">
         <v>217</v>
       </c>
-      <c r="P4" s="106">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="72"/>
+      <c r="P4" s="104">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="70"/>
     </row>
     <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="145"/>
-      <c r="C5" s="147"/>
+      <c r="B5" s="143"/>
+      <c r="C5" s="145"/>
       <c r="D5" s="67" t="s">
         <v>52</v>
       </c>
@@ -5381,23 +5652,25 @@
       <c r="G5" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="71"/>
+      <c r="H5" s="67" t="s">
+        <v>52</v>
+      </c>
       <c r="I5" s="67" t="s">
         <v>52</v>
       </c>
       <c r="J5" s="65"/>
       <c r="K5" s="65"/>
       <c r="L5" s="66"/>
-      <c r="N5" s="155">
+      <c r="N5" s="104">
         <v>2</v>
       </c>
-      <c r="O5" s="72" t="s">
+      <c r="O5" s="70" t="s">
         <v>218</v>
       </c>
-      <c r="P5" s="155">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="72"/>
+      <c r="P5" s="104">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="70"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="32">
@@ -5418,8 +5691,10 @@
       <c r="G6" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="45"/>
-      <c r="I6" s="70"/>
+      <c r="H6" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="69"/>
       <c r="J6" s="59">
         <v>48</v>
       </c>
@@ -5430,16 +5705,16 @@
         <f>(K6/J6)*100</f>
         <v>18.75</v>
       </c>
-      <c r="N6" s="155">
+      <c r="N6" s="104">
         <v>3</v>
       </c>
-      <c r="O6" s="156" t="s">
+      <c r="O6" s="70" t="s">
         <v>219</v>
       </c>
-      <c r="P6" s="155">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="72"/>
+      <c r="P6" s="104">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="70"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="34">
@@ -5450,21 +5725,21 @@
       <c r="E7" s="45"/>
       <c r="F7" s="45"/>
       <c r="G7" s="54"/>
-      <c r="H7" s="72"/>
+      <c r="H7" s="70"/>
       <c r="I7" s="44"/>
       <c r="J7" s="45"/>
       <c r="K7" s="45"/>
       <c r="L7" s="46"/>
-      <c r="N7" s="155">
+      <c r="N7" s="104">
         <v>4</v>
       </c>
-      <c r="O7" s="156" t="s">
+      <c r="O7" s="70" t="s">
         <v>220</v>
       </c>
-      <c r="P7" s="155">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="72"/>
+      <c r="P7" s="104">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="70"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="34">
@@ -5475,21 +5750,21 @@
       <c r="E8" s="45"/>
       <c r="F8" s="45"/>
       <c r="G8" s="54"/>
-      <c r="H8" s="72"/>
+      <c r="H8" s="70"/>
       <c r="I8" s="44"/>
       <c r="J8" s="45"/>
       <c r="K8" s="45"/>
       <c r="L8" s="46"/>
-      <c r="N8" s="106">
+      <c r="N8" s="104">
         <v>5</v>
       </c>
-      <c r="O8" s="72" t="s">
+      <c r="O8" s="70" t="s">
         <v>221</v>
       </c>
-      <c r="P8" s="106">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="72"/>
+      <c r="P8" s="104">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="70"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" s="34">
@@ -5500,21 +5775,21 @@
       <c r="E9" s="45"/>
       <c r="F9" s="45"/>
       <c r="G9" s="54"/>
-      <c r="H9" s="72"/>
+      <c r="H9" s="70"/>
       <c r="I9" s="44"/>
       <c r="J9" s="45"/>
       <c r="K9" s="45"/>
       <c r="L9" s="46"/>
-      <c r="N9" s="106">
+      <c r="N9" s="104">
         <v>6</v>
       </c>
-      <c r="O9" s="72" t="s">
+      <c r="O9" s="70" t="s">
         <v>222</v>
       </c>
-      <c r="P9" s="106">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="72"/>
+      <c r="P9" s="104">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="70"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="34">
@@ -5525,21 +5800,21 @@
       <c r="E10" s="45"/>
       <c r="F10" s="45"/>
       <c r="G10" s="54"/>
-      <c r="H10" s="72"/>
+      <c r="H10" s="70"/>
       <c r="I10" s="44"/>
       <c r="J10" s="45"/>
       <c r="K10" s="45"/>
       <c r="L10" s="46"/>
-      <c r="N10" s="106">
+      <c r="N10" s="104">
         <v>7</v>
       </c>
-      <c r="O10" s="72" t="s">
+      <c r="O10" s="70" t="s">
         <v>223</v>
       </c>
-      <c r="P10" s="106">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="72"/>
+      <c r="P10" s="104">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="70"/>
     </row>
     <row r="11" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="36">
@@ -5550,27 +5825,27 @@
       <c r="E11" s="48"/>
       <c r="F11" s="48"/>
       <c r="G11" s="55"/>
-      <c r="H11" s="72"/>
+      <c r="H11" s="70"/>
       <c r="I11" s="47"/>
       <c r="J11" s="48"/>
       <c r="K11" s="48"/>
       <c r="L11" s="49"/>
-      <c r="N11" s="106">
+      <c r="N11" s="104">
         <v>8</v>
       </c>
-      <c r="O11" s="72" t="s">
+      <c r="O11" s="70" t="s">
         <v>224</v>
       </c>
-      <c r="P11" s="106">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="72"/>
+      <c r="P11" s="104">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="70"/>
     </row>
     <row r="12" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="153" t="s">
+      <c r="B12" s="151" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="154"/>
+      <c r="C12" s="152"/>
       <c r="D12" s="38"/>
       <c r="E12" s="31" t="s">
         <v>154</v>
@@ -5578,17 +5853,25 @@
       <c r="F12" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="G12" s="69" t="s">
+      <c r="G12" s="68" t="s">
         <v>215</v>
       </c>
-      <c r="H12" s="72"/>
+      <c r="H12" s="70" t="s">
+        <v>215</v>
+      </c>
       <c r="J12" t="s">
         <v>188</v>
       </c>
-      <c r="N12" s="106"/>
-      <c r="O12" s="72"/>
-      <c r="P12" s="106"/>
-      <c r="Q12" s="72"/>
+      <c r="N12" s="104">
+        <v>9</v>
+      </c>
+      <c r="O12" s="70" t="s">
+        <v>240</v>
+      </c>
+      <c r="P12" s="104">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="70"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
@@ -5600,6 +5883,16 @@
       <c r="J13" t="s">
         <v>189</v>
       </c>
+      <c r="N13" s="154">
+        <v>10</v>
+      </c>
+      <c r="O13" s="155" t="s">
+        <v>241</v>
+      </c>
+      <c r="P13" s="104">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="70"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="F14" t="s">
@@ -5608,44 +5901,54 @@
       <c r="J14" t="s">
         <v>190</v>
       </c>
+      <c r="N14" s="154">
+        <v>11</v>
+      </c>
+      <c r="O14" s="155" t="s">
+        <v>242</v>
+      </c>
+      <c r="P14" s="104">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="70"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="J15" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="21" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N21" s="106"/>
-      <c r="O21" s="74" t="s">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="N16" s="104"/>
+      <c r="O16" s="72" t="s">
         <v>198</v>
       </c>
-      <c r="P21" s="135">
-        <f>SUM(P4:P11)</f>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="72"/>
-    </row>
-    <row r="22" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N22" s="106"/>
-      <c r="O22" s="74" t="s">
+      <c r="P16" s="133">
+        <f>SUM(P4:P14)</f>
+        <v>3</v>
+      </c>
+      <c r="Q16" s="70"/>
+    </row>
+    <row r="17" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="N17" s="104"/>
+      <c r="O17" s="72" t="s">
         <v>182</v>
       </c>
-      <c r="P22" s="135">
-        <f>COUNT(P4:P11)</f>
-        <v>8</v>
-      </c>
-      <c r="Q22" s="72"/>
-    </row>
-    <row r="23" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N23" s="106"/>
-      <c r="O23" s="74" t="s">
+      <c r="P17" s="133">
+        <f>COUNT(P4:P14)</f>
+        <v>11</v>
+      </c>
+      <c r="Q17" s="70"/>
+    </row>
+    <row r="18" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="N18" s="104"/>
+      <c r="O18" s="72" t="s">
         <v>207</v>
       </c>
-      <c r="P23" s="135">
-        <f>ROUND((P21/P22)*100,2)</f>
-        <v>0</v>
-      </c>
-      <c r="Q23" s="72"/>
+      <c r="P18" s="133">
+        <f>ROUND((P16/P17)*100,2)</f>
+        <v>27.27</v>
+      </c>
+      <c r="Q18" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
OPS of Physics & Maths
OPS of Physics & Maths
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/Ops-2023-11.xlsx
+++ b/Offline/BusinessManagement/Ops/Ops-2023-11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Ops\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B27A86E-8F7F-46CF-AE5D-7B32379EF909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F5EE52-5DFE-4F4D-9D81-3324D3D2B1F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="257">
   <si>
     <t>Course</t>
   </si>
@@ -902,6 +902,18 @@
   </si>
   <si>
     <t>Test Date</t>
+  </si>
+  <si>
+    <t>1) Elasticity MCQ</t>
+  </si>
+  <si>
+    <t>Started</t>
+  </si>
+  <si>
+    <t>1) Co-ordiante Geometry</t>
+  </si>
+  <si>
+    <t>Straight Line</t>
   </si>
 </sst>
 </file>
@@ -1091,7 +1103,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="47">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -1691,11 +1703,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1963,70 +2015,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2039,9 +2031,6 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2049,6 +2038,89 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="6" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2061,41 +2133,36 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="6" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2541,14 +2608,14 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="137" t="s">
+      <c r="B2" s="159" t="s">
         <v>183</v>
       </c>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138"/>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="139"/>
+      <c r="C2" s="160"/>
+      <c r="D2" s="160"/>
+      <c r="E2" s="160"/>
+      <c r="F2" s="160"/>
+      <c r="G2" s="161"/>
       <c r="M2" s="98" t="s">
         <v>179</v>
       </c>
@@ -2566,18 +2633,18 @@
       </c>
     </row>
     <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="140"/>
-      <c r="C3" s="141"/>
-      <c r="D3" s="141"/>
-      <c r="E3" s="141"/>
-      <c r="F3" s="141"/>
-      <c r="G3" s="141"/>
-      <c r="H3" s="147" t="s">
+      <c r="B3" s="162"/>
+      <c r="C3" s="163"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="163"/>
+      <c r="F3" s="163"/>
+      <c r="G3" s="163"/>
+      <c r="H3" s="169" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="148"/>
-      <c r="J3" s="148"/>
-      <c r="K3" s="149"/>
+      <c r="I3" s="170"/>
+      <c r="J3" s="170"/>
+      <c r="K3" s="171"/>
       <c r="M3" s="63"/>
       <c r="N3" s="97"/>
       <c r="O3" s="63"/>
@@ -2585,10 +2652,10 @@
       <c r="Q3" s="63"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="143" t="s">
+      <c r="B4" s="165" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="145" t="s">
+      <c r="C4" s="167" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="37">
@@ -2620,8 +2687,8 @@
       <c r="Q4" s="63"/>
     </row>
     <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="144"/>
-      <c r="C5" s="146"/>
+      <c r="B5" s="166"/>
+      <c r="C5" s="168"/>
       <c r="D5" s="66" t="s">
         <v>51</v>
       </c>
@@ -2807,10 +2874,10 @@
       <c r="Q11" s="63"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="142" t="s">
+      <c r="B12" s="164" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="142"/>
+      <c r="C12" s="164"/>
       <c r="D12" s="95" t="s">
         <v>161</v>
       </c>
@@ -4299,14 +4366,14 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="137" t="s">
+      <c r="B2" s="159" t="s">
         <v>187</v>
       </c>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138"/>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="139"/>
+      <c r="C2" s="160"/>
+      <c r="D2" s="160"/>
+      <c r="E2" s="160"/>
+      <c r="F2" s="160"/>
+      <c r="G2" s="161"/>
       <c r="M2" s="126" t="s">
         <v>177</v>
       </c>
@@ -4321,28 +4388,28 @@
       </c>
     </row>
     <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="140"/>
-      <c r="C3" s="141"/>
-      <c r="D3" s="141"/>
-      <c r="E3" s="141"/>
-      <c r="F3" s="141"/>
-      <c r="G3" s="141"/>
-      <c r="H3" s="147" t="s">
+      <c r="B3" s="162"/>
+      <c r="C3" s="163"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="163"/>
+      <c r="F3" s="163"/>
+      <c r="G3" s="163"/>
+      <c r="H3" s="169" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="148"/>
-      <c r="J3" s="148"/>
-      <c r="K3" s="149"/>
+      <c r="I3" s="170"/>
+      <c r="J3" s="170"/>
+      <c r="K3" s="171"/>
       <c r="M3" s="97"/>
       <c r="N3" s="63"/>
       <c r="O3" s="97"/>
       <c r="P3" s="63"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="143" t="s">
+      <c r="B4" s="165" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="145" t="s">
+      <c r="C4" s="167" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="37">
@@ -4373,8 +4440,8 @@
       <c r="P4" s="63"/>
     </row>
     <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="144"/>
-      <c r="C5" s="146"/>
+      <c r="B5" s="166"/>
+      <c r="C5" s="168"/>
       <c r="D5" s="66" t="s">
         <v>47</v>
       </c>
@@ -4557,10 +4624,10 @@
       <c r="P11" s="63"/>
     </row>
     <row r="12" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="142" t="s">
+      <c r="B12" s="164" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="142"/>
+      <c r="C12" s="164"/>
       <c r="D12" s="63" t="s">
         <v>63</v>
       </c>
@@ -4884,14 +4951,14 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="137" t="s">
+      <c r="B2" s="159" t="s">
         <v>186</v>
       </c>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138"/>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="139"/>
+      <c r="C2" s="160"/>
+      <c r="D2" s="160"/>
+      <c r="E2" s="160"/>
+      <c r="F2" s="160"/>
+      <c r="G2" s="161"/>
       <c r="M2" s="126" t="s">
         <v>177</v>
       </c>
@@ -4906,28 +4973,28 @@
       </c>
     </row>
     <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="140"/>
-      <c r="C3" s="141"/>
-      <c r="D3" s="141"/>
-      <c r="E3" s="141"/>
-      <c r="F3" s="141"/>
-      <c r="G3" s="141"/>
-      <c r="H3" s="147" t="s">
+      <c r="B3" s="162"/>
+      <c r="C3" s="163"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="163"/>
+      <c r="F3" s="163"/>
+      <c r="G3" s="163"/>
+      <c r="H3" s="169" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="148"/>
-      <c r="J3" s="148"/>
-      <c r="K3" s="149"/>
+      <c r="I3" s="170"/>
+      <c r="J3" s="170"/>
+      <c r="K3" s="171"/>
       <c r="M3" s="97"/>
       <c r="N3" s="63"/>
       <c r="O3" s="97"/>
       <c r="P3" s="63"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="143" t="s">
+      <c r="B4" s="165" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="145" t="s">
+      <c r="C4" s="167" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="37">
@@ -4958,8 +5025,8 @@
       <c r="P4" s="63"/>
     </row>
     <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="144"/>
-      <c r="C5" s="146"/>
+      <c r="B5" s="166"/>
+      <c r="C5" s="168"/>
       <c r="D5" s="39" t="s">
         <v>49</v>
       </c>
@@ -5142,10 +5209,10 @@
       <c r="P11" s="63"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B12" s="150" t="s">
+      <c r="B12" s="172" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="151"/>
+      <c r="C12" s="173"/>
       <c r="D12" s="127" t="s">
         <v>63</v>
       </c>
@@ -5237,10 +5304,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DABE7A-7845-46EA-BB0E-44CB73A3B0F1}">
-  <dimension ref="B1:Q24"/>
+  <dimension ref="B1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5253,62 +5320,65 @@
     <col min="7" max="7" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.21875" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="169" t="s">
+    <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="177" t="s">
         <v>185</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="171"/>
-      <c r="N2" s="99" t="s">
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="178"/>
+      <c r="F2" s="178"/>
+      <c r="G2" s="178"/>
+      <c r="H2" s="178"/>
+      <c r="I2" s="179"/>
+      <c r="J2" s="186"/>
+      <c r="O2" s="99" t="s">
         <v>177</v>
       </c>
-      <c r="O2" s="98" t="s">
+      <c r="P2" s="98" t="s">
         <v>180</v>
       </c>
-      <c r="P2" s="99" t="s">
+      <c r="Q2" s="99" t="s">
         <v>197</v>
       </c>
-      <c r="Q2" s="98" t="s">
+      <c r="R2" s="98" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="172"/>
-      <c r="C3" s="154"/>
-      <c r="D3" s="154"/>
-      <c r="E3" s="154"/>
-      <c r="F3" s="154"/>
-      <c r="G3" s="154"/>
-      <c r="H3" s="154"/>
-      <c r="I3" s="173"/>
-      <c r="J3" s="147" t="s">
+    <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="180"/>
+      <c r="C3" s="181"/>
+      <c r="D3" s="181"/>
+      <c r="E3" s="181"/>
+      <c r="F3" s="181"/>
+      <c r="G3" s="181"/>
+      <c r="H3" s="181"/>
+      <c r="I3" s="182"/>
+      <c r="J3" s="186"/>
+      <c r="K3" s="169" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="148"/>
-      <c r="L3" s="149"/>
-      <c r="N3" s="97"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="97"/>
-      <c r="Q3" s="63"/>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="152" t="s">
+      <c r="L3" s="170"/>
+      <c r="M3" s="171"/>
+      <c r="O3" s="97"/>
+      <c r="P3" s="63"/>
+      <c r="Q3" s="97"/>
+      <c r="R3" s="63"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B4" s="174" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="153" t="s">
+      <c r="C4" s="175" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="129">
@@ -5326,32 +5396,35 @@
       <c r="H4" s="130">
         <v>45249</v>
       </c>
-      <c r="I4" s="180">
+      <c r="I4" s="153">
         <v>45255</v>
       </c>
-      <c r="J4" s="183" t="s">
+      <c r="J4" s="153">
+        <v>45256</v>
+      </c>
+      <c r="K4" s="156" t="s">
         <v>158</v>
       </c>
-      <c r="K4" s="116" t="s">
+      <c r="L4" s="116" t="s">
         <v>159</v>
       </c>
-      <c r="L4" s="117" t="s">
+      <c r="M4" s="117" t="s">
         <v>160</v>
       </c>
-      <c r="N4" s="124">
+      <c r="O4" s="124">
         <v>1</v>
       </c>
-      <c r="O4" s="125" t="s">
+      <c r="P4" s="125" t="s">
         <v>226</v>
       </c>
-      <c r="P4" s="124">
+      <c r="Q4" s="124">
         <v>1</v>
       </c>
-      <c r="Q4" s="125"/>
-    </row>
-    <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="144"/>
-      <c r="C5" s="146"/>
+      <c r="R4" s="125"/>
+    </row>
+    <row r="5" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="166"/>
+      <c r="C5" s="168"/>
       <c r="D5" s="62" t="s">
         <v>53</v>
       </c>
@@ -5367,24 +5440,27 @@
       <c r="H5" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="175" t="s">
+      <c r="I5" s="149" t="s">
         <v>53</v>
       </c>
-      <c r="J5" s="184"/>
-      <c r="K5" s="60"/>
-      <c r="L5" s="61"/>
-      <c r="N5" s="124">
+      <c r="J5" s="149" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" s="157"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="61"/>
+      <c r="O5" s="124">
         <v>2</v>
       </c>
-      <c r="O5" s="125" t="s">
+      <c r="P5" s="125" t="s">
         <v>227</v>
       </c>
-      <c r="P5" s="124">
+      <c r="Q5" s="124">
         <v>1</v>
       </c>
-      <c r="Q5" s="125"/>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="R5" s="125"/>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="31">
         <v>1</v>
       </c>
@@ -5406,31 +5482,34 @@
       <c r="H6" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="181" t="s">
+      <c r="I6" s="154" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="53">
+      <c r="J6" s="154" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="53">
         <v>42</v>
       </c>
-      <c r="K6" s="54">
+      <c r="L6" s="54">
         <v>10</v>
       </c>
-      <c r="L6" s="55">
-        <f>ROUND((K6/J6)*100,2)</f>
+      <c r="M6" s="55">
+        <f>ROUND((L6/K6)*100,2)</f>
         <v>23.81</v>
       </c>
-      <c r="N6" s="97">
+      <c r="O6" s="97">
         <v>3</v>
       </c>
-      <c r="O6" s="63" t="s">
+      <c r="P6" s="63" t="s">
         <v>228</v>
       </c>
-      <c r="P6" s="97">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="63"/>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q6" s="97">
+        <v>0</v>
+      </c>
+      <c r="R6" s="63"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" s="33">
         <v>2</v>
       </c>
@@ -5440,22 +5519,23 @@
       <c r="F7" s="43"/>
       <c r="G7" s="50"/>
       <c r="H7" s="43"/>
-      <c r="I7" s="182"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="44"/>
-      <c r="N7" s="124">
+      <c r="I7" s="155"/>
+      <c r="J7" s="187"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="44"/>
+      <c r="O7" s="124">
         <v>4</v>
       </c>
-      <c r="O7" s="125" t="s">
+      <c r="P7" s="125" t="s">
         <v>229</v>
       </c>
-      <c r="P7" s="124">
+      <c r="Q7" s="124">
         <v>1</v>
       </c>
-      <c r="Q7" s="125"/>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="R7" s="125"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="33">
         <v>3</v>
       </c>
@@ -5465,22 +5545,23 @@
       <c r="F8" s="43"/>
       <c r="G8" s="50"/>
       <c r="H8" s="43"/>
-      <c r="I8" s="182"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="44"/>
-      <c r="N8" s="97">
+      <c r="I8" s="155"/>
+      <c r="J8" s="187"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="44"/>
+      <c r="O8" s="97">
         <v>5</v>
       </c>
-      <c r="O8" s="63" t="s">
+      <c r="P8" s="63" t="s">
         <v>230</v>
       </c>
-      <c r="P8" s="97">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="63"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q8" s="97">
+        <v>0</v>
+      </c>
+      <c r="R8" s="63"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="33">
         <v>4</v>
       </c>
@@ -5490,22 +5571,23 @@
       <c r="F9" s="43"/>
       <c r="G9" s="50"/>
       <c r="H9" s="43"/>
-      <c r="I9" s="182"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="44"/>
-      <c r="N9" s="124">
+      <c r="I9" s="155"/>
+      <c r="J9" s="187"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="44"/>
+      <c r="O9" s="124">
         <v>6</v>
       </c>
-      <c r="O9" s="125" t="s">
+      <c r="P9" s="125" t="s">
         <v>231</v>
       </c>
-      <c r="P9" s="124">
+      <c r="Q9" s="124">
         <v>1</v>
       </c>
-      <c r="Q9" s="125"/>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="R9" s="125"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" s="33">
         <v>5</v>
       </c>
@@ -5515,22 +5597,23 @@
       <c r="F10" s="43"/>
       <c r="G10" s="50"/>
       <c r="H10" s="43"/>
-      <c r="I10" s="182"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="44"/>
-      <c r="N10" s="97">
+      <c r="I10" s="155"/>
+      <c r="J10" s="187"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="44"/>
+      <c r="O10" s="97">
         <v>7</v>
       </c>
-      <c r="O10" s="63" t="s">
+      <c r="P10" s="63" t="s">
         <v>232</v>
       </c>
-      <c r="P10" s="97">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="63"/>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q10" s="97">
+        <v>0</v>
+      </c>
+      <c r="R10" s="63"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11" s="33">
         <v>6</v>
       </c>
@@ -5540,26 +5623,27 @@
       <c r="F11" s="43"/>
       <c r="G11" s="43"/>
       <c r="H11" s="43"/>
-      <c r="I11" s="182"/>
-      <c r="J11" s="185"/>
-      <c r="K11" s="134"/>
-      <c r="L11" s="136"/>
-      <c r="N11" s="124">
+      <c r="I11" s="155"/>
+      <c r="J11" s="188"/>
+      <c r="K11" s="158"/>
+      <c r="L11" s="134"/>
+      <c r="M11" s="136"/>
+      <c r="O11" s="124">
         <v>8</v>
       </c>
-      <c r="O11" s="125" t="s">
+      <c r="P11" s="125" t="s">
         <v>233</v>
       </c>
-      <c r="P11" s="124">
+      <c r="Q11" s="124">
         <v>1</v>
       </c>
-      <c r="Q11" s="125"/>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="179" t="s">
+      <c r="R11" s="125"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B12" s="176" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="142"/>
+      <c r="C12" s="164"/>
       <c r="D12" s="63"/>
       <c r="E12" s="63" t="s">
         <v>152</v>
@@ -5576,28 +5660,31 @@
       <c r="I12" s="34" t="s">
         <v>248</v>
       </c>
-      <c r="J12" s="161" t="s">
+      <c r="J12" s="189" t="s">
+        <v>253</v>
+      </c>
+      <c r="K12" s="141" t="s">
         <v>188</v>
       </c>
-      <c r="K12" s="63" t="s">
+      <c r="L12" s="63" t="s">
         <v>252</v>
       </c>
-      <c r="L12" s="162">
+      <c r="M12" s="142">
         <v>45255</v>
       </c>
-      <c r="N12" s="97">
+      <c r="O12" s="97">
         <v>9</v>
       </c>
-      <c r="O12" s="63" t="s">
+      <c r="P12" s="63" t="s">
         <v>234</v>
       </c>
-      <c r="P12" s="97">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="63"/>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B13" s="161"/>
+      <c r="Q12" s="97">
+        <v>0</v>
+      </c>
+      <c r="R12" s="63"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B13" s="141"/>
       <c r="C13" s="63"/>
       <c r="D13" s="63"/>
       <c r="E13" s="63"/>
@@ -5609,24 +5696,25 @@
       <c r="I13" s="34" t="s">
         <v>247</v>
       </c>
-      <c r="J13" s="161" t="s">
+      <c r="J13" s="189"/>
+      <c r="K13" s="141" t="s">
         <v>250</v>
       </c>
-      <c r="K13" s="63"/>
-      <c r="L13" s="34"/>
-      <c r="N13" s="97">
+      <c r="L13" s="63"/>
+      <c r="M13" s="34"/>
+      <c r="O13" s="97">
         <v>10</v>
       </c>
-      <c r="O13" s="63" t="s">
+      <c r="P13" s="63" t="s">
         <v>235</v>
       </c>
-      <c r="P13" s="97">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="63"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B14" s="161"/>
+      <c r="Q13" s="97">
+        <v>0</v>
+      </c>
+      <c r="R13" s="63"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B14" s="141"/>
       <c r="C14" s="63"/>
       <c r="D14" s="63"/>
       <c r="E14" s="63"/>
@@ -5634,122 +5722,124 @@
       <c r="G14" s="63"/>
       <c r="H14" s="63"/>
       <c r="I14" s="34"/>
-      <c r="J14" s="161" t="s">
+      <c r="J14" s="189"/>
+      <c r="K14" s="141" t="s">
         <v>251</v>
       </c>
-      <c r="K14" s="63"/>
-      <c r="L14" s="34"/>
-      <c r="N14" s="97">
+      <c r="L14" s="63"/>
+      <c r="M14" s="34"/>
+      <c r="O14" s="97">
         <v>11</v>
       </c>
-      <c r="O14" s="63" t="s">
+      <c r="P14" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="P14" s="97">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="63"/>
-    </row>
-    <row r="15" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="163"/>
-      <c r="C15" s="164"/>
-      <c r="D15" s="164"/>
-      <c r="E15" s="164"/>
-      <c r="F15" s="164"/>
-      <c r="G15" s="164"/>
-      <c r="H15" s="164"/>
+      <c r="Q14" s="97">
+        <v>0</v>
+      </c>
+      <c r="R14" s="63"/>
+    </row>
+    <row r="15" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="143"/>
+      <c r="C15" s="144"/>
+      <c r="D15" s="144"/>
+      <c r="E15" s="144"/>
+      <c r="F15" s="144"/>
+      <c r="G15" s="144"/>
+      <c r="H15" s="144"/>
       <c r="I15" s="36"/>
-      <c r="J15" s="163"/>
-      <c r="K15" s="164"/>
-      <c r="L15" s="36"/>
-      <c r="N15" s="97">
+      <c r="J15" s="190"/>
+      <c r="K15" s="143"/>
+      <c r="L15" s="144"/>
+      <c r="M15" s="36"/>
+      <c r="O15" s="97">
         <v>12</v>
       </c>
-      <c r="O15" s="63" t="s">
+      <c r="P15" s="63" t="s">
         <v>237</v>
       </c>
-      <c r="P15" s="97">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="63"/>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="N16" s="97">
+      <c r="Q15" s="97">
+        <v>0</v>
+      </c>
+      <c r="R15" s="63"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="O16" s="97">
         <v>13</v>
       </c>
-      <c r="O16" s="63" t="s">
+      <c r="P16" s="63" t="s">
         <v>236</v>
       </c>
-      <c r="P16" s="97">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="63"/>
-    </row>
-    <row r="17" spans="12:17" x14ac:dyDescent="0.3">
-      <c r="N17" s="97">
+      <c r="Q16" s="97">
+        <v>0</v>
+      </c>
+      <c r="R16" s="63"/>
+    </row>
+    <row r="17" spans="13:18" x14ac:dyDescent="0.3">
+      <c r="O17" s="97">
         <v>14</v>
       </c>
-      <c r="O17" s="63" t="s">
+      <c r="P17" s="63" t="s">
         <v>238</v>
       </c>
-      <c r="P17" s="97">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="63"/>
-    </row>
-    <row r="18" spans="12:17" x14ac:dyDescent="0.3">
-      <c r="N18" s="97">
+      <c r="Q17" s="97">
+        <v>0</v>
+      </c>
+      <c r="R17" s="63"/>
+    </row>
+    <row r="18" spans="13:18" x14ac:dyDescent="0.3">
+      <c r="O18" s="97">
         <v>15</v>
       </c>
-      <c r="O18" s="63" t="s">
+      <c r="P18" s="63" t="s">
         <v>239</v>
       </c>
-      <c r="P18" s="97">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="63"/>
-    </row>
-    <row r="21" spans="12:17" x14ac:dyDescent="0.3">
-      <c r="N21" s="97"/>
-      <c r="O21" s="65" t="s">
+      <c r="Q18" s="97">
+        <v>0</v>
+      </c>
+      <c r="R18" s="63"/>
+    </row>
+    <row r="21" spans="13:18" x14ac:dyDescent="0.3">
+      <c r="O21" s="97"/>
+      <c r="P21" s="65" t="s">
         <v>198</v>
       </c>
-      <c r="P21" s="126">
-        <f>SUM(P4:P15)</f>
+      <c r="Q21" s="126">
+        <f>SUM(Q4:Q15)</f>
         <v>5</v>
       </c>
-      <c r="Q21" s="63"/>
-    </row>
-    <row r="22" spans="12:17" x14ac:dyDescent="0.3">
-      <c r="N22" s="97"/>
-      <c r="O22" s="65" t="s">
+      <c r="R21" s="63"/>
+    </row>
+    <row r="22" spans="13:18" x14ac:dyDescent="0.3">
+      <c r="O22" s="97"/>
+      <c r="P22" s="65" t="s">
         <v>182</v>
       </c>
-      <c r="P22" s="126">
-        <f>COUNT(P4:P18)</f>
+      <c r="Q22" s="126">
+        <f>COUNT(Q4:Q18)</f>
         <v>15</v>
       </c>
-      <c r="Q22" s="63"/>
-    </row>
-    <row r="23" spans="12:17" x14ac:dyDescent="0.3">
-      <c r="N23" s="97"/>
-      <c r="O23" s="65" t="s">
+      <c r="R22" s="63"/>
+    </row>
+    <row r="23" spans="13:18" x14ac:dyDescent="0.3">
+      <c r="O23" s="97"/>
+      <c r="P23" s="65" t="s">
         <v>207</v>
       </c>
-      <c r="P23" s="126">
-        <f>ROUND((P21/P22)*100,2)</f>
+      <c r="Q23" s="126">
+        <f>ROUND((Q21/Q22)*100,2)</f>
         <v>33.33</v>
       </c>
-      <c r="Q23" s="63"/>
-    </row>
-    <row r="24" spans="12:17" x14ac:dyDescent="0.3">
-      <c r="L24" t="s">
+      <c r="R23" s="63"/>
+    </row>
+    <row r="24" spans="13:18" x14ac:dyDescent="0.3">
+      <c r="M24" t="s">
         <v>46</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="K3:M3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B12:C12"/>
@@ -5762,10 +5852,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0268C353-496F-4BD6-A7EF-D042619A03C3}">
-  <dimension ref="B1:Q18"/>
+  <dimension ref="B1:R18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5778,60 +5868,63 @@
     <col min="7" max="7" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.109375" customWidth="1"/>
-    <col min="10" max="10" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="169" t="s">
+    <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="177" t="s">
         <v>184</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="171"/>
-      <c r="N2" s="99" t="s">
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="178"/>
+      <c r="F2" s="178"/>
+      <c r="G2" s="178"/>
+      <c r="H2" s="178"/>
+      <c r="I2" s="179"/>
+      <c r="J2" s="186"/>
+      <c r="O2" s="99" t="s">
         <v>177</v>
       </c>
-      <c r="O2" s="98" t="s">
+      <c r="P2" s="98" t="s">
         <v>180</v>
       </c>
-      <c r="P2" s="99" t="s">
+      <c r="Q2" s="99" t="s">
         <v>197</v>
       </c>
-      <c r="Q2" s="98" t="s">
+      <c r="R2" s="98" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B3" s="172"/>
-      <c r="C3" s="154"/>
-      <c r="D3" s="154"/>
-      <c r="E3" s="154"/>
-      <c r="F3" s="154"/>
-      <c r="G3" s="154"/>
-      <c r="H3" s="154"/>
-      <c r="I3" s="173"/>
-      <c r="J3" s="165"/>
-      <c r="K3" s="157"/>
-      <c r="L3" s="158"/>
-      <c r="N3" s="97"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="97"/>
-      <c r="Q3" s="63"/>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="152" t="s">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B3" s="180"/>
+      <c r="C3" s="181"/>
+      <c r="D3" s="181"/>
+      <c r="E3" s="181"/>
+      <c r="F3" s="181"/>
+      <c r="G3" s="181"/>
+      <c r="H3" s="181"/>
+      <c r="I3" s="182"/>
+      <c r="J3" s="191"/>
+      <c r="K3" s="183"/>
+      <c r="L3" s="184"/>
+      <c r="M3" s="185"/>
+      <c r="O3" s="97"/>
+      <c r="P3" s="63"/>
+      <c r="Q3" s="97"/>
+      <c r="R3" s="63"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B4" s="174" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="153" t="s">
+      <c r="C4" s="175" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="129">
@@ -5849,32 +5942,35 @@
       <c r="H4" s="130">
         <v>45249</v>
       </c>
-      <c r="I4" s="174">
+      <c r="I4" s="148">
         <v>45255</v>
       </c>
-      <c r="J4" s="166" t="s">
+      <c r="J4" s="148">
+        <v>45256</v>
+      </c>
+      <c r="K4" s="145" t="s">
         <v>158</v>
       </c>
-      <c r="K4" s="155" t="s">
+      <c r="L4" s="137" t="s">
         <v>159</v>
       </c>
-      <c r="L4" s="159" t="s">
+      <c r="M4" s="139" t="s">
         <v>160</v>
       </c>
-      <c r="N4" s="124">
+      <c r="O4" s="124">
         <v>1</v>
       </c>
-      <c r="O4" s="125" t="s">
+      <c r="P4" s="125" t="s">
         <v>217</v>
       </c>
-      <c r="P4" s="124">
+      <c r="Q4" s="124">
         <v>1</v>
       </c>
-      <c r="Q4" s="125"/>
-    </row>
-    <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="144"/>
-      <c r="C5" s="146"/>
+      <c r="R4" s="125"/>
+    </row>
+    <row r="5" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="166"/>
+      <c r="C5" s="168"/>
       <c r="D5" s="62" t="s">
         <v>52</v>
       </c>
@@ -5890,24 +5986,27 @@
       <c r="H5" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="175" t="s">
+      <c r="I5" s="149" t="s">
         <v>52</v>
       </c>
-      <c r="J5" s="167"/>
-      <c r="K5" s="156"/>
-      <c r="L5" s="160"/>
-      <c r="N5" s="124">
+      <c r="J5" s="149" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" s="146"/>
+      <c r="L5" s="138"/>
+      <c r="M5" s="140"/>
+      <c r="O5" s="124">
         <v>2</v>
       </c>
-      <c r="O5" s="125" t="s">
+      <c r="P5" s="125" t="s">
         <v>218</v>
       </c>
-      <c r="P5" s="124">
+      <c r="Q5" s="124">
         <v>1</v>
       </c>
-      <c r="Q5" s="125"/>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="R5" s="125"/>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="31">
         <v>1</v>
       </c>
@@ -5929,31 +6028,34 @@
       <c r="H6" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="176" t="s">
+      <c r="I6" s="150" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="42">
+      <c r="J6" s="150" t="s">
         <v>48</v>
       </c>
-      <c r="K6" s="43">
+      <c r="K6" s="42">
+        <v>48</v>
+      </c>
+      <c r="L6" s="43">
         <v>9</v>
       </c>
-      <c r="L6" s="44">
-        <f>(K6/J6)*100</f>
+      <c r="M6" s="44">
+        <f>(L6/K6)*100</f>
         <v>18.75</v>
       </c>
-      <c r="N6" s="124">
+      <c r="O6" s="124">
         <v>3</v>
       </c>
-      <c r="O6" s="125" t="s">
+      <c r="P6" s="125" t="s">
         <v>219</v>
       </c>
-      <c r="P6" s="124">
+      <c r="Q6" s="124">
         <v>1</v>
       </c>
-      <c r="Q6" s="125"/>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="R6" s="125"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" s="33">
         <v>2</v>
       </c>
@@ -5963,22 +6065,25 @@
       <c r="F7" s="43"/>
       <c r="G7" s="50"/>
       <c r="H7" s="63"/>
-      <c r="I7" s="177"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="44"/>
-      <c r="N7" s="97">
+      <c r="I7" s="151"/>
+      <c r="J7" s="189"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="44"/>
+      <c r="O7" s="97">
         <v>4</v>
       </c>
-      <c r="O7" s="63" t="s">
+      <c r="P7" s="63" t="s">
         <v>220</v>
       </c>
-      <c r="P7" s="97">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="63"/>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q7" s="97">
+        <v>0</v>
+      </c>
+      <c r="R7" s="63" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="33">
         <v>3</v>
       </c>
@@ -5988,22 +6093,23 @@
       <c r="F8" s="43"/>
       <c r="G8" s="50"/>
       <c r="H8" s="63"/>
-      <c r="I8" s="177"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="44"/>
-      <c r="N8" s="97">
+      <c r="I8" s="151"/>
+      <c r="J8" s="189"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="44"/>
+      <c r="O8" s="97">
         <v>5</v>
       </c>
-      <c r="O8" s="63" t="s">
+      <c r="P8" s="63" t="s">
         <v>221</v>
       </c>
-      <c r="P8" s="97">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="63"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q8" s="97">
+        <v>0</v>
+      </c>
+      <c r="R8" s="63"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="33">
         <v>4</v>
       </c>
@@ -6013,22 +6119,23 @@
       <c r="F9" s="43"/>
       <c r="G9" s="50"/>
       <c r="H9" s="63"/>
-      <c r="I9" s="177"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="44"/>
-      <c r="N9" s="97">
+      <c r="I9" s="151"/>
+      <c r="J9" s="189"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="44"/>
+      <c r="O9" s="97">
         <v>6</v>
       </c>
-      <c r="O9" s="63" t="s">
+      <c r="P9" s="63" t="s">
         <v>222</v>
       </c>
-      <c r="P9" s="97">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="63"/>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q9" s="97">
+        <v>0</v>
+      </c>
+      <c r="R9" s="63"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" s="33">
         <v>5</v>
       </c>
@@ -6038,22 +6145,23 @@
       <c r="F10" s="43"/>
       <c r="G10" s="50"/>
       <c r="H10" s="63"/>
-      <c r="I10" s="177"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="44"/>
-      <c r="N10" s="97">
+      <c r="I10" s="151"/>
+      <c r="J10" s="189"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="44"/>
+      <c r="O10" s="97">
         <v>7</v>
       </c>
-      <c r="O10" s="63" t="s">
+      <c r="P10" s="63" t="s">
         <v>223</v>
       </c>
-      <c r="P10" s="97">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="63"/>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q10" s="97">
+        <v>0</v>
+      </c>
+      <c r="R10" s="63"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11" s="131">
         <v>6</v>
       </c>
@@ -6063,26 +6171,27 @@
       <c r="F11" s="134"/>
       <c r="G11" s="64"/>
       <c r="H11" s="135"/>
-      <c r="I11" s="178"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="44"/>
-      <c r="N11" s="97">
+      <c r="I11" s="152"/>
+      <c r="J11" s="192"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="44"/>
+      <c r="O11" s="97">
         <v>8</v>
       </c>
-      <c r="O11" s="63" t="s">
+      <c r="P11" s="63" t="s">
         <v>224</v>
       </c>
-      <c r="P11" s="97">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="63"/>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="179" t="s">
+      <c r="Q11" s="97">
+        <v>0</v>
+      </c>
+      <c r="R11" s="63"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B12" s="176" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="142"/>
+      <c r="C12" s="164"/>
       <c r="D12" s="63"/>
       <c r="E12" s="63" t="s">
         <v>154</v>
@@ -6099,28 +6208,31 @@
       <c r="I12" s="34" t="s">
         <v>246</v>
       </c>
-      <c r="J12" s="128" t="s">
+      <c r="J12" s="189" t="s">
+        <v>255</v>
+      </c>
+      <c r="K12" s="128" t="s">
         <v>188</v>
       </c>
-      <c r="K12" s="63" t="s">
+      <c r="L12" s="63" t="s">
         <v>252</v>
       </c>
-      <c r="L12" s="162">
+      <c r="M12" s="142">
         <v>45249</v>
       </c>
-      <c r="N12" s="97">
+      <c r="O12" s="97">
         <v>9</v>
       </c>
-      <c r="O12" s="63" t="s">
+      <c r="P12" s="63" t="s">
         <v>240</v>
       </c>
-      <c r="P12" s="97">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="63"/>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B13" s="161"/>
+      <c r="Q12" s="97">
+        <v>0</v>
+      </c>
+      <c r="R12" s="63"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B13" s="141"/>
       <c r="C13" s="63"/>
       <c r="D13" s="63"/>
       <c r="E13" s="63"/>
@@ -6134,24 +6246,27 @@
         <v>249</v>
       </c>
       <c r="I13" s="34"/>
-      <c r="J13" s="128" t="s">
+      <c r="J13" s="189" t="s">
+        <v>256</v>
+      </c>
+      <c r="K13" s="128" t="s">
         <v>189</v>
       </c>
-      <c r="K13" s="63"/>
-      <c r="L13" s="34"/>
-      <c r="N13" s="97">
+      <c r="L13" s="63"/>
+      <c r="M13" s="34"/>
+      <c r="O13" s="97">
         <v>10</v>
       </c>
-      <c r="O13" s="63" t="s">
+      <c r="P13" s="63" t="s">
         <v>241</v>
       </c>
-      <c r="P13" s="97">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="63"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B14" s="161"/>
+      <c r="Q13" s="97">
+        <v>0</v>
+      </c>
+      <c r="R13" s="63"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B14" s="141"/>
       <c r="C14" s="63"/>
       <c r="D14" s="63"/>
       <c r="E14" s="63"/>
@@ -6161,73 +6276,75 @@
       <c r="G14" s="63"/>
       <c r="H14" s="63"/>
       <c r="I14" s="34"/>
-      <c r="J14" s="128" t="s">
+      <c r="J14" s="189"/>
+      <c r="K14" s="128" t="s">
         <v>190</v>
       </c>
-      <c r="K14" s="63"/>
-      <c r="L14" s="34"/>
-      <c r="N14" s="97">
+      <c r="L14" s="63"/>
+      <c r="M14" s="34"/>
+      <c r="O14" s="97">
         <v>11</v>
       </c>
-      <c r="O14" s="63" t="s">
+      <c r="P14" s="63" t="s">
         <v>242</v>
       </c>
-      <c r="P14" s="97">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="63"/>
-    </row>
-    <row r="15" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="163"/>
-      <c r="C15" s="164"/>
-      <c r="D15" s="164"/>
-      <c r="E15" s="164"/>
-      <c r="F15" s="164"/>
-      <c r="G15" s="164"/>
-      <c r="H15" s="164"/>
+      <c r="Q14" s="97">
+        <v>0</v>
+      </c>
+      <c r="R14" s="63"/>
+    </row>
+    <row r="15" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="143"/>
+      <c r="C15" s="144"/>
+      <c r="D15" s="144"/>
+      <c r="E15" s="144"/>
+      <c r="F15" s="144"/>
+      <c r="G15" s="144"/>
+      <c r="H15" s="144"/>
       <c r="I15" s="36"/>
-      <c r="J15" s="168" t="s">
+      <c r="J15" s="190"/>
+      <c r="K15" s="147" t="s">
         <v>191</v>
       </c>
-      <c r="K15" s="164"/>
-      <c r="L15" s="36"/>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="N16" s="97"/>
-      <c r="O16" s="65" t="s">
+      <c r="L15" s="144"/>
+      <c r="M15" s="36"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="O16" s="97"/>
+      <c r="P16" s="65" t="s">
         <v>198</v>
       </c>
-      <c r="P16" s="126">
-        <f>SUM(P4:P14)</f>
+      <c r="Q16" s="126">
+        <f>SUM(Q4:Q14)</f>
         <v>3</v>
       </c>
-      <c r="Q16" s="63"/>
-    </row>
-    <row r="17" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N17" s="97"/>
-      <c r="O17" s="65" t="s">
+      <c r="R16" s="63"/>
+    </row>
+    <row r="17" spans="15:18" x14ac:dyDescent="0.3">
+      <c r="O17" s="97"/>
+      <c r="P17" s="65" t="s">
         <v>182</v>
       </c>
-      <c r="P17" s="126">
-        <f>COUNT(P4:P14)</f>
+      <c r="Q17" s="126">
+        <f>COUNT(Q4:Q14)</f>
         <v>11</v>
       </c>
-      <c r="Q17" s="63"/>
-    </row>
-    <row r="18" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N18" s="97"/>
-      <c r="O18" s="65" t="s">
+      <c r="R17" s="63"/>
+    </row>
+    <row r="18" spans="15:18" x14ac:dyDescent="0.3">
+      <c r="O18" s="97"/>
+      <c r="P18" s="65" t="s">
         <v>207</v>
       </c>
-      <c r="P18" s="126">
-        <f>ROUND((P16/P17)*100,2)</f>
+      <c r="Q18" s="126">
+        <f>ROUND((Q16/Q17)*100,2)</f>
         <v>27.27</v>
       </c>
-      <c r="Q18" s="63"/>
+      <c r="R18" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="K3:M3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B12:C12"/>

</xml_diff>

<commit_message>
Test records added for 30-12-2023
Test records added for 30-12-2023
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/Ops-2023-11.xlsx
+++ b/Offline/BusinessManagement/Ops/Ops-2023-11.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Ops\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86D177B-00F1-4EBD-A2C7-4138B5CDDAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B4AE5F-8778-48FB-B297-2F02D5CADC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
@@ -1115,7 +1115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="50">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -1643,67 +1643,6 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top/>
       <bottom style="thin">
@@ -1740,6 +1679,41 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -2031,50 +2005,40 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="6" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="6" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2120,6 +2084,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2135,7 +2102,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2144,7 +2111,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2156,10 +2123,21 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2605,15 +2583,15 @@
   <sheetData>
     <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="160" t="s">
         <v>182</v>
       </c>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="165"/>
-      <c r="F2" s="165"/>
-      <c r="G2" s="165"/>
-      <c r="H2" s="166"/>
+      <c r="C2" s="161"/>
+      <c r="D2" s="161"/>
+      <c r="E2" s="161"/>
+      <c r="F2" s="161"/>
+      <c r="G2" s="161"/>
+      <c r="H2" s="162"/>
       <c r="N2" s="98" t="s">
         <v>178</v>
       </c>
@@ -2631,19 +2609,19 @@
       </c>
     </row>
     <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="167"/>
-      <c r="C3" s="168"/>
-      <c r="D3" s="168"/>
-      <c r="E3" s="168"/>
-      <c r="F3" s="168"/>
-      <c r="G3" s="168"/>
-      <c r="H3" s="168"/>
-      <c r="I3" s="174" t="s">
+      <c r="B3" s="163"/>
+      <c r="C3" s="164"/>
+      <c r="D3" s="164"/>
+      <c r="E3" s="164"/>
+      <c r="F3" s="164"/>
+      <c r="G3" s="164"/>
+      <c r="H3" s="164"/>
+      <c r="I3" s="170" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="175"/>
-      <c r="K3" s="175"/>
-      <c r="L3" s="176"/>
+      <c r="J3" s="171"/>
+      <c r="K3" s="171"/>
+      <c r="L3" s="172"/>
       <c r="N3" s="63"/>
       <c r="O3" s="97"/>
       <c r="P3" s="63"/>
@@ -2651,10 +2629,10 @@
       <c r="R3" s="63"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B4" s="170" t="s">
+      <c r="B4" s="166" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="172" t="s">
+      <c r="C4" s="168" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="37">
@@ -2691,8 +2669,8 @@
       <c r="R4" s="63"/>
     </row>
     <row r="5" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="171"/>
-      <c r="C5" s="173"/>
+      <c r="B5" s="167"/>
+      <c r="C5" s="169"/>
       <c r="D5" s="66" t="s">
         <v>51</v>
       </c>
@@ -2893,10 +2871,10 @@
       <c r="R11" s="63"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="169" t="s">
+      <c r="B12" s="165" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="169"/>
+      <c r="C12" s="165"/>
       <c r="D12" s="95" t="s">
         <v>160</v>
       </c>
@@ -4398,14 +4376,14 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="160" t="s">
         <v>186</v>
       </c>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="165"/>
-      <c r="F2" s="165"/>
-      <c r="G2" s="166"/>
+      <c r="C2" s="161"/>
+      <c r="D2" s="161"/>
+      <c r="E2" s="161"/>
+      <c r="F2" s="161"/>
+      <c r="G2" s="162"/>
       <c r="M2" s="124" t="s">
         <v>176</v>
       </c>
@@ -4420,28 +4398,28 @@
       </c>
     </row>
     <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="167"/>
-      <c r="C3" s="168"/>
-      <c r="D3" s="168"/>
-      <c r="E3" s="168"/>
-      <c r="F3" s="168"/>
-      <c r="G3" s="168"/>
-      <c r="H3" s="174" t="s">
+      <c r="B3" s="163"/>
+      <c r="C3" s="164"/>
+      <c r="D3" s="164"/>
+      <c r="E3" s="164"/>
+      <c r="F3" s="164"/>
+      <c r="G3" s="164"/>
+      <c r="H3" s="170" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="175"/>
-      <c r="J3" s="175"/>
-      <c r="K3" s="176"/>
+      <c r="I3" s="171"/>
+      <c r="J3" s="171"/>
+      <c r="K3" s="172"/>
       <c r="M3" s="97"/>
       <c r="N3" s="63"/>
       <c r="O3" s="97"/>
       <c r="P3" s="63"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="170" t="s">
+      <c r="B4" s="166" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="172" t="s">
+      <c r="C4" s="168" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="37">
@@ -4472,8 +4450,8 @@
       <c r="P4" s="63"/>
     </row>
     <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="171"/>
-      <c r="C5" s="173"/>
+      <c r="B5" s="167"/>
+      <c r="C5" s="169"/>
       <c r="D5" s="66" t="s">
         <v>47</v>
       </c>
@@ -4656,10 +4634,10 @@
       <c r="P11" s="63"/>
     </row>
     <row r="12" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="169" t="s">
+      <c r="B12" s="165" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="169"/>
+      <c r="C12" s="165"/>
       <c r="D12" s="63" t="s">
         <v>63</v>
       </c>
@@ -4965,7 +4943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A980A2-087E-4BDA-864D-B7CC763A9F65}">
   <dimension ref="B1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
@@ -4983,14 +4961,14 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="160" t="s">
         <v>185</v>
       </c>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="165"/>
-      <c r="F2" s="165"/>
-      <c r="G2" s="166"/>
+      <c r="C2" s="161"/>
+      <c r="D2" s="161"/>
+      <c r="E2" s="161"/>
+      <c r="F2" s="161"/>
+      <c r="G2" s="162"/>
       <c r="M2" s="124" t="s">
         <v>176</v>
       </c>
@@ -5005,28 +4983,28 @@
       </c>
     </row>
     <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="167"/>
-      <c r="C3" s="168"/>
-      <c r="D3" s="168"/>
-      <c r="E3" s="168"/>
-      <c r="F3" s="168"/>
-      <c r="G3" s="168"/>
-      <c r="H3" s="174" t="s">
+      <c r="B3" s="163"/>
+      <c r="C3" s="164"/>
+      <c r="D3" s="164"/>
+      <c r="E3" s="164"/>
+      <c r="F3" s="164"/>
+      <c r="G3" s="164"/>
+      <c r="H3" s="170" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="175"/>
-      <c r="J3" s="175"/>
-      <c r="K3" s="176"/>
+      <c r="I3" s="171"/>
+      <c r="J3" s="171"/>
+      <c r="K3" s="172"/>
       <c r="M3" s="97"/>
       <c r="N3" s="63"/>
       <c r="O3" s="97"/>
       <c r="P3" s="63"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="170" t="s">
+      <c r="B4" s="166" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="172" t="s">
+      <c r="C4" s="168" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="37">
@@ -5057,8 +5035,8 @@
       <c r="P4" s="63"/>
     </row>
     <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="171"/>
-      <c r="C5" s="173"/>
+      <c r="B5" s="167"/>
+      <c r="C5" s="169"/>
       <c r="D5" s="39" t="s">
         <v>49</v>
       </c>
@@ -5133,13 +5111,13 @@
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
       <c r="K7" s="44"/>
-      <c r="M7" s="191">
+      <c r="M7" s="97">
         <v>4</v>
       </c>
-      <c r="N7" s="192" t="s">
+      <c r="N7" s="63" t="s">
         <v>201</v>
       </c>
-      <c r="O7" s="191">
+      <c r="O7" s="97">
         <v>0</v>
       </c>
       <c r="P7" s="63"/>
@@ -5241,10 +5219,10 @@
       <c r="P11" s="63"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B12" s="177" t="s">
+      <c r="B12" s="173" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="178"/>
+      <c r="C12" s="174"/>
       <c r="D12" s="125" t="s">
         <v>63</v>
       </c>
@@ -5338,8 +5316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DABE7A-7845-46EA-BB0E-44CB73A3B0F1}">
   <dimension ref="B1:R24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5362,17 +5340,17 @@
   <sheetData>
     <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="182" t="s">
+      <c r="B2" s="179" t="s">
         <v>184</v>
       </c>
-      <c r="C2" s="183"/>
-      <c r="D2" s="183"/>
-      <c r="E2" s="183"/>
-      <c r="F2" s="183"/>
-      <c r="G2" s="183"/>
-      <c r="H2" s="183"/>
-      <c r="I2" s="184"/>
-      <c r="J2" s="157"/>
+      <c r="C2" s="180"/>
+      <c r="D2" s="180"/>
+      <c r="E2" s="180"/>
+      <c r="F2" s="180"/>
+      <c r="G2" s="180"/>
+      <c r="H2" s="180"/>
+      <c r="I2" s="181"/>
+      <c r="J2" s="149"/>
       <c r="O2" s="99" t="s">
         <v>176</v>
       </c>
@@ -5387,30 +5365,30 @@
       </c>
     </row>
     <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="185"/>
-      <c r="C3" s="186"/>
-      <c r="D3" s="186"/>
-      <c r="E3" s="186"/>
-      <c r="F3" s="186"/>
-      <c r="G3" s="186"/>
-      <c r="H3" s="186"/>
-      <c r="I3" s="187"/>
-      <c r="J3" s="157"/>
-      <c r="K3" s="174" t="s">
+      <c r="B3" s="182"/>
+      <c r="C3" s="183"/>
+      <c r="D3" s="183"/>
+      <c r="E3" s="183"/>
+      <c r="F3" s="183"/>
+      <c r="G3" s="183"/>
+      <c r="H3" s="183"/>
+      <c r="I3" s="184"/>
+      <c r="J3" s="149"/>
+      <c r="K3" s="175" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="175"/>
-      <c r="M3" s="176"/>
+      <c r="L3" s="171"/>
+      <c r="M3" s="172"/>
       <c r="O3" s="97"/>
       <c r="P3" s="63"/>
       <c r="Q3" s="97"/>
       <c r="R3" s="63"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B4" s="179" t="s">
+      <c r="B4" s="176" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="180" t="s">
+      <c r="C4" s="177" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="127">
@@ -5428,13 +5406,13 @@
       <c r="H4" s="128">
         <v>45249</v>
       </c>
-      <c r="I4" s="151">
+      <c r="I4" s="150">
         <v>45255</v>
       </c>
-      <c r="J4" s="151">
+      <c r="J4" s="158">
         <v>45256</v>
       </c>
-      <c r="K4" s="154" t="s">
+      <c r="K4" s="155" t="s">
         <v>157</v>
       </c>
       <c r="L4" s="114" t="s">
@@ -5455,8 +5433,8 @@
       <c r="R4" s="123"/>
     </row>
     <row r="5" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="171"/>
-      <c r="C5" s="173"/>
+      <c r="B5" s="167"/>
+      <c r="C5" s="169"/>
       <c r="D5" s="62" t="s">
         <v>53</v>
       </c>
@@ -5472,13 +5450,13 @@
       <c r="H5" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="147" t="s">
+      <c r="I5" s="151" t="s">
         <v>53</v>
       </c>
-      <c r="J5" s="147" t="s">
+      <c r="J5" s="159" t="s">
         <v>53</v>
       </c>
-      <c r="K5" s="155"/>
+      <c r="K5" s="156"/>
       <c r="L5" s="60"/>
       <c r="M5" s="61"/>
       <c r="O5" s="122">
@@ -5517,10 +5495,10 @@
       <c r="I6" s="152" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="152" t="s">
+      <c r="J6" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="K6" s="53">
+      <c r="K6" s="157">
         <v>42</v>
       </c>
       <c r="L6" s="54">
@@ -5551,9 +5529,9 @@
       <c r="F7" s="43"/>
       <c r="G7" s="50"/>
       <c r="H7" s="43"/>
-      <c r="I7" s="153"/>
-      <c r="J7" s="158"/>
-      <c r="K7" s="51"/>
+      <c r="I7" s="146"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="42"/>
       <c r="L7" s="43"/>
       <c r="M7" s="44"/>
       <c r="O7" s="122">
@@ -5577,9 +5555,9 @@
       <c r="F8" s="43"/>
       <c r="G8" s="50"/>
       <c r="H8" s="43"/>
-      <c r="I8" s="153"/>
-      <c r="J8" s="158"/>
-      <c r="K8" s="51"/>
+      <c r="I8" s="146"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="42"/>
       <c r="L8" s="43"/>
       <c r="M8" s="44"/>
       <c r="O8" s="97">
@@ -5603,9 +5581,9 @@
       <c r="F9" s="43"/>
       <c r="G9" s="50"/>
       <c r="H9" s="43"/>
-      <c r="I9" s="153"/>
-      <c r="J9" s="158"/>
-      <c r="K9" s="51"/>
+      <c r="I9" s="146"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="42"/>
       <c r="L9" s="43"/>
       <c r="M9" s="44"/>
       <c r="O9" s="122">
@@ -5629,9 +5607,9 @@
       <c r="F10" s="43"/>
       <c r="G10" s="50"/>
       <c r="H10" s="43"/>
-      <c r="I10" s="153"/>
-      <c r="J10" s="158"/>
-      <c r="K10" s="51"/>
+      <c r="I10" s="146"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="42"/>
       <c r="L10" s="43"/>
       <c r="M10" s="44"/>
       <c r="O10" s="97">
@@ -5655,9 +5633,9 @@
       <c r="F11" s="43"/>
       <c r="G11" s="43"/>
       <c r="H11" s="43"/>
-      <c r="I11" s="153"/>
-      <c r="J11" s="159"/>
-      <c r="K11" s="156"/>
+      <c r="I11" s="146"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="131"/>
       <c r="L11" s="132"/>
       <c r="M11" s="134"/>
       <c r="O11" s="122">
@@ -5672,10 +5650,10 @@
       <c r="R11" s="123"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="181" t="s">
+      <c r="B12" s="178" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="169"/>
+      <c r="C12" s="165"/>
       <c r="D12" s="63"/>
       <c r="E12" s="63" t="s">
         <v>151</v>
@@ -5689,13 +5667,13 @@
       <c r="H12" s="63" t="s">
         <v>224</v>
       </c>
-      <c r="I12" s="34" t="s">
+      <c r="I12" s="153" t="s">
         <v>247</v>
       </c>
-      <c r="J12" s="160" t="s">
+      <c r="J12" s="63" t="s">
         <v>252</v>
       </c>
-      <c r="K12" s="139" t="s">
+      <c r="K12" s="126" t="s">
         <v>187</v>
       </c>
       <c r="L12" s="63" t="s">
@@ -5725,11 +5703,11 @@
         <v>213</v>
       </c>
       <c r="H13" s="63"/>
-      <c r="I13" s="34" t="s">
+      <c r="I13" s="153" t="s">
         <v>246</v>
       </c>
-      <c r="J13" s="160"/>
-      <c r="K13" s="139" t="s">
+      <c r="J13" s="63"/>
+      <c r="K13" s="126" t="s">
         <v>249</v>
       </c>
       <c r="L13" s="63"/>
@@ -5753,9 +5731,9 @@
       <c r="F14" s="63"/>
       <c r="G14" s="63"/>
       <c r="H14" s="63"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="160"/>
-      <c r="K14" s="139" t="s">
+      <c r="I14" s="153"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="126" t="s">
         <v>250</v>
       </c>
       <c r="L14" s="63"/>
@@ -5779,9 +5757,9 @@
       <c r="F15" s="142"/>
       <c r="G15" s="142"/>
       <c r="H15" s="142"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="161"/>
-      <c r="K15" s="141"/>
+      <c r="I15" s="154"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="145"/>
       <c r="L15" s="142"/>
       <c r="M15" s="36"/>
       <c r="O15" s="97">
@@ -5886,8 +5864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0268C353-496F-4BD6-A7EF-D042619A03C3}">
   <dimension ref="B1:R18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5910,17 +5888,17 @@
   <sheetData>
     <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="182" t="s">
+      <c r="B2" s="179" t="s">
         <v>183</v>
       </c>
-      <c r="C2" s="183"/>
-      <c r="D2" s="183"/>
-      <c r="E2" s="183"/>
-      <c r="F2" s="183"/>
-      <c r="G2" s="183"/>
-      <c r="H2" s="183"/>
-      <c r="I2" s="184"/>
-      <c r="J2" s="157"/>
+      <c r="C2" s="180"/>
+      <c r="D2" s="180"/>
+      <c r="E2" s="180"/>
+      <c r="F2" s="180"/>
+      <c r="G2" s="180"/>
+      <c r="H2" s="180"/>
+      <c r="I2" s="181"/>
+      <c r="J2" s="190"/>
       <c r="O2" s="99" t="s">
         <v>176</v>
       </c>
@@ -5935,28 +5913,28 @@
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B3" s="185"/>
-      <c r="C3" s="186"/>
-      <c r="D3" s="186"/>
-      <c r="E3" s="186"/>
-      <c r="F3" s="186"/>
-      <c r="G3" s="186"/>
-      <c r="H3" s="186"/>
-      <c r="I3" s="187"/>
-      <c r="J3" s="162"/>
-      <c r="K3" s="188"/>
-      <c r="L3" s="189"/>
-      <c r="M3" s="190"/>
+      <c r="B3" s="182"/>
+      <c r="C3" s="183"/>
+      <c r="D3" s="183"/>
+      <c r="E3" s="183"/>
+      <c r="F3" s="183"/>
+      <c r="G3" s="183"/>
+      <c r="H3" s="183"/>
+      <c r="I3" s="184"/>
+      <c r="J3" s="191"/>
+      <c r="K3" s="185"/>
+      <c r="L3" s="186"/>
+      <c r="M3" s="187"/>
       <c r="O3" s="97"/>
       <c r="P3" s="63"/>
       <c r="Q3" s="97"/>
       <c r="R3" s="63"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B4" s="179" t="s">
+      <c r="B4" s="176" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="180" t="s">
+      <c r="C4" s="177" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="127">
@@ -5974,10 +5952,10 @@
       <c r="H4" s="128">
         <v>45249</v>
       </c>
-      <c r="I4" s="146">
+      <c r="I4" s="188">
         <v>45255</v>
       </c>
-      <c r="J4" s="146">
+      <c r="J4" s="128">
         <v>45256</v>
       </c>
       <c r="K4" s="143" t="s">
@@ -6001,8 +5979,8 @@
       <c r="R4" s="123"/>
     </row>
     <row r="5" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="171"/>
-      <c r="C5" s="173"/>
+      <c r="B5" s="167"/>
+      <c r="C5" s="169"/>
       <c r="D5" s="62" t="s">
         <v>52</v>
       </c>
@@ -6018,10 +5996,10 @@
       <c r="H5" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="147" t="s">
+      <c r="I5" s="151" t="s">
         <v>52</v>
       </c>
-      <c r="J5" s="147" t="s">
+      <c r="J5" s="192" t="s">
         <v>52</v>
       </c>
       <c r="K5" s="144"/>
@@ -6060,10 +6038,10 @@
       <c r="H6" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="148" t="s">
+      <c r="I6" s="189" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="148" t="s">
+      <c r="J6" s="54" t="s">
         <v>48</v>
       </c>
       <c r="K6" s="42">
@@ -6097,8 +6075,8 @@
       <c r="F7" s="43"/>
       <c r="G7" s="50"/>
       <c r="H7" s="63"/>
-      <c r="I7" s="149"/>
-      <c r="J7" s="160"/>
+      <c r="I7" s="147"/>
+      <c r="J7" s="63"/>
       <c r="K7" s="42"/>
       <c r="L7" s="43"/>
       <c r="M7" s="44"/>
@@ -6125,8 +6103,8 @@
       <c r="F8" s="43"/>
       <c r="G8" s="50"/>
       <c r="H8" s="63"/>
-      <c r="I8" s="149"/>
-      <c r="J8" s="160"/>
+      <c r="I8" s="147"/>
+      <c r="J8" s="63"/>
       <c r="K8" s="42"/>
       <c r="L8" s="43"/>
       <c r="M8" s="44"/>
@@ -6151,8 +6129,8 @@
       <c r="F9" s="43"/>
       <c r="G9" s="50"/>
       <c r="H9" s="63"/>
-      <c r="I9" s="149"/>
-      <c r="J9" s="160"/>
+      <c r="I9" s="147"/>
+      <c r="J9" s="63"/>
       <c r="K9" s="42"/>
       <c r="L9" s="43"/>
       <c r="M9" s="44"/>
@@ -6177,8 +6155,8 @@
       <c r="F10" s="43"/>
       <c r="G10" s="50"/>
       <c r="H10" s="63"/>
-      <c r="I10" s="149"/>
-      <c r="J10" s="160"/>
+      <c r="I10" s="147"/>
+      <c r="J10" s="63"/>
       <c r="K10" s="42"/>
       <c r="L10" s="43"/>
       <c r="M10" s="44"/>
@@ -6203,8 +6181,8 @@
       <c r="F11" s="132"/>
       <c r="G11" s="64"/>
       <c r="H11" s="133"/>
-      <c r="I11" s="150"/>
-      <c r="J11" s="163"/>
+      <c r="I11" s="148"/>
+      <c r="J11" s="133"/>
       <c r="K11" s="42"/>
       <c r="L11" s="43"/>
       <c r="M11" s="44"/>
@@ -6220,10 +6198,10 @@
       <c r="R11" s="63"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="181" t="s">
+      <c r="B12" s="178" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="169"/>
+      <c r="C12" s="165"/>
       <c r="D12" s="63"/>
       <c r="E12" s="63" t="s">
         <v>153</v>
@@ -6237,10 +6215,10 @@
       <c r="H12" s="63" t="s">
         <v>247</v>
       </c>
-      <c r="I12" s="34" t="s">
+      <c r="I12" s="153" t="s">
         <v>245</v>
       </c>
-      <c r="J12" s="160" t="s">
+      <c r="J12" s="63" t="s">
         <v>254</v>
       </c>
       <c r="K12" s="126" t="s">
@@ -6277,8 +6255,8 @@
       <c r="H13" s="63" t="s">
         <v>248</v>
       </c>
-      <c r="I13" s="34"/>
-      <c r="J13" s="160" t="s">
+      <c r="I13" s="153"/>
+      <c r="J13" s="63" t="s">
         <v>255</v>
       </c>
       <c r="K13" s="126" t="s">
@@ -6307,8 +6285,8 @@
       </c>
       <c r="G14" s="63"/>
       <c r="H14" s="63"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="160"/>
+      <c r="I14" s="153"/>
+      <c r="J14" s="63"/>
       <c r="K14" s="126" t="s">
         <v>189</v>
       </c>
@@ -6333,8 +6311,8 @@
       <c r="F15" s="142"/>
       <c r="G15" s="142"/>
       <c r="H15" s="142"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="161"/>
+      <c r="I15" s="154"/>
+      <c r="J15" s="63"/>
       <c r="K15" s="145" t="s">
         <v>190</v>
       </c>

</xml_diff>